<commit_message>
Updating Q1 Type of ATD (Based on Li et al 2015)
</commit_message>
<xml_diff>
--- a/dataset/Extraction_form_basic.xlsx
+++ b/dataset/Extraction_form_basic.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-38220" yWindow="-2360" windowWidth="38220" windowHeight="22440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15020"/>
   </bookViews>
   <sheets>
     <sheet name="Folha 1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="768">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="773">
   <si>
     <t>Paper Id</t>
   </si>
@@ -4072,9 +4072,6 @@
 Third, our approach relies on mining error-prone files from a project’s revision history and bug tracking data. We use the bug report ID that developers enter into commits to locate error-prone files.</t>
   </si>
   <si>
-    <t>Q1 Type of ATD</t>
-  </si>
-  <si>
     <t>Q7 Research Type (Evaluation Research, Validation Research, Solution Proposal, Philosophycal paper, Other)</t>
   </si>
   <si>
@@ -4114,6 +4111,24 @@
  approuch:"GQM, questionaries, interview"
  #
  tools:"no"</t>
+  </si>
+  <si>
+    <t>Q1 Type of ATD (Based on Li et al 2015)</t>
+  </si>
+  <si>
+    <t>Complex architectural behavioral dependencies</t>
+  </si>
+  <si>
+    <t>System-level structure quality issues</t>
+  </si>
+  <si>
+    <t>Architectural compliance issues</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Violations of good architectural practices</t>
   </si>
 </sst>
 </file>
@@ -4462,8 +4477,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="84">
+  <cellStyleXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4898,7 +4916,7 @@
       <alignment vertical="justify" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="84">
+  <cellStyles count="85">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -4982,6 +5000,7 @@
     <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6134,11 +6153,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -6239,10 +6258,10 @@
         <v>714</v>
       </c>
       <c r="V1" s="37" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="W1" s="37" t="s">
-        <v>760</v>
+        <v>767</v>
       </c>
       <c r="X1" s="37" t="s">
         <v>742</v>
@@ -6348,7 +6367,9 @@
       <c r="V2" s="38" t="s">
         <v>637</v>
       </c>
-      <c r="W2" s="38"/>
+      <c r="W2" s="38" t="s">
+        <v>699</v>
+      </c>
       <c r="X2" s="3" t="s">
         <v>643</v>
       </c>
@@ -6451,7 +6472,9 @@
       <c r="V3" s="11" t="s">
         <v>637</v>
       </c>
-      <c r="W3" s="11"/>
+      <c r="W3" s="11" t="s">
+        <v>768</v>
+      </c>
       <c r="X3" s="11" t="s">
         <v>638</v>
       </c>
@@ -6554,7 +6577,9 @@
       <c r="V4" s="11" t="s">
         <v>652</v>
       </c>
-      <c r="W4" s="11"/>
+      <c r="W4" s="11" t="s">
+        <v>701</v>
+      </c>
       <c r="X4" s="11" t="s">
         <v>648</v>
       </c>
@@ -6657,7 +6682,9 @@
       <c r="V5" s="11" t="s">
         <v>637</v>
       </c>
-      <c r="W5" s="11"/>
+      <c r="W5" s="11" t="s">
+        <v>768</v>
+      </c>
       <c r="X5" s="9" t="s">
         <v>654</v>
       </c>
@@ -6760,7 +6787,9 @@
       <c r="V6" s="11" t="s">
         <v>637</v>
       </c>
-      <c r="W6" s="11"/>
+      <c r="W6" s="11" t="s">
+        <v>768</v>
+      </c>
       <c r="X6" s="9" t="s">
         <v>658</v>
       </c>
@@ -6863,7 +6892,9 @@
       <c r="V7" s="11" t="s">
         <v>652</v>
       </c>
-      <c r="W7" s="11"/>
+      <c r="W7" s="11" t="s">
+        <v>769</v>
+      </c>
       <c r="X7" s="9" t="s">
         <v>662</v>
       </c>
@@ -6966,7 +6997,9 @@
       <c r="V8" s="11" t="s">
         <v>652</v>
       </c>
-      <c r="W8" s="11"/>
+      <c r="W8" s="11" t="s">
+        <v>770</v>
+      </c>
       <c r="X8" s="11" t="s">
         <v>666</v>
       </c>
@@ -7069,7 +7102,9 @@
       <c r="V9" s="11" t="s">
         <v>637</v>
       </c>
-      <c r="W9" s="11"/>
+      <c r="W9" s="11" t="s">
+        <v>770</v>
+      </c>
       <c r="X9" s="9" t="s">
         <v>90</v>
       </c>
@@ -7172,7 +7207,9 @@
       <c r="V10" s="9" t="s">
         <v>652</v>
       </c>
-      <c r="W10" s="9"/>
+      <c r="W10" s="9" t="s">
+        <v>701</v>
+      </c>
       <c r="X10" s="9" t="s">
         <v>671</v>
       </c>
@@ -7275,7 +7312,9 @@
       <c r="V11" s="11" t="s">
         <v>674</v>
       </c>
-      <c r="W11" s="11"/>
+      <c r="W11" s="11" t="s">
+        <v>699</v>
+      </c>
       <c r="X11" s="9" t="s">
         <v>675</v>
       </c>
@@ -7378,7 +7417,9 @@
       <c r="V12" s="11" t="s">
         <v>699</v>
       </c>
-      <c r="W12" s="11"/>
+      <c r="W12" s="11" t="s">
+        <v>771</v>
+      </c>
       <c r="X12" s="11" t="s">
         <v>677</v>
       </c>
@@ -7479,7 +7520,7 @@
         <v>682</v>
       </c>
       <c r="Z13" s="40" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="AA13" s="40" t="s">
         <v>125</v>
@@ -7562,7 +7603,9 @@
       <c r="V14" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="W14" s="11"/>
+      <c r="W14" s="11" t="s">
+        <v>771</v>
+      </c>
       <c r="X14" s="9" t="s">
         <v>26</v>
       </c>
@@ -7575,7 +7618,9 @@
       <c r="AA14" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="AB14" s="23"/>
+      <c r="AB14" s="23" t="s">
+        <v>26</v>
+      </c>
       <c r="AC14" s="23" t="s">
         <v>135</v>
       </c>
@@ -7665,7 +7710,9 @@
       <c r="V15" s="11" t="s">
         <v>637</v>
       </c>
-      <c r="W15" s="11"/>
+      <c r="W15" s="11" t="s">
+        <v>770</v>
+      </c>
       <c r="X15" s="11" t="s">
         <v>687</v>
       </c>
@@ -7768,7 +7815,9 @@
       <c r="V16" s="11" t="s">
         <v>637</v>
       </c>
-      <c r="W16" s="11"/>
+      <c r="W16" s="11" t="s">
+        <v>770</v>
+      </c>
       <c r="X16" s="11" t="s">
         <v>690</v>
       </c>
@@ -7871,7 +7920,9 @@
       <c r="V17" s="11" t="s">
         <v>637</v>
       </c>
-      <c r="W17" s="11"/>
+      <c r="W17" s="11" t="s">
+        <v>769</v>
+      </c>
       <c r="X17" s="11" t="s">
         <v>547</v>
       </c>
@@ -8120,7 +8171,9 @@
       <c r="V20" s="11" t="s">
         <v>637</v>
       </c>
-      <c r="W20" s="11"/>
+      <c r="W20" s="11" t="s">
+        <v>769</v>
+      </c>
       <c r="X20" s="9" t="s">
         <v>695</v>
       </c>
@@ -8223,7 +8276,9 @@
       <c r="V21" s="11" t="s">
         <v>637</v>
       </c>
-      <c r="W21" s="11"/>
+      <c r="W21" s="11" t="s">
+        <v>770</v>
+      </c>
       <c r="X21" s="11" t="s">
         <v>26</v>
       </c>
@@ -8231,7 +8286,7 @@
         <v>26</v>
       </c>
       <c r="Z21" s="13" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="AA21" s="11" t="s">
         <v>26</v>
@@ -8326,7 +8381,9 @@
       <c r="V22" s="13" t="s">
         <v>652</v>
       </c>
-      <c r="W22" s="13"/>
+      <c r="W22" s="13" t="s">
+        <v>701</v>
+      </c>
       <c r="X22" s="13" t="s">
         <v>697</v>
       </c>
@@ -8334,7 +8391,7 @@
         <v>403</v>
       </c>
       <c r="Z22" s="13" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="AA22" s="11" t="s">
         <v>26</v>
@@ -8429,7 +8486,9 @@
       <c r="V23" s="22" t="s">
         <v>637</v>
       </c>
-      <c r="W23" s="22"/>
+      <c r="W23" s="22" t="s">
+        <v>770</v>
+      </c>
       <c r="X23" s="11" t="s">
         <v>198</v>
       </c>
@@ -8532,7 +8591,9 @@
       <c r="V24" s="11" t="s">
         <v>699</v>
       </c>
-      <c r="W24" s="11"/>
+      <c r="W24" s="11" t="s">
+        <v>771</v>
+      </c>
       <c r="X24" s="11" t="s">
         <v>26</v>
       </c>
@@ -8635,7 +8696,9 @@
       <c r="V25" s="11" t="s">
         <v>652</v>
       </c>
-      <c r="W25" s="11"/>
+      <c r="W25" s="11" t="s">
+        <v>769</v>
+      </c>
       <c r="X25" s="11" t="s">
         <v>700</v>
       </c>
@@ -8738,7 +8801,9 @@
       <c r="V26" s="11" t="s">
         <v>637</v>
       </c>
-      <c r="W26" s="11"/>
+      <c r="W26" s="11" t="s">
+        <v>772</v>
+      </c>
       <c r="X26" s="11" t="s">
         <v>225</v>
       </c>
@@ -8841,7 +8906,9 @@
       <c r="V27" s="11" t="s">
         <v>699</v>
       </c>
-      <c r="W27" s="11"/>
+      <c r="W27" s="11" t="s">
+        <v>771</v>
+      </c>
       <c r="X27" s="11" t="s">
         <v>26</v>
       </c>
@@ -8944,7 +9011,9 @@
       <c r="V28" s="11" t="s">
         <v>637</v>
       </c>
-      <c r="W28" s="11"/>
+      <c r="W28" s="11" t="s">
+        <v>769</v>
+      </c>
       <c r="X28" s="11" t="s">
         <v>247</v>
       </c>
@@ -9047,7 +9116,9 @@
       <c r="V29" s="11" t="s">
         <v>652</v>
       </c>
-      <c r="W29" s="11"/>
+      <c r="W29" s="11" t="s">
+        <v>701</v>
+      </c>
       <c r="X29" s="11" t="s">
         <v>701</v>
       </c>
@@ -9150,7 +9221,9 @@
       <c r="V30" s="11" t="s">
         <v>652</v>
       </c>
-      <c r="W30" s="11"/>
+      <c r="W30" s="11" t="s">
+        <v>701</v>
+      </c>
       <c r="X30" s="11" t="s">
         <v>701</v>
       </c>
@@ -9326,7 +9399,9 @@
       <c r="V32" s="11" t="s">
         <v>674</v>
       </c>
-      <c r="W32" s="11"/>
+      <c r="W32" s="11" t="s">
+        <v>770</v>
+      </c>
       <c r="X32" s="11" t="s">
         <v>281</v>
       </c>
@@ -9429,7 +9504,9 @@
       <c r="V33" s="11" t="s">
         <v>699</v>
       </c>
-      <c r="W33" s="11"/>
+      <c r="W33" s="11" t="s">
+        <v>771</v>
+      </c>
       <c r="X33" s="11" t="s">
         <v>26</v>
       </c>
@@ -9532,7 +9609,9 @@
       <c r="V34" s="11" t="s">
         <v>637</v>
       </c>
-      <c r="W34" s="11"/>
+      <c r="W34" s="11" t="s">
+        <v>771</v>
+      </c>
       <c r="X34" s="11" t="s">
         <v>26</v>
       </c>
@@ -9540,7 +9619,7 @@
         <v>26</v>
       </c>
       <c r="Z34" s="11" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="AA34" s="11" t="s">
         <v>26</v>
@@ -9635,7 +9714,9 @@
       <c r="V35" s="11" t="s">
         <v>637</v>
       </c>
-      <c r="W35" s="11"/>
+      <c r="W35" s="11" t="s">
+        <v>771</v>
+      </c>
       <c r="X35" s="11" t="s">
         <v>26</v>
       </c>
@@ -9738,7 +9819,9 @@
       <c r="V36" s="11" t="s">
         <v>652</v>
       </c>
-      <c r="W36" s="11"/>
+      <c r="W36" s="11" t="s">
+        <v>771</v>
+      </c>
       <c r="X36" s="11" t="s">
         <v>26</v>
       </c>
@@ -9993,7 +10076,9 @@
       <c r="V39" s="11" t="s">
         <v>699</v>
       </c>
-      <c r="W39" s="11"/>
+      <c r="W39" s="11" t="s">
+        <v>771</v>
+      </c>
       <c r="X39" s="13" t="s">
         <v>26</v>
       </c>
@@ -10096,7 +10181,9 @@
       <c r="V40" s="11" t="s">
         <v>674</v>
       </c>
-      <c r="W40" s="11"/>
+      <c r="W40" s="11" t="s">
+        <v>771</v>
+      </c>
       <c r="X40" s="13" t="s">
         <v>26</v>
       </c>
@@ -10104,7 +10191,7 @@
         <v>26</v>
       </c>
       <c r="Z40" s="13" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="AA40" s="13" t="s">
         <v>26</v>
@@ -10199,7 +10286,9 @@
       <c r="V41" s="11" t="s">
         <v>637</v>
       </c>
-      <c r="W41" s="11"/>
+      <c r="W41" s="11" t="s">
+        <v>772</v>
+      </c>
       <c r="X41" s="11" t="s">
         <v>473</v>
       </c>
@@ -10207,7 +10296,7 @@
         <v>26</v>
       </c>
       <c r="Z41" s="13" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="AA41" s="13" t="s">
         <v>472</v>
@@ -10302,7 +10391,9 @@
       <c r="V42" s="11" t="s">
         <v>637</v>
       </c>
-      <c r="W42" s="11"/>
+      <c r="W42" s="11" t="s">
+        <v>772</v>
+      </c>
       <c r="X42" s="13" t="s">
         <v>382</v>
       </c>
@@ -10310,7 +10401,7 @@
         <v>26</v>
       </c>
       <c r="Z42" s="13" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="AA42" s="11" t="s">
         <v>453</v>
@@ -10478,7 +10569,9 @@
       <c r="V44" s="11" t="s">
         <v>637</v>
       </c>
-      <c r="W44" s="11"/>
+      <c r="W44" s="11" t="s">
+        <v>769</v>
+      </c>
       <c r="X44" s="11" t="s">
         <v>705</v>
       </c>
@@ -10581,7 +10674,9 @@
       <c r="V45" s="11" t="s">
         <v>652</v>
       </c>
-      <c r="W45" s="11"/>
+      <c r="W45" s="11" t="s">
+        <v>699</v>
+      </c>
       <c r="X45" s="11" t="s">
         <v>26</v>
       </c>
@@ -10684,7 +10779,9 @@
       <c r="V46" s="11" t="s">
         <v>699</v>
       </c>
-      <c r="W46" s="11"/>
+      <c r="W46" s="11" t="s">
+        <v>771</v>
+      </c>
       <c r="X46" s="11" t="s">
         <v>476</v>
       </c>
@@ -10787,7 +10884,9 @@
       <c r="V47" s="11" t="s">
         <v>707</v>
       </c>
-      <c r="W47" s="11"/>
+      <c r="W47" s="11" t="s">
+        <v>771</v>
+      </c>
       <c r="X47" s="11" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Removed the paper id 82 because is sub of 81
</commit_message>
<xml_diff>
--- a/dataset/Extraction_form_basic.xlsx
+++ b/dataset/Extraction_form_basic.xlsx
@@ -11,7 +11,7 @@
   </sheets>
   <definedNames>
     <definedName name="_3___R._Kazman__Y._Cai__R._Mo__Q._Feng__L._Xiao__S._Haziyev__V._Fedak__and_A._Shapochka._A_case_study_in_locating_the_architectural_roots_of_technical_debt._In_Proc._37th_International_Conference_on_Software__Engineering__May_2015.____8___R._Mo__W._Snip">'Folha 1'!#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Folha 1'!$B$1:$B$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Folha 1'!$B$1:$B$47</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1252" uniqueCount="760">
   <si>
     <t>Paper Id</t>
   </si>
@@ -1118,14 +1118,6 @@
     <t>IEEE Newspaper</t>
   </si>
   <si>
-    <t xml:space="preserve">MTD 2012, Zurich, Switzerland 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">International Workshop on Managing Technical Debt (MTD)
-</t>
-  </si>
-  <si>
     <t>Kumar et al 2018</t>
   </si>
   <si>
@@ -1255,21 +1247,6 @@
   </si>
   <si>
     <t>The authors collected important metrics regard to architectural metrics and complex metrics.The authors created a usefull plugin that take a way good information to manager and devolopers about architectural metrics and complex metrics directy from github repositories. The plugin is available on https://www.scitools.com/support/gui-plugins/ as called Understand</t>
-  </si>
-  <si>
-    <t>Bill Curtis, Jay Sappidi,  Alexandra Szynkarski</t>
-  </si>
-  <si>
-    <t>The study have access to a large repository from real cases (160) with varius types of technology. This repository was provided by CAST company.</t>
-  </si>
-  <si>
-    <t>The main tool used is a commercial tool and there is no free licence to get the tool to replicate the study.</t>
-  </si>
-  <si>
-    <t>The study did not share the dataset to evaluate. Besides, even calculating the TD cost, there is ATD specif cost</t>
-  </si>
-  <si>
-    <t>It was measurte TD based on Health Factors, but there is no specific ATD measure in this paper</t>
   </si>
   <si>
     <t>Describe a kind of ATD, more spefically scalability ATD and the authors proposed a lightweight approach to manage scalibity debt. The case study conducted a method to identify, estimate and prioritize scalability debt.</t>
@@ -2174,78 +2151,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">Estimating the Size, Cost, and Types of Technical Debt </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">This study summarizes results of a study of Technical Debt across 745 business applications comprising 365 million lines of code collected from 160 companies in 10 industry segments. These applications were submitted to a static analysis that evaluates quality within and across application layers that may be coded in different languages. The analysis consists of evaluating the application against a repository of over 1200 rules of good architectural and coding practice. A formula for estimating Technical Debt with adjustable parameters is presented. Results are presented for Technical Debt across the entire sample as well as for different programming languages and quality factors. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">software metrics, software structural quality, technical debt, static analysis, benchmarking </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">The purpose of this study is to explore a method for quantifying an estimate of the Technical Debt within a business application. Such studies are needed to help IT organizations make visible the costs and risks hidden within their application portfolio, as well as establish a benchmark for making decisions about investments in application quality, and especially structural quality. 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Technical Debt 
-TD-Principal =
-(Σ high severity violations) x .5) 1 hr.) x 75$) +
-(Σ medium severity violations) x .25) 1 hr.) x 75$) + (Σ low severity violations) x .1) 1 hr.) x 75$) 
-However, there is specific formula to calculate the ATD cost
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">This work identifies various design debt causes in a cloud computing system from various dimensions of design debt. Even though immature, un-ripen coded service accessible over the Internet using the cloud computing paradigm may work fine and be wholly tolerable to the patron; but excess quantities will make a service progression that may lead to extreme specialist of software developers and finally an inflexible product. Delivery of the earliest primary beginning coded service without ripeness or maturity is like going into debts or arrears or due to obligation. A petite tiny debt rates progress so protracted as it is paid or rewarded back punctually with a rewrite/redraft/revising/reworking. The risk arises when the debt is not repaid and settled. Every miniature infinitesimal effort spent on imprecise code reckons as interest on that arrears/debt. Intact engineering business can be brought to be idle under the balance load of an unconsolidated, non-solicit implementation, execution, and performance discharging object-oriented, func- tional or procedural or otherwise. This work uses refactoring as a solution for the identified debt in the multilateral cloud security architecture to secure the cloud services. 
 </t>
   </si>
@@ -3275,9 +3180,6 @@
   </si>
   <si>
     <t>Good; due to the authors proposed an effetive way to calculate the principal of TD based on catalog of rules to detect the violations of qualities attributes like performance, securtiy, robustness, trasferability and changeabilite. So, those characteristics are so close to architectural technical debt.</t>
-  </si>
-  <si>
-    <t>Regular; due to even calculating the TD cost, there is NO ATD specif cost</t>
   </si>
   <si>
     <t>Good;due to the authors proposed a method to identify, estimate and prioritize a kind of ATD, more specifically scalability debt.</t>
@@ -4289,7 +4191,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -4458,19 +4360,6 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
       <right/>
       <top/>
       <bottom/>
@@ -4734,7 +4623,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -4900,13 +4789,10 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="17" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6151,13 +6037,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI48"/>
+  <dimension ref="A1:AI47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W1" sqref="W1"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -6204,7 +6090,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="37" t="s">
-        <v>752</v>
+        <v>739</v>
       </c>
       <c r="E1" s="37" t="s">
         <v>3</v>
@@ -6240,43 +6126,43 @@
         <v>13</v>
       </c>
       <c r="P1" s="37" t="s">
-        <v>633</v>
+        <v>620</v>
       </c>
       <c r="Q1" s="37" t="s">
-        <v>635</v>
+        <v>622</v>
       </c>
       <c r="R1" s="37" t="s">
-        <v>712</v>
+        <v>699</v>
       </c>
       <c r="S1" s="37" t="s">
-        <v>636</v>
+        <v>623</v>
       </c>
       <c r="T1" s="37" t="s">
-        <v>713</v>
+        <v>700</v>
       </c>
       <c r="U1" s="37" t="s">
-        <v>714</v>
+        <v>701</v>
       </c>
       <c r="V1" s="37" t="s">
-        <v>760</v>
+        <v>747</v>
       </c>
       <c r="W1" s="37" t="s">
-        <v>767</v>
+        <v>754</v>
       </c>
       <c r="X1" s="37" t="s">
-        <v>742</v>
+        <v>729</v>
       </c>
       <c r="Y1" s="37" t="s">
-        <v>743</v>
+        <v>730</v>
       </c>
       <c r="Z1" s="37" t="s">
+        <v>731</v>
+      </c>
+      <c r="AA1" s="37" t="s">
+        <v>732</v>
+      </c>
+      <c r="AB1" s="37" t="s">
         <v>744</v>
-      </c>
-      <c r="AA1" s="37" t="s">
-        <v>745</v>
-      </c>
-      <c r="AB1" s="37" t="s">
-        <v>757</v>
       </c>
       <c r="AC1" s="37" t="s">
         <v>14</v>
@@ -6285,10 +6171,10 @@
         <v>15</v>
       </c>
       <c r="AE1" s="37" t="s">
-        <v>710</v>
+        <v>697</v>
       </c>
       <c r="AF1" s="37" t="s">
-        <v>711</v>
+        <v>698</v>
       </c>
       <c r="AG1" s="37" t="s">
         <v>16</v>
@@ -6297,7 +6183,7 @@
         <v>17</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>739</v>
+        <v>726</v>
       </c>
     </row>
     <row r="2" spans="1:35" ht="160" customHeight="1">
@@ -6323,7 +6209,7 @@
         <v>2019</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>524</v>
+        <v>512</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>21</v>
@@ -6344,65 +6230,65 @@
         <v>5</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>26</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>755</v>
+        <v>742</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>746</v>
+        <v>733</v>
       </c>
       <c r="V2" s="38" t="s">
-        <v>637</v>
+        <v>624</v>
       </c>
       <c r="W2" s="38" t="s">
-        <v>699</v>
+        <v>686</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>643</v>
+        <v>630</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>644</v>
+        <v>631</v>
       </c>
       <c r="Z2" s="5" t="s">
-        <v>550</v>
+        <v>538</v>
       </c>
       <c r="AA2" s="5" t="s">
-        <v>645</v>
+        <v>632</v>
       </c>
       <c r="AB2" s="5"/>
       <c r="AC2" s="3" t="s">
         <v>27</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>646</v>
+        <v>633</v>
       </c>
       <c r="AE2" s="3" t="s">
         <v>28</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>573</v>
+        <v>561</v>
       </c>
       <c r="AG2" s="7" t="s">
-        <v>647</v>
+        <v>634</v>
       </c>
       <c r="AH2" s="3" t="s">
         <v>29</v>
       </c>
       <c r="AI2" s="1" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="3" spans="1:35" ht="301" customHeight="1">
@@ -6443,62 +6329,62 @@
         <v>36</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>534</v>
+        <v>522</v>
       </c>
       <c r="N3" s="10">
         <v>16</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>632</v>
+        <v>619</v>
       </c>
       <c r="P3" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="R3" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S3" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="T3" s="11" t="s">
-        <v>715</v>
+        <v>702</v>
       </c>
       <c r="U3" s="11" t="s">
         <v>37</v>
       </c>
       <c r="V3" s="11" t="s">
-        <v>637</v>
+        <v>624</v>
       </c>
       <c r="W3" s="11" t="s">
-        <v>768</v>
+        <v>755</v>
       </c>
       <c r="X3" s="11" t="s">
-        <v>638</v>
+        <v>625</v>
       </c>
       <c r="Y3" s="11" t="s">
-        <v>639</v>
+        <v>626</v>
       </c>
       <c r="Z3" s="11" t="s">
-        <v>756</v>
+        <v>743</v>
       </c>
       <c r="AA3" s="9" t="s">
-        <v>640</v>
+        <v>627</v>
       </c>
       <c r="AB3" s="9"/>
       <c r="AC3" s="12" t="s">
-        <v>641</v>
+        <v>628</v>
       </c>
       <c r="AD3" s="12" t="s">
-        <v>642</v>
+        <v>629</v>
       </c>
       <c r="AE3" s="9" t="s">
-        <v>609</v>
+        <v>596</v>
       </c>
       <c r="AF3" s="9" t="s">
-        <v>574</v>
+        <v>562</v>
       </c>
       <c r="AG3" s="9" t="s">
         <v>38</v>
@@ -6507,7 +6393,7 @@
         <v>26</v>
       </c>
       <c r="AI3" s="1" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="4" spans="1:35" ht="310" customHeight="1">
@@ -6554,65 +6440,65 @@
         <v>9</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>470</v>
+        <v>458</v>
       </c>
       <c r="P4" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="Q4" s="9" t="s">
         <v>26</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="S4" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="T4" s="11" t="s">
-        <v>623</v>
+        <v>610</v>
       </c>
       <c r="U4" s="11" t="s">
         <v>46</v>
       </c>
       <c r="V4" s="11" t="s">
-        <v>652</v>
+        <v>639</v>
       </c>
       <c r="W4" s="11" t="s">
-        <v>701</v>
+        <v>688</v>
       </c>
       <c r="X4" s="11" t="s">
-        <v>648</v>
+        <v>635</v>
       </c>
       <c r="Y4" s="11" t="s">
-        <v>649</v>
+        <v>636</v>
       </c>
       <c r="Z4" s="11" t="s">
-        <v>551</v>
+        <v>539</v>
       </c>
       <c r="AA4" s="11" t="s">
         <v>26</v>
       </c>
       <c r="AB4" s="11"/>
       <c r="AC4" s="13" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="AD4" s="13" t="s">
         <v>47</v>
       </c>
       <c r="AE4" s="11" t="s">
-        <v>610</v>
+        <v>597</v>
       </c>
       <c r="AF4" s="11" t="s">
-        <v>575</v>
+        <v>563</v>
       </c>
       <c r="AG4" s="11" t="s">
-        <v>650</v>
+        <v>637</v>
       </c>
       <c r="AH4" s="11" t="s">
-        <v>651</v>
+        <v>638</v>
       </c>
       <c r="AI4" s="1" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="5" spans="1:35" ht="216" customHeight="1">
@@ -6623,10 +6509,10 @@
         <v>48</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>753</v>
+        <v>740</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>50</v>
@@ -6659,56 +6545,56 @@
         <v>4</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="R5" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S5" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="T5" s="11" t="s">
-        <v>716</v>
+        <v>703</v>
       </c>
       <c r="U5" s="9" t="s">
-        <v>653</v>
+        <v>640</v>
       </c>
       <c r="V5" s="11" t="s">
-        <v>637</v>
+        <v>624</v>
       </c>
       <c r="W5" s="11" t="s">
-        <v>768</v>
+        <v>755</v>
       </c>
       <c r="X5" s="9" t="s">
-        <v>654</v>
+        <v>641</v>
       </c>
       <c r="Y5" s="11" t="s">
-        <v>655</v>
+        <v>642</v>
       </c>
       <c r="Z5" s="9" t="s">
-        <v>552</v>
+        <v>540</v>
       </c>
       <c r="AA5" s="11" t="s">
-        <v>656</v>
+        <v>643</v>
       </c>
       <c r="AB5" s="11"/>
       <c r="AC5" s="11" t="s">
         <v>54</v>
       </c>
       <c r="AD5" s="11" t="s">
-        <v>657</v>
+        <v>644</v>
       </c>
       <c r="AE5" s="11" t="s">
-        <v>611</v>
+        <v>598</v>
       </c>
       <c r="AF5" s="11" t="s">
-        <v>576</v>
+        <v>564</v>
       </c>
       <c r="AG5" s="11" t="s">
         <v>55</v>
@@ -6717,7 +6603,7 @@
         <v>56</v>
       </c>
       <c r="AI5" s="1" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="6" spans="1:35" ht="231" customHeight="1">
@@ -6752,7 +6638,7 @@
         <v>61</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>527</v>
+        <v>515</v>
       </c>
       <c r="L6" s="11" t="s">
         <v>44</v>
@@ -6764,65 +6650,65 @@
         <v>10</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="P6" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="Q6" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="R6" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S6" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="T6" s="11" t="s">
-        <v>716</v>
+        <v>703</v>
       </c>
       <c r="U6" s="9" t="s">
         <v>63</v>
       </c>
       <c r="V6" s="11" t="s">
-        <v>637</v>
+        <v>624</v>
       </c>
       <c r="W6" s="11" t="s">
-        <v>768</v>
+        <v>755</v>
       </c>
       <c r="X6" s="9" t="s">
-        <v>658</v>
+        <v>645</v>
       </c>
       <c r="Y6" s="9" t="s">
-        <v>499</v>
+        <v>487</v>
       </c>
       <c r="Z6" s="13" t="s">
-        <v>659</v>
+        <v>646</v>
       </c>
       <c r="AA6" s="11" t="s">
-        <v>660</v>
+        <v>647</v>
       </c>
       <c r="AB6" s="11"/>
       <c r="AC6" s="13" t="s">
-        <v>500</v>
+        <v>488</v>
       </c>
       <c r="AD6" s="13" t="s">
         <v>250</v>
       </c>
       <c r="AE6" s="13" t="s">
-        <v>491</v>
+        <v>479</v>
       </c>
       <c r="AF6" s="13" t="s">
-        <v>577</v>
+        <v>565</v>
       </c>
       <c r="AG6" s="13" t="s">
-        <v>661</v>
+        <v>648</v>
       </c>
       <c r="AH6" s="13" t="s">
         <v>26</v>
       </c>
       <c r="AI6" s="1" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="7" spans="1:35" ht="231" customHeight="1">
@@ -6836,7 +6722,7 @@
         <v>49</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>754</v>
+        <v>741</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>65</v>
@@ -6872,62 +6758,62 @@
         <v>72</v>
       </c>
       <c r="P7" s="11" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="Q7" s="11" t="s">
         <v>26</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="S7" s="11" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="T7" s="11" t="s">
-        <v>717</v>
+        <v>704</v>
       </c>
       <c r="U7" s="9" t="s">
         <v>73</v>
       </c>
       <c r="V7" s="11" t="s">
-        <v>652</v>
+        <v>639</v>
       </c>
       <c r="W7" s="11" t="s">
-        <v>769</v>
+        <v>756</v>
       </c>
       <c r="X7" s="9" t="s">
-        <v>662</v>
+        <v>649</v>
       </c>
       <c r="Y7" s="11" t="s">
-        <v>663</v>
+        <v>650</v>
       </c>
       <c r="Z7" s="9" t="s">
-        <v>572</v>
+        <v>560</v>
       </c>
       <c r="AA7" s="11" t="s">
-        <v>664</v>
+        <v>651</v>
       </c>
       <c r="AB7" s="11"/>
       <c r="AC7" s="13" t="s">
-        <v>504</v>
+        <v>492</v>
       </c>
       <c r="AD7" s="13" t="s">
-        <v>502</v>
+        <v>490</v>
       </c>
       <c r="AE7" s="13" t="s">
-        <v>503</v>
+        <v>491</v>
       </c>
       <c r="AF7" s="13" t="s">
-        <v>578</v>
+        <v>566</v>
       </c>
       <c r="AG7" s="13" t="s">
-        <v>665</v>
+        <v>652</v>
       </c>
       <c r="AH7" s="13" t="s">
-        <v>501</v>
+        <v>489</v>
       </c>
       <c r="AI7" s="1" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="8" spans="1:35" ht="255" customHeight="1">
@@ -6974,65 +6860,65 @@
         <v>10</v>
       </c>
       <c r="O8" s="11" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="P8" s="11" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="Q8" s="11" t="s">
         <v>26</v>
       </c>
       <c r="R8" s="11" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="S8" s="11" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="T8" s="11" t="s">
-        <v>718</v>
+        <v>705</v>
       </c>
       <c r="U8" s="11" t="s">
-        <v>613</v>
+        <v>600</v>
       </c>
       <c r="V8" s="11" t="s">
-        <v>652</v>
+        <v>639</v>
       </c>
       <c r="W8" s="11" t="s">
-        <v>770</v>
+        <v>757</v>
       </c>
       <c r="X8" s="11" t="s">
-        <v>666</v>
+        <v>653</v>
       </c>
       <c r="Y8" s="11" t="s">
-        <v>667</v>
+        <v>654</v>
       </c>
       <c r="Z8" s="13" t="s">
-        <v>758</v>
+        <v>745</v>
       </c>
       <c r="AA8" s="11" t="s">
-        <v>668</v>
+        <v>655</v>
       </c>
       <c r="AB8" s="11"/>
       <c r="AC8" s="13" t="s">
-        <v>669</v>
+        <v>656</v>
       </c>
       <c r="AD8" s="13" t="s">
-        <v>498</v>
+        <v>486</v>
       </c>
       <c r="AE8" s="13" t="s">
-        <v>491</v>
+        <v>479</v>
       </c>
       <c r="AF8" s="13" t="s">
-        <v>579</v>
+        <v>567</v>
       </c>
       <c r="AG8" s="13" t="s">
-        <v>497</v>
+        <v>485</v>
       </c>
       <c r="AH8" s="13" t="s">
-        <v>496</v>
+        <v>484</v>
       </c>
       <c r="AI8" s="1" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="9" spans="1:35" ht="226" customHeight="1">
@@ -7073,7 +6959,7 @@
         <v>88</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>535</v>
+        <v>523</v>
       </c>
       <c r="N9" s="10">
         <v>10</v>
@@ -7082,28 +6968,28 @@
         <v>89</v>
       </c>
       <c r="P9" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="Q9" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="R9" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S9" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="T9" s="11" t="s">
-        <v>747</v>
+        <v>734</v>
       </c>
       <c r="U9" s="9" t="s">
-        <v>748</v>
+        <v>735</v>
       </c>
       <c r="V9" s="11" t="s">
-        <v>637</v>
+        <v>624</v>
       </c>
       <c r="W9" s="11" t="s">
-        <v>770</v>
+        <v>757</v>
       </c>
       <c r="X9" s="9" t="s">
         <v>90</v>
@@ -7112,32 +6998,32 @@
         <v>91</v>
       </c>
       <c r="Z9" s="11" t="s">
-        <v>553</v>
+        <v>541</v>
       </c>
       <c r="AA9" s="11" t="s">
-        <v>670</v>
+        <v>657</v>
       </c>
       <c r="AB9" s="11"/>
       <c r="AC9" s="13" t="s">
-        <v>494</v>
+        <v>482</v>
       </c>
       <c r="AD9" s="13" t="s">
-        <v>493</v>
+        <v>481</v>
       </c>
       <c r="AE9" s="13" t="s">
-        <v>491</v>
+        <v>479</v>
       </c>
       <c r="AF9" s="13" t="s">
-        <v>580</v>
+        <v>568</v>
       </c>
       <c r="AG9" s="13" t="s">
-        <v>492</v>
+        <v>480</v>
       </c>
       <c r="AH9" s="13" t="s">
-        <v>495</v>
+        <v>483</v>
       </c>
       <c r="AI9" s="1" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="10" spans="1:35" ht="409.5" customHeight="1">
@@ -7184,65 +7070,65 @@
         <v>11</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>517</v>
+        <v>505</v>
       </c>
       <c r="P10" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="Q10" s="9" t="s">
         <v>26</v>
       </c>
       <c r="R10" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="S10" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="T10" s="9" t="s">
-        <v>717</v>
+        <v>704</v>
       </c>
       <c r="U10" s="9" t="s">
-        <v>719</v>
+        <v>706</v>
       </c>
       <c r="V10" s="9" t="s">
-        <v>652</v>
+        <v>639</v>
       </c>
       <c r="W10" s="9" t="s">
-        <v>701</v>
+        <v>688</v>
       </c>
       <c r="X10" s="9" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="Y10" s="11" t="s">
-        <v>672</v>
+        <v>659</v>
       </c>
       <c r="Z10" s="9" t="s">
-        <v>554</v>
+        <v>542</v>
       </c>
       <c r="AA10" s="11" t="s">
-        <v>673</v>
+        <v>660</v>
       </c>
       <c r="AB10" s="11"/>
       <c r="AC10" s="13" t="s">
-        <v>518</v>
+        <v>506</v>
       </c>
       <c r="AD10" s="13" t="s">
-        <v>519</v>
+        <v>507</v>
       </c>
       <c r="AE10" s="13" t="s">
-        <v>503</v>
+        <v>491</v>
       </c>
       <c r="AF10" s="13" t="s">
-        <v>581</v>
+        <v>569</v>
       </c>
       <c r="AG10" s="13" t="s">
-        <v>759</v>
+        <v>746</v>
       </c>
       <c r="AH10" s="13" t="s">
-        <v>720</v>
+        <v>707</v>
       </c>
       <c r="AI10" s="1" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="11" spans="1:35" ht="175" customHeight="1">
@@ -7304,25 +7190,25 @@
         <v>26</v>
       </c>
       <c r="T11" s="11" t="s">
-        <v>614</v>
+        <v>601</v>
       </c>
       <c r="U11" s="9" t="s">
         <v>108</v>
       </c>
       <c r="V11" s="11" t="s">
-        <v>674</v>
+        <v>661</v>
       </c>
       <c r="W11" s="11" t="s">
-        <v>699</v>
+        <v>686</v>
       </c>
       <c r="X11" s="9" t="s">
-        <v>675</v>
+        <v>662</v>
       </c>
       <c r="Y11" s="11" t="s">
         <v>26</v>
       </c>
       <c r="Z11" s="11" t="s">
-        <v>555</v>
+        <v>543</v>
       </c>
       <c r="AA11" s="11" t="s">
         <v>26</v>
@@ -7338,16 +7224,16 @@
         <v>111</v>
       </c>
       <c r="AF11" s="11" t="s">
-        <v>582</v>
+        <v>570</v>
       </c>
       <c r="AG11" s="11" t="s">
         <v>112</v>
       </c>
       <c r="AH11" s="11" t="s">
-        <v>676</v>
+        <v>663</v>
       </c>
       <c r="AI11" s="1" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="12" spans="1:35" ht="171" customHeight="1">
@@ -7367,7 +7253,7 @@
         <v>114</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>721</v>
+        <v>708</v>
       </c>
       <c r="G12" s="8">
         <v>2019</v>
@@ -7409,25 +7295,25 @@
         <v>26</v>
       </c>
       <c r="T12" s="11" t="s">
-        <v>615</v>
+        <v>602</v>
       </c>
       <c r="U12" s="11" t="s">
         <v>118</v>
       </c>
       <c r="V12" s="11" t="s">
-        <v>699</v>
+        <v>686</v>
       </c>
       <c r="W12" s="11" t="s">
-        <v>771</v>
+        <v>758</v>
       </c>
       <c r="X12" s="11" t="s">
-        <v>677</v>
+        <v>664</v>
       </c>
       <c r="Y12" s="11" t="s">
-        <v>678</v>
+        <v>665</v>
       </c>
       <c r="Z12" s="11" t="s">
-        <v>556</v>
+        <v>544</v>
       </c>
       <c r="AA12" s="11" t="s">
         <v>26</v>
@@ -7437,22 +7323,22 @@
         <v>120</v>
       </c>
       <c r="AD12" s="11" t="s">
-        <v>679</v>
+        <v>666</v>
       </c>
       <c r="AE12" s="11" t="s">
         <v>121</v>
       </c>
       <c r="AF12" s="11" t="s">
-        <v>583</v>
+        <v>571</v>
       </c>
       <c r="AG12" s="11" t="s">
-        <v>616</v>
+        <v>603</v>
       </c>
       <c r="AH12" s="11" t="s">
         <v>26</v>
       </c>
       <c r="AI12" s="1" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="13" spans="1:35" s="43" customFormat="1" ht="291" customHeight="1">
@@ -7478,7 +7364,7 @@
         <v>2017</v>
       </c>
       <c r="H13" s="40" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="I13" s="40" t="s">
         <v>34</v>
@@ -7490,16 +7376,16 @@
         <v>124</v>
       </c>
       <c r="L13" s="40" t="s">
-        <v>532</v>
+        <v>520</v>
       </c>
       <c r="M13" s="40" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="N13" s="39">
         <v>18</v>
       </c>
       <c r="O13" s="40" t="s">
-        <v>680</v>
+        <v>667</v>
       </c>
       <c r="P13" s="40"/>
       <c r="Q13" s="40"/>
@@ -7509,18 +7395,18 @@
         <v>314</v>
       </c>
       <c r="U13" s="40" t="s">
-        <v>749</v>
+        <v>736</v>
       </c>
       <c r="V13" s="40"/>
       <c r="W13" s="40"/>
       <c r="X13" s="40" t="s">
-        <v>681</v>
+        <v>668</v>
       </c>
       <c r="Y13" s="40" t="s">
-        <v>682</v>
+        <v>669</v>
       </c>
       <c r="Z13" s="40" t="s">
-        <v>764</v>
+        <v>751</v>
       </c>
       <c r="AA13" s="40" t="s">
         <v>125</v>
@@ -7533,7 +7419,7 @@
       <c r="AG13" s="42"/>
       <c r="AH13" s="42"/>
       <c r="AI13" s="43" t="s">
-        <v>741</v>
+        <v>728</v>
       </c>
     </row>
     <row r="14" spans="1:35" ht="234" customHeight="1">
@@ -7580,31 +7466,31 @@
         <v>3</v>
       </c>
       <c r="O14" s="9" t="s">
-        <v>546</v>
+        <v>534</v>
       </c>
       <c r="P14" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="Q14" s="9" t="s">
         <v>26</v>
       </c>
       <c r="R14" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="S14" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="T14" s="11" t="s">
-        <v>722</v>
+        <v>709</v>
       </c>
       <c r="U14" s="9" t="s">
-        <v>617</v>
+        <v>604</v>
       </c>
       <c r="V14" s="11" t="s">
         <v>26</v>
       </c>
       <c r="W14" s="11" t="s">
-        <v>771</v>
+        <v>758</v>
       </c>
       <c r="X14" s="9" t="s">
         <v>26</v>
@@ -7613,7 +7499,7 @@
         <v>26</v>
       </c>
       <c r="Z14" s="11" t="s">
-        <v>557</v>
+        <v>545</v>
       </c>
       <c r="AA14" s="11" t="s">
         <v>26</v>
@@ -7625,13 +7511,13 @@
         <v>135</v>
       </c>
       <c r="AD14" s="24" t="s">
-        <v>683</v>
+        <v>670</v>
       </c>
       <c r="AE14" s="24" t="s">
-        <v>684</v>
+        <v>671</v>
       </c>
       <c r="AF14" s="24" t="s">
-        <v>685</v>
+        <v>672</v>
       </c>
       <c r="AG14" s="24" t="s">
         <v>136</v>
@@ -7640,7 +7526,7 @@
         <v>137</v>
       </c>
       <c r="AI14" s="54" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="15" spans="1:35" ht="267" customHeight="1">
@@ -7653,7 +7539,7 @@
       <c r="C15" s="19">
         <v>36</v>
       </c>
-      <c r="D15" s="58">
+      <c r="D15" s="57">
         <v>2015</v>
       </c>
       <c r="E15" s="18" t="s">
@@ -7687,65 +7573,65 @@
         <v>10</v>
       </c>
       <c r="O15" s="9" t="s">
-        <v>686</v>
+        <v>673</v>
       </c>
       <c r="P15" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="Q15" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="R15" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S15" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="T15" s="11" t="s">
         <v>314</v>
       </c>
       <c r="U15" s="11" t="s">
-        <v>723</v>
+        <v>710</v>
       </c>
       <c r="V15" s="11" t="s">
-        <v>637</v>
+        <v>624</v>
       </c>
       <c r="W15" s="11" t="s">
-        <v>770</v>
+        <v>757</v>
       </c>
       <c r="X15" s="11" t="s">
-        <v>687</v>
+        <v>674</v>
       </c>
       <c r="Y15" s="11" t="s">
-        <v>688</v>
+        <v>675</v>
       </c>
       <c r="Z15" s="11" t="s">
-        <v>558</v>
+        <v>546</v>
       </c>
       <c r="AA15" s="11" t="s">
         <v>146</v>
       </c>
       <c r="AB15" s="11"/>
       <c r="AC15" s="13" t="s">
-        <v>484</v>
+        <v>472</v>
       </c>
       <c r="AD15" s="13" t="s">
-        <v>485</v>
+        <v>473</v>
       </c>
       <c r="AE15" s="13" t="s">
         <v>28</v>
       </c>
       <c r="AF15" s="13" t="s">
-        <v>584</v>
+        <v>572</v>
       </c>
       <c r="AG15" s="13" t="s">
-        <v>483</v>
+        <v>471</v>
       </c>
       <c r="AH15" s="13" t="s">
-        <v>482</v>
+        <v>470</v>
       </c>
       <c r="AI15" s="54" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="16" spans="1:35" ht="224" customHeight="1">
@@ -7792,65 +7678,65 @@
         <v>8</v>
       </c>
       <c r="O16" s="11" t="s">
-        <v>689</v>
+        <v>676</v>
       </c>
       <c r="P16" s="11" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="Q16" s="11" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="R16" s="11" t="s">
         <v>26</v>
       </c>
       <c r="S16" s="11" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="T16" s="11" t="s">
         <v>314</v>
       </c>
       <c r="U16" s="11" t="s">
-        <v>724</v>
+        <v>711</v>
       </c>
       <c r="V16" s="11" t="s">
-        <v>637</v>
+        <v>624</v>
       </c>
       <c r="W16" s="11" t="s">
-        <v>770</v>
+        <v>757</v>
       </c>
       <c r="X16" s="11" t="s">
-        <v>690</v>
+        <v>677</v>
       </c>
       <c r="Y16" s="11" t="s">
-        <v>691</v>
+        <v>678</v>
       </c>
       <c r="Z16" s="11" t="s">
-        <v>559</v>
+        <v>547</v>
       </c>
       <c r="AA16" s="11" t="s">
-        <v>692</v>
+        <v>679</v>
       </c>
       <c r="AB16" s="11"/>
       <c r="AC16" s="13" t="s">
-        <v>545</v>
+        <v>533</v>
       </c>
       <c r="AD16" s="13" t="s">
         <v>228</v>
       </c>
       <c r="AE16" s="13" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="AF16" s="13" t="s">
-        <v>585</v>
+        <v>573</v>
       </c>
       <c r="AG16" s="13" t="s">
-        <v>725</v>
+        <v>712</v>
       </c>
       <c r="AH16" s="13" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="AI16" s="54" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="17" spans="1:35" ht="291" customHeight="1">
@@ -7891,7 +7777,7 @@
         <v>88</v>
       </c>
       <c r="M17" s="9" t="s">
-        <v>536</v>
+        <v>524</v>
       </c>
       <c r="N17" s="8">
         <v>8</v>
@@ -7900,62 +7786,62 @@
         <v>157</v>
       </c>
       <c r="P17" s="11" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="Q17" s="11" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="R17" s="11" t="s">
         <v>26</v>
       </c>
       <c r="S17" s="11" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="T17" s="11" t="s">
         <v>314</v>
       </c>
       <c r="U17" s="11" t="s">
-        <v>726</v>
+        <v>713</v>
       </c>
       <c r="V17" s="11" t="s">
-        <v>637</v>
+        <v>624</v>
       </c>
       <c r="W17" s="11" t="s">
-        <v>769</v>
+        <v>756</v>
       </c>
       <c r="X17" s="11" t="s">
-        <v>547</v>
+        <v>535</v>
       </c>
       <c r="Y17" s="11" t="s">
         <v>158</v>
       </c>
       <c r="Z17" s="11" t="s">
-        <v>560</v>
+        <v>548</v>
       </c>
       <c r="AA17" s="11" t="s">
-        <v>693</v>
+        <v>680</v>
       </c>
       <c r="AB17" s="11"/>
       <c r="AC17" s="13" t="s">
-        <v>465</v>
+        <v>453</v>
       </c>
       <c r="AD17" s="13" t="s">
-        <v>464</v>
+        <v>452</v>
       </c>
       <c r="AE17" s="13" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="AF17" s="13" t="s">
-        <v>586</v>
+        <v>574</v>
       </c>
       <c r="AG17" s="13" t="s">
-        <v>463</v>
+        <v>451</v>
       </c>
       <c r="AH17" s="29" t="s">
-        <v>462</v>
+        <v>450</v>
       </c>
       <c r="AI17" s="54" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="18" spans="1:35" ht="199" customHeight="1">
@@ -8002,7 +7888,7 @@
         <v>16</v>
       </c>
       <c r="O18" s="40" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="P18" s="40"/>
       <c r="Q18" s="40"/>
@@ -8012,7 +7898,7 @@
         <v>314</v>
       </c>
       <c r="U18" s="40" t="s">
-        <v>750</v>
+        <v>737</v>
       </c>
       <c r="V18" s="40"/>
       <c r="W18" s="40"/>
@@ -8028,7 +7914,7 @@
       <c r="AG18" s="42"/>
       <c r="AH18" s="42"/>
       <c r="AI18" s="1" t="s">
-        <v>741</v>
+        <v>728</v>
       </c>
     </row>
     <row r="19" spans="1:35" ht="220" customHeight="1">
@@ -8045,7 +7931,7 @@
         <v>2016</v>
       </c>
       <c r="E19" s="40" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="F19" s="40" t="s">
         <v>166</v>
@@ -8054,7 +7940,7 @@
         <v>2016</v>
       </c>
       <c r="H19" s="40" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="I19" s="40" t="s">
         <v>167</v>
@@ -8066,7 +7952,7 @@
         <v>169</v>
       </c>
       <c r="L19" s="40" t="s">
-        <v>533</v>
+        <v>521</v>
       </c>
       <c r="M19" s="40" t="s">
         <v>170</v>
@@ -8075,17 +7961,17 @@
         <v>4</v>
       </c>
       <c r="O19" s="40" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="P19" s="40"/>
       <c r="Q19" s="40"/>
       <c r="R19" s="40"/>
       <c r="S19" s="40"/>
       <c r="T19" s="40" t="s">
-        <v>717</v>
+        <v>704</v>
       </c>
       <c r="U19" s="40" t="s">
-        <v>751</v>
+        <v>738</v>
       </c>
       <c r="V19" s="40"/>
       <c r="W19" s="40"/>
@@ -8101,7 +7987,7 @@
       <c r="AG19" s="42"/>
       <c r="AH19" s="42"/>
       <c r="AI19" s="1" t="s">
-        <v>741</v>
+        <v>728</v>
       </c>
     </row>
     <row r="20" spans="1:35" ht="408" customHeight="1">
@@ -8147,66 +8033,66 @@
       <c r="N20" s="8">
         <v>10</v>
       </c>
-      <c r="O20" s="59" t="s">
-        <v>694</v>
+      <c r="O20" s="58" t="s">
+        <v>681</v>
       </c>
       <c r="P20" s="11" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="Q20" s="11" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="R20" s="11" t="s">
         <v>26</v>
       </c>
       <c r="S20" s="11" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="T20" s="11" t="s">
         <v>314</v>
       </c>
       <c r="U20" s="9" t="s">
-        <v>727</v>
+        <v>714</v>
       </c>
       <c r="V20" s="11" t="s">
-        <v>637</v>
+        <v>624</v>
       </c>
       <c r="W20" s="11" t="s">
-        <v>769</v>
+        <v>756</v>
       </c>
       <c r="X20" s="9" t="s">
-        <v>695</v>
+        <v>682</v>
       </c>
       <c r="Y20" s="11" t="s">
         <v>179</v>
       </c>
       <c r="Z20" s="11" t="s">
-        <v>561</v>
+        <v>549</v>
       </c>
       <c r="AA20" s="11" t="s">
-        <v>696</v>
+        <v>683</v>
       </c>
       <c r="AB20" s="11"/>
       <c r="AC20" s="13" t="s">
-        <v>511</v>
+        <v>499</v>
       </c>
       <c r="AD20" s="13" t="s">
-        <v>512</v>
+        <v>500</v>
       </c>
       <c r="AE20" s="13" t="s">
-        <v>503</v>
+        <v>491</v>
       </c>
       <c r="AF20" s="13" t="s">
-        <v>587</v>
+        <v>575</v>
       </c>
       <c r="AG20" s="13" t="s">
-        <v>512</v>
+        <v>500</v>
       </c>
       <c r="AH20" s="13" t="s">
-        <v>510</v>
+        <v>498</v>
       </c>
       <c r="AI20" s="54" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="21" spans="1:35" ht="198" customHeight="1">
@@ -8232,7 +8118,7 @@
         <v>2015</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>628</v>
+        <v>615</v>
       </c>
       <c r="I21" s="11" t="s">
         <v>21</v>
@@ -8253,31 +8139,31 @@
         <v>8</v>
       </c>
       <c r="O21" s="11" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="P21" s="11" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="Q21" s="11" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="R21" s="11" t="s">
         <v>26</v>
       </c>
       <c r="S21" s="11" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="T21" s="11" t="s">
         <v>314</v>
       </c>
       <c r="U21" s="11" t="s">
-        <v>728</v>
+        <v>715</v>
       </c>
       <c r="V21" s="11" t="s">
-        <v>637</v>
+        <v>624</v>
       </c>
       <c r="W21" s="11" t="s">
-        <v>770</v>
+        <v>757</v>
       </c>
       <c r="X21" s="11" t="s">
         <v>26</v>
@@ -8286,32 +8172,32 @@
         <v>26</v>
       </c>
       <c r="Z21" s="13" t="s">
-        <v>765</v>
+        <v>752</v>
       </c>
       <c r="AA21" s="11" t="s">
         <v>26</v>
       </c>
       <c r="AB21" s="11"/>
       <c r="AC21" s="13" t="s">
-        <v>468</v>
+        <v>456</v>
       </c>
       <c r="AD21" s="13" t="s">
-        <v>467</v>
+        <v>455</v>
       </c>
       <c r="AE21" s="13" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="AF21" s="13" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
       <c r="AG21" s="13" t="s">
-        <v>469</v>
+        <v>457</v>
       </c>
       <c r="AH21" s="13" t="s">
-        <v>466</v>
+        <v>454</v>
       </c>
       <c r="AI21" s="54" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="22" spans="1:35" ht="272" customHeight="1">
@@ -8352,71 +8238,71 @@
         <v>144</v>
       </c>
       <c r="M22" s="11" t="s">
-        <v>537</v>
+        <v>525</v>
       </c>
       <c r="N22" s="8">
         <v>8</v>
       </c>
       <c r="O22" s="11" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="P22" s="11" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="Q22" s="11" t="s">
         <v>26</v>
       </c>
       <c r="R22" s="11" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="S22" s="11" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="T22" s="13" t="s">
-        <v>717</v>
+        <v>704</v>
       </c>
       <c r="U22" s="13" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="V22" s="13" t="s">
-        <v>652</v>
+        <v>639</v>
       </c>
       <c r="W22" s="13" t="s">
-        <v>701</v>
+        <v>688</v>
       </c>
       <c r="X22" s="13" t="s">
-        <v>697</v>
+        <v>684</v>
       </c>
       <c r="Y22" s="11" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="Z22" s="13" t="s">
-        <v>761</v>
+        <v>748</v>
       </c>
       <c r="AA22" s="11" t="s">
         <v>26</v>
       </c>
       <c r="AB22" s="11"/>
       <c r="AC22" s="13" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="AD22" s="13" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="AE22" s="13" t="s">
         <v>300</v>
       </c>
       <c r="AF22" s="13" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
       <c r="AG22" s="13" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="AH22" s="13" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="AI22" s="54" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="23" spans="1:35" ht="250" customHeight="1">
@@ -8466,62 +8352,62 @@
         <v>197</v>
       </c>
       <c r="P23" s="11" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="Q23" s="11" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="R23" s="11" t="s">
         <v>26</v>
       </c>
       <c r="S23" s="11" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="T23" s="22" t="s">
         <v>314</v>
       </c>
       <c r="U23" s="11" t="s">
-        <v>729</v>
+        <v>716</v>
       </c>
       <c r="V23" s="22" t="s">
-        <v>637</v>
+        <v>624</v>
       </c>
       <c r="W23" s="22" t="s">
-        <v>770</v>
+        <v>757</v>
       </c>
       <c r="X23" s="11" t="s">
         <v>198</v>
       </c>
       <c r="Y23" s="11" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="Z23" s="13" t="s">
-        <v>562</v>
+        <v>550</v>
       </c>
       <c r="AA23" s="13" t="s">
-        <v>698</v>
+        <v>685</v>
       </c>
       <c r="AB23" s="13"/>
       <c r="AC23" s="13" t="s">
-        <v>516</v>
+        <v>504</v>
       </c>
       <c r="AD23" s="13" t="s">
-        <v>515</v>
+        <v>503</v>
       </c>
       <c r="AE23" s="13" t="s">
         <v>293</v>
       </c>
       <c r="AF23" s="13" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
       <c r="AG23" s="13" t="s">
-        <v>514</v>
+        <v>502</v>
       </c>
       <c r="AH23" s="13" t="s">
-        <v>513</v>
+        <v>501</v>
       </c>
       <c r="AI23" s="54" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="24" spans="1:35" ht="217" customHeight="1">
@@ -8547,7 +8433,7 @@
         <v>2019</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="I24" s="9" t="s">
         <v>21</v>
@@ -8583,16 +8469,16 @@
         <v>26</v>
       </c>
       <c r="T24" s="11" t="s">
-        <v>615</v>
+        <v>602</v>
       </c>
       <c r="U24" s="11" t="s">
-        <v>618</v>
+        <v>605</v>
       </c>
       <c r="V24" s="11" t="s">
-        <v>699</v>
+        <v>686</v>
       </c>
       <c r="W24" s="11" t="s">
-        <v>771</v>
+        <v>758</v>
       </c>
       <c r="X24" s="11" t="s">
         <v>26</v>
@@ -8614,10 +8500,10 @@
         <v>207</v>
       </c>
       <c r="AE24" s="11" t="s">
-        <v>612</v>
+        <v>599</v>
       </c>
       <c r="AF24" s="11" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
       <c r="AG24" s="11" t="s">
         <v>208</v>
@@ -8626,7 +8512,7 @@
         <v>26</v>
       </c>
       <c r="AI24" s="54" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="25" spans="1:35" ht="231" customHeight="1">
@@ -8673,40 +8559,40 @@
         <v>4</v>
       </c>
       <c r="O25" s="9" t="s">
-        <v>619</v>
+        <v>606</v>
       </c>
       <c r="P25" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="Q25" s="9" t="s">
         <v>26</v>
       </c>
       <c r="R25" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="S25" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="T25" s="11" t="s">
-        <v>717</v>
+        <v>704</v>
       </c>
       <c r="U25" s="11" t="s">
-        <v>620</v>
+        <v>607</v>
       </c>
       <c r="V25" s="11" t="s">
-        <v>652</v>
+        <v>639</v>
       </c>
       <c r="W25" s="11" t="s">
-        <v>769</v>
+        <v>756</v>
       </c>
       <c r="X25" s="11" t="s">
-        <v>700</v>
+        <v>687</v>
       </c>
       <c r="Y25" s="11" t="s">
         <v>26</v>
       </c>
       <c r="Z25" s="9" t="s">
-        <v>563</v>
+        <v>551</v>
       </c>
       <c r="AA25" s="11" t="s">
         <v>26</v>
@@ -8719,10 +8605,10 @@
         <v>217</v>
       </c>
       <c r="AE25" s="11" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="AF25" s="11" t="s">
-        <v>592</v>
+        <v>580</v>
       </c>
       <c r="AG25" s="11" t="s">
         <v>218</v>
@@ -8731,7 +8617,7 @@
         <v>26</v>
       </c>
       <c r="AI25" s="54" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="26" spans="1:35" ht="301" customHeight="1">
@@ -8772,37 +8658,37 @@
         <v>24</v>
       </c>
       <c r="M26" s="9" t="s">
-        <v>538</v>
+        <v>526</v>
       </c>
       <c r="N26" s="10">
         <v>8</v>
       </c>
       <c r="O26" s="9" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="P26" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="Q26" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="R26" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S26" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="T26" s="11" t="s">
-        <v>716</v>
+        <v>703</v>
       </c>
       <c r="U26" s="11" t="s">
-        <v>730</v>
+        <v>717</v>
       </c>
       <c r="V26" s="11" t="s">
-        <v>637</v>
+        <v>624</v>
       </c>
       <c r="W26" s="11" t="s">
-        <v>772</v>
+        <v>759</v>
       </c>
       <c r="X26" s="11" t="s">
         <v>225</v>
@@ -8811,7 +8697,7 @@
         <v>226</v>
       </c>
       <c r="Z26" s="9" t="s">
-        <v>564</v>
+        <v>552</v>
       </c>
       <c r="AA26" s="11" t="s">
         <v>225</v>
@@ -8824,10 +8710,10 @@
         <v>228</v>
       </c>
       <c r="AE26" s="11" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="AF26" s="11" t="s">
-        <v>593</v>
+        <v>581</v>
       </c>
       <c r="AG26" s="11" t="s">
         <v>229</v>
@@ -8836,7 +8722,7 @@
         <v>230</v>
       </c>
       <c r="AI26" s="54" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="27" spans="1:35" ht="223" customHeight="1">
@@ -8883,7 +8769,7 @@
         <v>4</v>
       </c>
       <c r="O27" s="9" t="s">
-        <v>731</v>
+        <v>718</v>
       </c>
       <c r="P27" s="9" t="s">
         <v>26</v>
@@ -8898,16 +8784,16 @@
         <v>26</v>
       </c>
       <c r="T27" s="11" t="s">
-        <v>615</v>
+        <v>602</v>
       </c>
       <c r="U27" s="11" t="s">
         <v>235</v>
       </c>
       <c r="V27" s="11" t="s">
-        <v>699</v>
+        <v>686</v>
       </c>
       <c r="W27" s="11" t="s">
-        <v>771</v>
+        <v>758</v>
       </c>
       <c r="X27" s="11" t="s">
         <v>26</v>
@@ -8916,7 +8802,7 @@
         <v>26</v>
       </c>
       <c r="Z27" s="9" t="s">
-        <v>565</v>
+        <v>553</v>
       </c>
       <c r="AA27" s="11" t="s">
         <v>26</v>
@@ -8929,10 +8815,10 @@
         <v>237</v>
       </c>
       <c r="AE27" s="11" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="AF27" s="11" t="s">
-        <v>592</v>
+        <v>580</v>
       </c>
       <c r="AG27" s="11" t="s">
         <v>238</v>
@@ -8941,7 +8827,7 @@
         <v>239</v>
       </c>
       <c r="AI27" s="54" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="28" spans="1:35" ht="187" customHeight="1">
@@ -8967,7 +8853,7 @@
         <v>2016</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="I28" s="9" t="s">
         <v>34</v>
@@ -8982,37 +8868,37 @@
         <v>245</v>
       </c>
       <c r="M28" s="9" t="s">
-        <v>539</v>
+        <v>527</v>
       </c>
       <c r="N28" s="10">
         <v>13</v>
       </c>
       <c r="O28" s="9" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="P28" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="Q28" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="R28" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S28" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="T28" s="11" t="s">
-        <v>717</v>
+        <v>704</v>
       </c>
       <c r="U28" s="11" t="s">
         <v>246</v>
       </c>
       <c r="V28" s="11" t="s">
-        <v>637</v>
+        <v>624</v>
       </c>
       <c r="W28" s="11" t="s">
-        <v>769</v>
+        <v>756</v>
       </c>
       <c r="X28" s="11" t="s">
         <v>247</v>
@@ -9021,7 +8907,7 @@
         <v>26</v>
       </c>
       <c r="Z28" s="9" t="s">
-        <v>566</v>
+        <v>554</v>
       </c>
       <c r="AA28" s="11" t="s">
         <v>248</v>
@@ -9037,7 +8923,7 @@
         <v>28</v>
       </c>
       <c r="AF28" s="11" t="s">
-        <v>594</v>
+        <v>582</v>
       </c>
       <c r="AG28" s="11" t="s">
         <v>251</v>
@@ -9046,7 +8932,7 @@
         <v>252</v>
       </c>
       <c r="AI28" s="54" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="29" spans="1:35" ht="195" customHeight="1">
@@ -9093,40 +8979,40 @@
         <v>11</v>
       </c>
       <c r="O29" s="9" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="P29" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="Q29" s="9" t="s">
         <v>26</v>
       </c>
       <c r="R29" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="S29" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="T29" s="11" t="s">
         <v>314</v>
       </c>
       <c r="U29" s="11" t="s">
-        <v>732</v>
+        <v>719</v>
       </c>
       <c r="V29" s="11" t="s">
-        <v>652</v>
+        <v>639</v>
       </c>
       <c r="W29" s="11" t="s">
-        <v>701</v>
+        <v>688</v>
       </c>
       <c r="X29" s="11" t="s">
-        <v>701</v>
+        <v>688</v>
       </c>
       <c r="Y29" s="11" t="s">
         <v>261</v>
       </c>
       <c r="Z29" s="9" t="s">
-        <v>567</v>
+        <v>555</v>
       </c>
       <c r="AA29" s="11" t="s">
         <v>26</v>
@@ -9142,7 +9028,7 @@
         <v>28</v>
       </c>
       <c r="AF29" s="11" t="s">
-        <v>592</v>
+        <v>580</v>
       </c>
       <c r="AG29" s="11" t="s">
         <v>264</v>
@@ -9151,7 +9037,7 @@
         <v>265</v>
       </c>
       <c r="AI29" s="54" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="30" spans="1:35" ht="317" customHeight="1">
@@ -9168,7 +9054,7 @@
         <v>2019</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="F30" s="15" t="s">
         <v>267</v>
@@ -9192,25 +9078,25 @@
         <v>144</v>
       </c>
       <c r="M30" s="9" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="N30" s="10">
         <v>8</v>
       </c>
       <c r="O30" s="52" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="P30" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="Q30" s="9" t="s">
         <v>26</v>
       </c>
       <c r="R30" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="S30" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="T30" s="11" t="s">
         <v>314</v>
@@ -9219,13 +9105,13 @@
         <v>271</v>
       </c>
       <c r="V30" s="11" t="s">
-        <v>652</v>
+        <v>639</v>
       </c>
       <c r="W30" s="11" t="s">
-        <v>701</v>
+        <v>688</v>
       </c>
       <c r="X30" s="11" t="s">
-        <v>701</v>
+        <v>688</v>
       </c>
       <c r="Y30" s="11" t="s">
         <v>26</v>
@@ -9238,25 +9124,25 @@
       </c>
       <c r="AB30" s="11"/>
       <c r="AC30" s="13" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="AD30" s="13" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="AE30" s="13" t="s">
         <v>28</v>
       </c>
       <c r="AF30" s="13" t="s">
-        <v>595</v>
+        <v>583</v>
       </c>
       <c r="AG30" s="13" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="AH30" s="13" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="AI30" s="54" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="31" spans="1:35" ht="238" customHeight="1">
@@ -9273,7 +9159,7 @@
         <v>2019</v>
       </c>
       <c r="E31" s="41" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="F31" s="40" t="s">
         <v>273</v>
@@ -9297,20 +9183,20 @@
         <v>88</v>
       </c>
       <c r="M31" s="41" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="N31" s="45">
         <v>31</v>
       </c>
       <c r="O31" s="41" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="P31" s="41"/>
       <c r="Q31" s="41"/>
       <c r="R31" s="41"/>
       <c r="S31" s="41"/>
       <c r="T31" s="40" t="s">
-        <v>622</v>
+        <v>609</v>
       </c>
       <c r="U31" s="40" t="s">
         <v>276</v>
@@ -9329,7 +9215,7 @@
       <c r="AG31" s="42"/>
       <c r="AH31" s="42"/>
       <c r="AI31" s="1" t="s">
-        <v>741</v>
+        <v>728</v>
       </c>
     </row>
     <row r="32" spans="1:35" ht="226" customHeight="1">
@@ -9346,7 +9232,7 @@
         <v>2018</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="F32" s="11" t="s">
         <v>278</v>
@@ -9361,22 +9247,22 @@
         <v>21</v>
       </c>
       <c r="J32" s="26" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="K32" s="26" t="s">
-        <v>528</v>
+        <v>516</v>
       </c>
       <c r="L32" s="11" t="s">
         <v>24</v>
       </c>
       <c r="M32" s="9" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="N32" s="10">
         <v>5</v>
       </c>
       <c r="O32" s="9" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="P32" s="9" t="s">
         <v>26</v>
@@ -9391,16 +9277,16 @@
         <v>26</v>
       </c>
       <c r="T32" s="11" t="s">
-        <v>733</v>
+        <v>720</v>
       </c>
       <c r="U32" s="11" t="s">
         <v>280</v>
       </c>
       <c r="V32" s="11" t="s">
-        <v>674</v>
+        <v>661</v>
       </c>
       <c r="W32" s="11" t="s">
-        <v>770</v>
+        <v>757</v>
       </c>
       <c r="X32" s="11" t="s">
         <v>281</v>
@@ -9409,10 +9295,10 @@
         <v>26</v>
       </c>
       <c r="Z32" s="9" t="s">
-        <v>568</v>
+        <v>556</v>
       </c>
       <c r="AA32" s="11" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="AB32" s="11"/>
       <c r="AC32" s="11" t="s">
@@ -9425,7 +9311,7 @@
         <v>284</v>
       </c>
       <c r="AF32" s="11" t="s">
-        <v>596</v>
+        <v>584</v>
       </c>
       <c r="AG32" s="11" t="s">
         <v>285</v>
@@ -9434,7 +9320,7 @@
         <v>26</v>
       </c>
       <c r="AI32" s="54" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="33" spans="1:35" ht="274" customHeight="1">
@@ -9451,7 +9337,7 @@
         <v>2017</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="F33" s="27" t="s">
         <v>287</v>
@@ -9466,10 +9352,10 @@
         <v>21</v>
       </c>
       <c r="J33" s="26" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="K33" s="26" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="L33" s="11" t="s">
         <v>259</v>
@@ -9481,19 +9367,19 @@
         <v>11</v>
       </c>
       <c r="O33" s="52" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="P33" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="Q33" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="R33" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S33" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="T33" s="11" t="s">
         <v>290</v>
@@ -9502,10 +9388,10 @@
         <v>290</v>
       </c>
       <c r="V33" s="11" t="s">
-        <v>699</v>
+        <v>686</v>
       </c>
       <c r="W33" s="11" t="s">
-        <v>771</v>
+        <v>758</v>
       </c>
       <c r="X33" s="11" t="s">
         <v>26</v>
@@ -9530,16 +9416,16 @@
         <v>293</v>
       </c>
       <c r="AF33" s="11" t="s">
-        <v>597</v>
+        <v>585</v>
       </c>
       <c r="AG33" s="11" t="s">
         <v>294</v>
       </c>
       <c r="AH33" s="11" t="s">
-        <v>629</v>
+        <v>616</v>
       </c>
       <c r="AI33" s="54" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="34" spans="1:35" ht="235" customHeight="1">
@@ -9556,7 +9442,7 @@
         <v>2016</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="F34" s="11" t="s">
         <v>296</v>
@@ -9571,46 +9457,46 @@
         <v>167</v>
       </c>
       <c r="J34" s="26" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="K34" s="26" t="s">
-        <v>529</v>
+        <v>517</v>
       </c>
       <c r="L34" s="11" t="s">
         <v>24</v>
       </c>
       <c r="M34" s="9" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="N34" s="10">
         <v>8</v>
       </c>
       <c r="O34" s="9" t="s">
-        <v>548</v>
+        <v>536</v>
       </c>
       <c r="P34" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="Q34" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="R34" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S34" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="T34" s="11" t="s">
         <v>314</v>
       </c>
       <c r="U34" s="11" t="s">
-        <v>734</v>
+        <v>721</v>
       </c>
       <c r="V34" s="11" t="s">
-        <v>637</v>
+        <v>624</v>
       </c>
       <c r="W34" s="11" t="s">
-        <v>771</v>
+        <v>758</v>
       </c>
       <c r="X34" s="11" t="s">
         <v>26</v>
@@ -9619,7 +9505,7 @@
         <v>26</v>
       </c>
       <c r="Z34" s="11" t="s">
-        <v>766</v>
+        <v>753</v>
       </c>
       <c r="AA34" s="11" t="s">
         <v>26</v>
@@ -9635,7 +9521,7 @@
         <v>300</v>
       </c>
       <c r="AF34" s="11" t="s">
-        <v>598</v>
+        <v>586</v>
       </c>
       <c r="AG34" s="11" t="s">
         <v>301</v>
@@ -9644,7 +9530,7 @@
         <v>26</v>
       </c>
       <c r="AI34" s="54" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="35" spans="1:35" ht="270" customHeight="1">
@@ -9661,7 +9547,7 @@
         <v>2016</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="F35" s="28" t="s">
         <v>303</v>
@@ -9670,7 +9556,7 @@
         <v>2016</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>525</v>
+        <v>513</v>
       </c>
       <c r="I35" s="26" t="s">
         <v>21</v>
@@ -9691,31 +9577,31 @@
         <v>8</v>
       </c>
       <c r="O35" s="9" t="s">
-        <v>702</v>
+        <v>689</v>
       </c>
       <c r="P35" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="Q35" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="R35" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S35" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="T35" s="11" t="s">
         <v>314</v>
       </c>
       <c r="U35" s="11" t="s">
-        <v>735</v>
+        <v>722</v>
       </c>
       <c r="V35" s="11" t="s">
-        <v>637</v>
+        <v>624</v>
       </c>
       <c r="W35" s="11" t="s">
-        <v>771</v>
+        <v>758</v>
       </c>
       <c r="X35" s="11" t="s">
         <v>26</v>
@@ -9731,25 +9617,25 @@
       </c>
       <c r="AB35" s="13"/>
       <c r="AC35" s="13" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="AD35" s="13" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="AE35" s="13" t="s">
         <v>293</v>
       </c>
       <c r="AF35" s="13" t="s">
-        <v>599</v>
+        <v>587</v>
       </c>
       <c r="AG35" s="13" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="AH35" s="13" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="AI35" s="54" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="36" spans="1:35" ht="202" customHeight="1">
@@ -9766,7 +9652,7 @@
         <v>2017</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
       <c r="F36" s="28" t="s">
         <v>307</v>
@@ -9799,28 +9685,28 @@
         <v>313</v>
       </c>
       <c r="P36" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="Q36" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="R36" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S36" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="T36" s="11" t="s">
         <v>314</v>
       </c>
       <c r="U36" s="11" t="s">
-        <v>622</v>
+        <v>609</v>
       </c>
       <c r="V36" s="11" t="s">
-        <v>652</v>
+        <v>639</v>
       </c>
       <c r="W36" s="11" t="s">
-        <v>771</v>
+        <v>758</v>
       </c>
       <c r="X36" s="11" t="s">
         <v>26</v>
@@ -9836,25 +9722,25 @@
       </c>
       <c r="AB36" s="11"/>
       <c r="AC36" s="13" t="s">
-        <v>509</v>
+        <v>497</v>
       </c>
       <c r="AD36" s="13" t="s">
-        <v>506</v>
+        <v>494</v>
       </c>
       <c r="AE36" s="13" t="s">
-        <v>508</v>
+        <v>496</v>
       </c>
       <c r="AF36" s="13" t="s">
-        <v>600</v>
+        <v>588</v>
       </c>
       <c r="AG36" s="13" t="s">
-        <v>507</v>
+        <v>495</v>
       </c>
       <c r="AH36" s="30" t="s">
-        <v>505</v>
+        <v>493</v>
       </c>
       <c r="AI36" s="54" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="37" spans="1:35" ht="225" customHeight="1">
@@ -9871,7 +9757,7 @@
         <v>2015</v>
       </c>
       <c r="E37" s="41" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="F37" s="41" t="s">
         <v>316</v>
@@ -9880,7 +9766,7 @@
         <v>2015</v>
       </c>
       <c r="H37" s="9" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="I37" s="26" t="s">
         <v>34</v>
@@ -9895,34 +9781,34 @@
         <v>311</v>
       </c>
       <c r="M37" s="9" t="s">
-        <v>540</v>
+        <v>528</v>
       </c>
       <c r="N37" s="10">
         <v>17</v>
       </c>
       <c r="O37" s="41" t="s">
-        <v>549</v>
+        <v>537</v>
       </c>
       <c r="P37" s="41" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="Q37" s="41" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="R37" s="41" t="s">
         <v>26</v>
       </c>
       <c r="S37" s="41" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="T37" s="40" t="s">
         <v>314</v>
       </c>
       <c r="U37" s="40" t="s">
-        <v>736</v>
+        <v>723</v>
       </c>
       <c r="V37" s="40" t="s">
-        <v>637</v>
+        <v>624</v>
       </c>
       <c r="W37" s="40"/>
       <c r="X37" s="40"/>
@@ -9937,7 +9823,7 @@
       <c r="AG37" s="42"/>
       <c r="AH37" s="42"/>
       <c r="AI37" s="1" t="s">
-        <v>741</v>
+        <v>728</v>
       </c>
     </row>
     <row r="38" spans="1:35" ht="270" customHeight="1">
@@ -9954,7 +9840,7 @@
         <v>2018</v>
       </c>
       <c r="E38" s="41" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="F38" s="41" t="s">
         <v>319</v>
@@ -9963,7 +9849,7 @@
         <v>2018</v>
       </c>
       <c r="H38" s="41" t="s">
-        <v>630</v>
+        <v>617</v>
       </c>
       <c r="I38" s="44" t="s">
         <v>21</v>
@@ -9978,13 +9864,13 @@
         <v>88</v>
       </c>
       <c r="M38" s="41" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
       <c r="N38" s="45">
         <v>27</v>
       </c>
       <c r="O38" s="41" t="s">
-        <v>624</v>
+        <v>611</v>
       </c>
       <c r="P38" s="41"/>
       <c r="Q38" s="41"/>
@@ -10006,7 +9892,7 @@
       <c r="AG38" s="42"/>
       <c r="AH38" s="42"/>
       <c r="AI38" s="1" t="s">
-        <v>741</v>
+        <v>728</v>
       </c>
     </row>
     <row r="39" spans="1:35" ht="243" customHeight="1">
@@ -10032,7 +9918,7 @@
         <v>2019</v>
       </c>
       <c r="H39" s="9" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="I39" s="9" t="s">
         <v>21</v>
@@ -10047,37 +9933,37 @@
         <v>259</v>
       </c>
       <c r="M39" s="9" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="N39" s="10">
         <v>11</v>
       </c>
       <c r="O39" s="9" t="s">
-        <v>703</v>
+        <v>690</v>
       </c>
       <c r="P39" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="Q39" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="R39" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S39" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="T39" s="11" t="s">
         <v>290</v>
       </c>
       <c r="U39" s="13" t="s">
-        <v>737</v>
+        <v>724</v>
       </c>
       <c r="V39" s="11" t="s">
-        <v>699</v>
+        <v>686</v>
       </c>
       <c r="W39" s="11" t="s">
-        <v>771</v>
+        <v>758</v>
       </c>
       <c r="X39" s="13" t="s">
         <v>26</v>
@@ -10093,25 +9979,25 @@
       </c>
       <c r="AB39" s="13"/>
       <c r="AC39" s="13" t="s">
-        <v>523</v>
+        <v>511</v>
       </c>
       <c r="AD39" s="13" t="s">
-        <v>522</v>
+        <v>510</v>
       </c>
       <c r="AE39" s="13" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="AF39" s="13" t="s">
-        <v>601</v>
+        <v>589</v>
       </c>
       <c r="AG39" s="13" t="s">
-        <v>521</v>
+        <v>509</v>
       </c>
       <c r="AH39" s="13" t="s">
-        <v>520</v>
+        <v>508</v>
       </c>
       <c r="AI39" s="54" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="40" spans="1:35" ht="220" customHeight="1">
@@ -10131,7 +10017,7 @@
         <v>328</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="G40" s="8">
         <v>2017</v>
@@ -10143,22 +10029,22 @@
         <v>21</v>
       </c>
       <c r="J40" s="9" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="K40" s="9" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="L40" s="11" t="s">
         <v>88</v>
       </c>
       <c r="M40" s="9" t="s">
-        <v>541</v>
+        <v>529</v>
       </c>
       <c r="N40" s="10">
         <v>5</v>
       </c>
       <c r="O40" s="9" t="s">
-        <v>704</v>
+        <v>691</v>
       </c>
       <c r="P40" s="9" t="s">
         <v>26</v>
@@ -10173,16 +10059,16 @@
         <v>26</v>
       </c>
       <c r="T40" s="11" t="s">
-        <v>625</v>
+        <v>612</v>
       </c>
       <c r="U40" s="11" t="s">
-        <v>625</v>
+        <v>612</v>
       </c>
       <c r="V40" s="11" t="s">
-        <v>674</v>
+        <v>661</v>
       </c>
       <c r="W40" s="11" t="s">
-        <v>771</v>
+        <v>758</v>
       </c>
       <c r="X40" s="13" t="s">
         <v>26</v>
@@ -10191,32 +10077,32 @@
         <v>26</v>
       </c>
       <c r="Z40" s="13" t="s">
-        <v>762</v>
+        <v>749</v>
       </c>
       <c r="AA40" s="13" t="s">
         <v>26</v>
       </c>
       <c r="AB40" s="13"/>
       <c r="AC40" s="13" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="AD40" s="13" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="AE40" s="13" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="AF40" s="13" t="s">
-        <v>602</v>
+        <v>590</v>
       </c>
       <c r="AG40" s="13" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="AH40" s="13" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="AI40" s="54" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="41" spans="1:35" ht="227" customHeight="1">
@@ -10233,7 +10119,7 @@
         <v>2012</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="F41" s="9" t="s">
         <v>331</v>
@@ -10242,7 +10128,7 @@
         <v>2012</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>526</v>
+        <v>514</v>
       </c>
       <c r="I41" s="9" t="s">
         <v>34</v>
@@ -10263,738 +10149,633 @@
         <v>9</v>
       </c>
       <c r="O41" s="9" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="P41" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="Q41" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="R41" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S41" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="T41" s="11" t="s">
         <v>314</v>
       </c>
       <c r="U41" s="11" t="s">
-        <v>631</v>
+        <v>618</v>
       </c>
       <c r="V41" s="11" t="s">
-        <v>637</v>
+        <v>624</v>
       </c>
       <c r="W41" s="11" t="s">
-        <v>772</v>
+        <v>759</v>
       </c>
       <c r="X41" s="11" t="s">
-        <v>473</v>
+        <v>461</v>
       </c>
       <c r="Y41" s="13" t="s">
         <v>26</v>
       </c>
       <c r="Z41" s="13" t="s">
-        <v>763</v>
+        <v>750</v>
       </c>
       <c r="AA41" s="13" t="s">
-        <v>472</v>
+        <v>460</v>
       </c>
       <c r="AB41" s="13"/>
       <c r="AC41" s="13" t="s">
-        <v>626</v>
+        <v>613</v>
       </c>
       <c r="AD41" s="13" t="s">
-        <v>474</v>
+        <v>462</v>
       </c>
       <c r="AE41" s="13" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="AF41" s="13" t="s">
-        <v>603</v>
+        <v>591</v>
       </c>
       <c r="AG41" s="13" t="s">
-        <v>474</v>
+        <v>462</v>
       </c>
       <c r="AH41" s="13" t="s">
-        <v>475</v>
+        <v>463</v>
       </c>
       <c r="AI41" s="54" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
-    <row r="42" spans="1:35" ht="195" customHeight="1">
-      <c r="A42" s="8">
-        <v>82</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>330</v>
-      </c>
-      <c r="C42" s="8">
-        <v>106</v>
+    <row r="42" spans="1:35" ht="205" customHeight="1">
+      <c r="A42" s="39">
+        <v>85</v>
+      </c>
+      <c r="B42" s="41" t="s">
+        <v>334</v>
+      </c>
+      <c r="C42" s="39">
+        <v>1</v>
       </c>
       <c r="D42" s="55">
-        <v>2012</v>
-      </c>
-      <c r="E42" s="16" t="s">
+        <v>2018</v>
+      </c>
+      <c r="E42" s="46" t="s">
+        <v>335</v>
+      </c>
+      <c r="F42" s="47" t="s">
+        <v>336</v>
+      </c>
+      <c r="G42" s="48">
+        <v>2018</v>
+      </c>
+      <c r="H42" s="41" t="s">
+        <v>442</v>
+      </c>
+      <c r="I42" s="41" t="s">
+        <v>337</v>
+      </c>
+      <c r="J42" s="41" t="s">
+        <v>443</v>
+      </c>
+      <c r="K42" s="41" t="s">
+        <v>444</v>
+      </c>
+      <c r="L42" s="40" t="s">
+        <v>338</v>
+      </c>
+      <c r="M42" s="41" t="s">
+        <v>530</v>
+      </c>
+      <c r="N42" s="45">
+        <v>13</v>
+      </c>
+      <c r="O42" s="41" t="s">
+        <v>445</v>
+      </c>
+      <c r="P42" s="41"/>
+      <c r="Q42" s="41"/>
+      <c r="R42" s="41"/>
+      <c r="S42" s="41"/>
+      <c r="T42" s="40" t="s">
+        <v>314</v>
+      </c>
+      <c r="U42" s="40" t="s">
+        <v>314</v>
+      </c>
+      <c r="V42" s="40"/>
+      <c r="W42" s="40"/>
+      <c r="X42" s="40"/>
+      <c r="Y42" s="42"/>
+      <c r="Z42" s="42"/>
+      <c r="AA42" s="42"/>
+      <c r="AB42" s="42"/>
+      <c r="AC42" s="42"/>
+      <c r="AD42" s="42"/>
+      <c r="AE42" s="42"/>
+      <c r="AF42" s="42"/>
+      <c r="AG42" s="42"/>
+      <c r="AH42" s="42"/>
+      <c r="AI42" s="1" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="43" spans="1:35" ht="276" customHeight="1">
+      <c r="A43" s="8">
+        <v>88</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="C43" s="8">
+        <v>2</v>
+      </c>
+      <c r="D43" s="56">
+        <v>2019</v>
+      </c>
+      <c r="E43" s="36" t="s">
+        <v>340</v>
+      </c>
+      <c r="F43" s="31" t="s">
+        <v>341</v>
+      </c>
+      <c r="G43" s="21">
+        <v>2019</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>446</v>
+      </c>
+      <c r="I43" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J43" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K43" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="L43" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="M43" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="N43" s="10">
+        <v>5</v>
+      </c>
+      <c r="O43" s="9" t="s">
+        <v>447</v>
+      </c>
+      <c r="P43" s="9" t="s">
+        <v>621</v>
+      </c>
+      <c r="Q43" s="9" t="s">
+        <v>621</v>
+      </c>
+      <c r="R43" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="S43" s="9" t="s">
+        <v>621</v>
+      </c>
+      <c r="T43" s="11" t="s">
+        <v>314</v>
+      </c>
+      <c r="U43" s="11" t="s">
+        <v>725</v>
+      </c>
+      <c r="V43" s="11" t="s">
+        <v>624</v>
+      </c>
+      <c r="W43" s="11" t="s">
+        <v>756</v>
+      </c>
+      <c r="X43" s="11" t="s">
+        <v>692</v>
+      </c>
+      <c r="Y43" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z43" s="9" t="s">
+        <v>557</v>
+      </c>
+      <c r="AA43" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB43" s="11"/>
+      <c r="AC43" s="13" t="s">
+        <v>376</v>
+      </c>
+      <c r="AD43" s="13" t="s">
         <v>378</v>
       </c>
-      <c r="F42" s="16" t="s">
-        <v>449</v>
-      </c>
-      <c r="G42" s="8">
-        <v>2012</v>
-      </c>
-      <c r="H42" s="9" t="s">
-        <v>450</v>
-      </c>
-      <c r="I42" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="J42" s="9" t="s">
-        <v>334</v>
-      </c>
-      <c r="K42" s="9" t="s">
-        <v>335</v>
-      </c>
-      <c r="L42" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="M42" s="9" t="s">
-        <v>451</v>
-      </c>
-      <c r="N42" s="10">
-        <v>5</v>
-      </c>
-      <c r="O42" s="9" t="s">
-        <v>452</v>
-      </c>
-      <c r="P42" s="9" t="s">
-        <v>634</v>
-      </c>
-      <c r="Q42" s="9" t="s">
-        <v>634</v>
-      </c>
-      <c r="R42" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="S42" s="9" t="s">
-        <v>634</v>
-      </c>
-      <c r="T42" s="11" t="s">
-        <v>314</v>
-      </c>
-      <c r="U42" s="11" t="s">
-        <v>631</v>
-      </c>
-      <c r="V42" s="11" t="s">
-        <v>637</v>
-      </c>
-      <c r="W42" s="11" t="s">
-        <v>772</v>
-      </c>
-      <c r="X42" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="Y42" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z42" s="13" t="s">
-        <v>763</v>
-      </c>
-      <c r="AA42" s="11" t="s">
-        <v>453</v>
-      </c>
-      <c r="AB42" s="11"/>
-      <c r="AC42" s="13" t="s">
+      <c r="AE43" s="13" t="s">
+        <v>377</v>
+      </c>
+      <c r="AF43" s="13" t="s">
+        <v>592</v>
+      </c>
+      <c r="AG43" s="13" t="s">
+        <v>378</v>
+      </c>
+      <c r="AH43" s="13" t="s">
         <v>379</v>
       </c>
-      <c r="AD42" s="13" t="s">
-        <v>381</v>
-      </c>
-      <c r="AE42" s="13" t="s">
-        <v>375</v>
-      </c>
-      <c r="AF42" s="13" t="s">
-        <v>604</v>
-      </c>
-      <c r="AG42" s="13" t="s">
-        <v>380</v>
-      </c>
-      <c r="AH42" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="AI42" s="54" t="s">
-        <v>740</v>
+      <c r="AI43" s="54" t="s">
+        <v>727</v>
       </c>
     </row>
-    <row r="43" spans="1:35" ht="205" customHeight="1">
-      <c r="A43" s="39">
-        <v>85</v>
-      </c>
-      <c r="B43" s="41" t="s">
-        <v>336</v>
-      </c>
-      <c r="C43" s="39">
-        <v>1</v>
-      </c>
-      <c r="D43" s="56">
-        <v>2018</v>
-      </c>
-      <c r="E43" s="46" t="s">
-        <v>337</v>
-      </c>
-      <c r="F43" s="47" t="s">
-        <v>338</v>
-      </c>
-      <c r="G43" s="48">
-        <v>2018</v>
-      </c>
-      <c r="H43" s="41" t="s">
-        <v>454</v>
-      </c>
-      <c r="I43" s="41" t="s">
-        <v>339</v>
-      </c>
-      <c r="J43" s="41" t="s">
-        <v>455</v>
-      </c>
-      <c r="K43" s="41" t="s">
-        <v>456</v>
-      </c>
-      <c r="L43" s="40" t="s">
-        <v>340</v>
-      </c>
-      <c r="M43" s="41" t="s">
-        <v>542</v>
-      </c>
-      <c r="N43" s="45">
-        <v>13</v>
-      </c>
-      <c r="O43" s="41" t="s">
-        <v>457</v>
-      </c>
-      <c r="P43" s="41"/>
-      <c r="Q43" s="41"/>
-      <c r="R43" s="41"/>
-      <c r="S43" s="41"/>
-      <c r="T43" s="40" t="s">
-        <v>314</v>
-      </c>
-      <c r="U43" s="40" t="s">
-        <v>314</v>
-      </c>
-      <c r="V43" s="40"/>
-      <c r="W43" s="40"/>
-      <c r="X43" s="40"/>
-      <c r="Y43" s="42"/>
-      <c r="Z43" s="42"/>
-      <c r="AA43" s="42"/>
-      <c r="AB43" s="42"/>
-      <c r="AC43" s="42"/>
-      <c r="AD43" s="42"/>
-      <c r="AE43" s="42"/>
-      <c r="AF43" s="42"/>
-      <c r="AG43" s="42"/>
-      <c r="AH43" s="42"/>
-      <c r="AI43" s="1" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="44" spans="1:35" ht="276" customHeight="1">
+    <row r="44" spans="1:35" ht="231" customHeight="1">
       <c r="A44" s="8">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="C44" s="8">
-        <v>2</v>
-      </c>
-      <c r="D44" s="57">
+        <v>6</v>
+      </c>
+      <c r="D44" s="56">
         <v>2019</v>
       </c>
       <c r="E44" s="36" t="s">
-        <v>342</v>
-      </c>
-      <c r="F44" s="31" t="s">
-        <v>343</v>
+        <v>344</v>
+      </c>
+      <c r="F44" s="32" t="s">
+        <v>345</v>
       </c>
       <c r="G44" s="21">
         <v>2019</v>
       </c>
       <c r="H44" s="9" t="s">
-        <v>458</v>
+        <v>346</v>
       </c>
       <c r="I44" s="9" t="s">
         <v>21</v>
       </c>
       <c r="J44" s="9" t="s">
-        <v>22</v>
+        <v>347</v>
       </c>
       <c r="K44" s="9" t="s">
-        <v>23</v>
+        <v>518</v>
       </c>
       <c r="L44" s="11" t="s">
-        <v>24</v>
+        <v>88</v>
       </c>
       <c r="M44" s="9" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="N44" s="10">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="O44" s="9" t="s">
-        <v>459</v>
+        <v>693</v>
       </c>
       <c r="P44" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="Q44" s="9" t="s">
-        <v>634</v>
+        <v>26</v>
       </c>
       <c r="R44" s="9" t="s">
-        <v>26</v>
+        <v>621</v>
       </c>
       <c r="S44" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="T44" s="11" t="s">
         <v>314</v>
       </c>
       <c r="U44" s="11" t="s">
-        <v>738</v>
+        <v>608</v>
       </c>
       <c r="V44" s="11" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="W44" s="11" t="s">
-        <v>769</v>
+        <v>686</v>
       </c>
       <c r="X44" s="11" t="s">
-        <v>705</v>
-      </c>
-      <c r="Y44" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z44" s="9" t="s">
-        <v>569</v>
+        <v>26</v>
+      </c>
+      <c r="Y44" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z44" s="13" t="s">
+        <v>558</v>
       </c>
       <c r="AA44" s="11" t="s">
         <v>26</v>
       </c>
       <c r="AB44" s="11"/>
       <c r="AC44" s="13" t="s">
-        <v>383</v>
+        <v>475</v>
       </c>
       <c r="AD44" s="13" t="s">
-        <v>385</v>
+        <v>478</v>
       </c>
       <c r="AE44" s="13" t="s">
-        <v>384</v>
+        <v>476</v>
       </c>
       <c r="AF44" s="13" t="s">
-        <v>605</v>
+        <v>593</v>
       </c>
       <c r="AG44" s="13" t="s">
-        <v>385</v>
+        <v>477</v>
       </c>
       <c r="AH44" s="13" t="s">
-        <v>386</v>
+        <v>474</v>
       </c>
       <c r="AI44" s="54" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
-    <row r="45" spans="1:35" ht="231" customHeight="1">
+    <row r="45" spans="1:35" ht="268" customHeight="1">
       <c r="A45" s="8">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="C45" s="8">
-        <v>6</v>
-      </c>
-      <c r="D45" s="57">
-        <v>2019</v>
+        <v>10</v>
+      </c>
+      <c r="D45" s="56">
+        <v>2018</v>
       </c>
       <c r="E45" s="36" t="s">
-        <v>346</v>
-      </c>
-      <c r="F45" s="32" t="s">
-        <v>347</v>
+        <v>531</v>
+      </c>
+      <c r="F45" s="33" t="s">
+        <v>614</v>
       </c>
       <c r="G45" s="21">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="H45" s="9" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="I45" s="9" t="s">
         <v>21</v>
       </c>
       <c r="J45" s="9" t="s">
-        <v>349</v>
+        <v>448</v>
       </c>
       <c r="K45" s="9" t="s">
-        <v>530</v>
+        <v>519</v>
       </c>
       <c r="L45" s="11" t="s">
-        <v>88</v>
+        <v>24</v>
       </c>
       <c r="M45" s="9" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="N45" s="10">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O45" s="9" t="s">
-        <v>706</v>
+        <v>469</v>
       </c>
       <c r="P45" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="Q45" s="9" t="s">
         <v>26</v>
       </c>
       <c r="R45" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="S45" s="9" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="T45" s="11" t="s">
-        <v>314</v>
+        <v>610</v>
       </c>
       <c r="U45" s="11" t="s">
-        <v>621</v>
+        <v>290</v>
       </c>
       <c r="V45" s="11" t="s">
-        <v>652</v>
+        <v>686</v>
       </c>
       <c r="W45" s="11" t="s">
-        <v>699</v>
+        <v>758</v>
       </c>
       <c r="X45" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y45" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z45" s="13" t="s">
-        <v>570</v>
-      </c>
-      <c r="AA45" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB45" s="11"/>
+        <v>464</v>
+      </c>
+      <c r="Y45" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z45" s="9" t="s">
+        <v>559</v>
+      </c>
+      <c r="AA45" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB45" s="13"/>
       <c r="AC45" s="13" t="s">
-        <v>487</v>
+        <v>468</v>
       </c>
       <c r="AD45" s="13" t="s">
-        <v>490</v>
+        <v>467</v>
       </c>
       <c r="AE45" s="13" t="s">
-        <v>488</v>
+        <v>373</v>
       </c>
       <c r="AF45" s="13" t="s">
-        <v>606</v>
+        <v>594</v>
       </c>
       <c r="AG45" s="13" t="s">
-        <v>489</v>
+        <v>466</v>
       </c>
       <c r="AH45" s="13" t="s">
-        <v>486</v>
+        <v>465</v>
       </c>
       <c r="AI45" s="54" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
-    <row r="46" spans="1:35" ht="268" customHeight="1">
+    <row r="46" spans="1:35" ht="159" customHeight="1">
       <c r="A46" s="8">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C46" s="8">
-        <v>10</v>
-      </c>
-      <c r="D46" s="57">
-        <v>2018</v>
+        <v>0</v>
+      </c>
+      <c r="D46" s="56">
+        <v>2017</v>
       </c>
       <c r="E46" s="36" t="s">
-        <v>543</v>
-      </c>
-      <c r="F46" s="33" t="s">
-        <v>627</v>
+        <v>353</v>
+      </c>
+      <c r="F46" s="32" t="s">
+        <v>354</v>
       </c>
       <c r="G46" s="21">
-        <v>2018</v>
-      </c>
-      <c r="H46" s="9" t="s">
-        <v>352</v>
+        <v>2017</v>
+      </c>
+      <c r="H46" s="15" t="s">
+        <v>355</v>
       </c>
       <c r="I46" s="9" t="s">
         <v>21</v>
       </c>
       <c r="J46" s="9" t="s">
-        <v>460</v>
+        <v>356</v>
       </c>
       <c r="K46" s="9" t="s">
-        <v>531</v>
+        <v>357</v>
       </c>
       <c r="L46" s="11" t="s">
-        <v>24</v>
+        <v>144</v>
       </c>
       <c r="M46" s="9" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
       <c r="N46" s="10">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="O46" s="9" t="s">
-        <v>481</v>
+        <v>416</v>
       </c>
       <c r="P46" s="9" t="s">
-        <v>634</v>
+        <v>26</v>
       </c>
       <c r="Q46" s="9" t="s">
         <v>26</v>
       </c>
       <c r="R46" s="9" t="s">
-        <v>634</v>
+        <v>26</v>
       </c>
       <c r="S46" s="9" t="s">
-        <v>634</v>
+        <v>26</v>
       </c>
       <c r="T46" s="11" t="s">
-        <v>623</v>
+        <v>720</v>
       </c>
       <c r="U46" s="11" t="s">
-        <v>290</v>
+        <v>359</v>
       </c>
       <c r="V46" s="11" t="s">
-        <v>699</v>
+        <v>694</v>
       </c>
       <c r="W46" s="11" t="s">
-        <v>771</v>
+        <v>758</v>
       </c>
       <c r="X46" s="11" t="s">
-        <v>476</v>
+        <v>26</v>
       </c>
       <c r="Y46" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="Z46" s="9" t="s">
-        <v>571</v>
-      </c>
-      <c r="AA46" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB46" s="13"/>
-      <c r="AC46" s="13" t="s">
-        <v>480</v>
-      </c>
-      <c r="AD46" s="13" t="s">
-        <v>479</v>
-      </c>
-      <c r="AE46" s="13" t="s">
-        <v>375</v>
-      </c>
-      <c r="AF46" s="13" t="s">
-        <v>607</v>
-      </c>
-      <c r="AG46" s="13" t="s">
-        <v>478</v>
-      </c>
-      <c r="AH46" s="13" t="s">
-        <v>477</v>
+      <c r="Z46" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA46" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB46" s="11"/>
+      <c r="AC46" s="11" t="s">
+        <v>695</v>
+      </c>
+      <c r="AD46" s="11" t="s">
+        <v>696</v>
+      </c>
+      <c r="AE46" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="AF46" s="11" t="s">
+        <v>595</v>
+      </c>
+      <c r="AG46" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="AH46" s="11" t="s">
+        <v>362</v>
       </c>
       <c r="AI46" s="54" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
-    <row r="47" spans="1:35" ht="159" customHeight="1">
-      <c r="A47" s="8">
-        <v>97</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>354</v>
-      </c>
-      <c r="C47" s="8">
-        <v>0</v>
-      </c>
-      <c r="D47" s="57">
-        <v>2017</v>
-      </c>
-      <c r="E47" s="36" t="s">
-        <v>355</v>
-      </c>
-      <c r="F47" s="32" t="s">
-        <v>356</v>
-      </c>
-      <c r="G47" s="21">
-        <v>2017</v>
-      </c>
-      <c r="H47" s="15" t="s">
-        <v>357</v>
-      </c>
-      <c r="I47" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J47" s="9" t="s">
-        <v>358</v>
-      </c>
-      <c r="K47" s="9" t="s">
-        <v>359</v>
-      </c>
-      <c r="L47" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="M47" s="9" t="s">
-        <v>360</v>
-      </c>
-      <c r="N47" s="10">
-        <v>4</v>
-      </c>
-      <c r="O47" s="9" t="s">
-        <v>423</v>
-      </c>
-      <c r="P47" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q47" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="R47" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="S47" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="T47" s="11" t="s">
-        <v>733</v>
-      </c>
-      <c r="U47" s="11" t="s">
-        <v>361</v>
-      </c>
-      <c r="V47" s="11" t="s">
-        <v>707</v>
-      </c>
-      <c r="W47" s="11" t="s">
-        <v>771</v>
-      </c>
-      <c r="X47" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y47" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z47" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA47" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB47" s="11"/>
-      <c r="AC47" s="11" t="s">
-        <v>708</v>
-      </c>
-      <c r="AD47" s="11" t="s">
-        <v>709</v>
-      </c>
-      <c r="AE47" s="11" t="s">
-        <v>362</v>
-      </c>
-      <c r="AF47" s="11" t="s">
-        <v>608</v>
-      </c>
-      <c r="AG47" s="11" t="s">
+    <row r="47" spans="1:35" ht="283" customHeight="1">
+      <c r="A47" s="39">
+        <v>40</v>
+      </c>
+      <c r="B47" s="41" t="s">
         <v>363</v>
       </c>
-      <c r="AH47" s="11" t="s">
+      <c r="C47" s="39">
+        <v>3</v>
+      </c>
+      <c r="D47" s="55">
+        <v>2019</v>
+      </c>
+      <c r="E47" s="49" t="s">
         <v>364</v>
       </c>
-      <c r="AI47" s="54" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="48" spans="1:35" ht="283" customHeight="1">
-      <c r="A48" s="39">
-        <v>40</v>
-      </c>
-      <c r="B48" s="41" t="s">
+      <c r="F47" s="50" t="s">
         <v>365</v>
       </c>
-      <c r="C48" s="39">
-        <v>3</v>
-      </c>
-      <c r="D48" s="56">
+      <c r="G47" s="48">
         <v>2019</v>
       </c>
-      <c r="E48" s="49" t="s">
+      <c r="H47" s="51" t="s">
         <v>366</v>
       </c>
-      <c r="F48" s="50" t="s">
+      <c r="I47" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="J47" s="41" t="s">
         <v>367</v>
       </c>
-      <c r="G48" s="48">
-        <v>2019</v>
-      </c>
-      <c r="H48" s="51" t="s">
+      <c r="K47" s="41" t="s">
         <v>368</v>
       </c>
-      <c r="I48" s="41" t="s">
-        <v>34</v>
-      </c>
-      <c r="J48" s="41" t="s">
+      <c r="L47" s="40" t="s">
         <v>369</v>
       </c>
-      <c r="K48" s="41" t="s">
+      <c r="M47" s="41" t="s">
         <v>370</v>
       </c>
-      <c r="L48" s="40" t="s">
-        <v>371</v>
-      </c>
-      <c r="M48" s="41" t="s">
-        <v>372</v>
-      </c>
-      <c r="N48" s="45">
+      <c r="N47" s="45">
         <v>18</v>
       </c>
-      <c r="O48" s="41" t="s">
-        <v>461</v>
-      </c>
-      <c r="P48" s="41"/>
-      <c r="Q48" s="41"/>
-      <c r="R48" s="41"/>
-      <c r="S48" s="41"/>
-      <c r="T48" s="42"/>
-      <c r="U48" s="40" t="s">
+      <c r="O47" s="41" t="s">
+        <v>449</v>
+      </c>
+      <c r="P47" s="41"/>
+      <c r="Q47" s="41"/>
+      <c r="R47" s="41"/>
+      <c r="S47" s="41"/>
+      <c r="T47" s="42"/>
+      <c r="U47" s="40" t="s">
         <v>314</v>
       </c>
-      <c r="V48" s="42"/>
-      <c r="W48" s="42"/>
-      <c r="X48" s="40"/>
-      <c r="Y48" s="42"/>
-      <c r="Z48" s="42"/>
-      <c r="AA48" s="42"/>
-      <c r="AB48" s="42"/>
-      <c r="AC48" s="42"/>
-      <c r="AD48" s="42"/>
-      <c r="AE48" s="42"/>
-      <c r="AF48" s="42"/>
-      <c r="AG48" s="42"/>
-      <c r="AH48" s="42"/>
-      <c r="AI48" s="1" t="s">
-        <v>741</v>
+      <c r="V47" s="42"/>
+      <c r="W47" s="42"/>
+      <c r="X47" s="40"/>
+      <c r="Y47" s="42"/>
+      <c r="Z47" s="42"/>
+      <c r="AA47" s="42"/>
+      <c r="AB47" s="42"/>
+      <c r="AC47" s="42"/>
+      <c r="AD47" s="42"/>
+      <c r="AE47" s="42"/>
+      <c r="AF47" s="42"/>
+      <c r="AG47" s="42"/>
+      <c r="AH47" s="42"/>
+      <c r="AI47" s="1" t="s">
+        <v>728</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:B48"/>
+  <autoFilter ref="B1:B47"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" display="A Proposed Model-driven Approach to Manage Architectural Technical Debt Life Cycle _x000a_"/>
@@ -11005,7 +10786,6 @@
     <hyperlink ref="O41" r:id="rId6" display="Analyse a set of application from Cast database system tWe analyzed these applications us- ing CAST’s Application Intelligence Platform (AIP),7 which analyzes an en- tire application using more than 1,200 rules to detect violations of good ar- chitectural and coding practice. We drew these rules from software engi- neering literature, repositories such as the Common Weakness Enumeration (CWE; cwe.mitre.org), online discus- sion groups of structural quality prob- lems, and customer experience as re- ported from defect logs and application architects. As an example, security- related violations would include SQL injection, cross-site scripting, buffer overflows, and other violations from the CWE. _x000a_"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
We review the papers and updating latex tables
</commit_message>
<xml_diff>
--- a/dataset/Extraction_form_basic.xlsx
+++ b/dataset/Extraction_form_basic.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Folha 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_3___R._Kazman__Y._Cai__R._Mo__Q._Feng__L._Xiao__S._Haziyev__V._Fedak__and_A._Shapochka._A_case_study_in_locating_the_architectural_roots_of_technical_debt._In_Proc._37th_International_Conference_on_Software__Engineering__May_2015.____8___R._Mo__W._Snip">'Folha 1'!#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Folha 1'!$B$1:$B$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Folha 1'!$AI$1:$AI$47</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1252" uniqueCount="760">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1345" uniqueCount="782">
   <si>
     <t>Paper Id</t>
   </si>
@@ -1548,19 +1548,6 @@
   </si>
   <si>
     <t xml:space="preserve">agile software development, architectural technical debt, effort, multiple case study, qualitative model, sociotechnical phenomena 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In this study we aim at answering the fol- lowing RQs:
-– RQ 1: How do AS help practitioners in identifying ATD?
-– RQ 2: How do practitioners prioritize ATD revealed through AS?
-– RQ 2.1: How is the AS’s negative impact (interest) perceived by the practitioners?
-– RQ 2.2: What is the refactoring cost (principal) of AS perceived by the practitioners?
-By answering RQ1, we aim at understanding if AS are useful to automati- cally identify ATD in industrial projects. Answering RQ2 means answering the combination of RQ2.1 and RQ2.2: understanding what negative impact is gen- erated by the ATD and what cost of refactoring is required. This would help identifying which AS are more critical for the practitioners to prioritize.
-The objectives of the case-study were: 
-automatically identify the AS in the industrial projects (RQ1) 
-evaluate the output in terms of negative impact (RQ2.1) and cost of refac- 
-toring (RQ2.2), to prioritize the ATD. 
 </t>
   </si>
   <si>
@@ -3869,9 +3856,6 @@
     <t>Complete</t>
   </si>
   <si>
-    <t>Incomplete</t>
-  </si>
-  <si>
     <t>Q2(Measure)</t>
   </si>
   <si>
@@ -4031,6 +4015,88 @@
   </si>
   <si>
     <t>Violations of good architectural practices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">we study architecture evolution by identifying the major design decisions that were introduced along a number of the most significant releases (see Section 4). Such design decisions are mainly: (a) architecture components, including their interfaces, such as the kernel, shells, and libraries; (b) architecture connectors such as pipes and C header files; (c) architecture patterns [71] that were applied in the system, such as layering and reflection; and (d) the princi- ples that guide the system architecture, such as modularity and separation of concerns. A quantitative point of view. Specifically we look at how metrics of size and complexity evolve over time; these metrics concern system features (e.g. number of user commands or system calls), as determined by the Unix reference documentation </t>
+  </si>
+  <si>
+    <t>analysis of unix documentation, analysis of repository of unix history, souce code analysis, measure complexity, calculate cyclomatic complexity, component level, Constant Comparison, Another major force that has been driving the software architecture is portability.</t>
+  </si>
+  <si>
+    <t>The architecture technical debt is systematically paid back despite increasing system size and complexity; identified, repayment, monitored</t>
+  </si>
+  <si>
+    <t>Archtecture Social Debt, architecture incommunicability</t>
+  </si>
+  <si>
+    <t>Yes, using a owner formula to calculate the effort to fix the social smell.</t>
+  </si>
+  <si>
+    <t>Not Applicable because it is a framework that creates a graph with socialtechnical network extracted from each architecture decision</t>
+  </si>
+  <si>
+    <t>Security TD</t>
+  </si>
+  <si>
+    <t>Weak</t>
+  </si>
+  <si>
+    <t>Tracking architecture roots, architecutre flaws and Decopling Level for each version analysed by Titan tool</t>
+  </si>
+  <si>
+    <t>Titan, architecture smells, Decopling Level, DRSpace, Propagation Cost, DSM</t>
+  </si>
+  <si>
+    <t>Yes, using a owner formula to calculate the effort to fix the architecture smell</t>
+  </si>
+  <si>
+    <t>Yes; identify, measure, monitoring</t>
+  </si>
+  <si>
+    <t>Strong</t>
+  </si>
+  <si>
+    <t>Validation Research</t>
+  </si>
+  <si>
+    <t>Yes, using a owner formula to calculate the effort to fix the architecture root</t>
+  </si>
+  <si>
+    <t>DRSpace, Architectural Root, Architecture Smell, DSM, DRH, Coupling, latix, source code analysis</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In this study we aim at answering the following RQs:
+– RQ 1: How do AS help practitioners in identifying ATD?
+– RQ 2: How do practitioners prioritize ATD revealed through AS?
+– RQ 2.1: How is the AS’s negative impact (interest) perceived by the practitioners?
+– RQ 2.2: What is the refactoring cost (principal) of AS perceived by the practitioners?
+By answering RQ1, we aim at understanding if AS are useful to automatically identify ATD in industrial projects. Answering RQ2 means answering the combination of RQ2.1 and RQ2.2: understanding what negative impact is generated by the ATD and what cost of refactoring is required. This would help identifying which AS are more critical for the practitioners to prioritize.
+The objectives of the case-study were: 
+automatically identify the AS in the industrial projects (RQ1) 
+evaluate the output in terms of negative impact (RQ2.1) and cost of refac- 
+toring (RQ2.2), to prioritize the ATD. 
+</t>
+  </si>
+  <si>
+    <t>Yes; identify, measure, prioritize, repayment, monitoring</t>
+  </si>
+  <si>
+    <t>Great</t>
+  </si>
+  <si>
+    <t>Yes, using a owner formula to calculate the tim effort to fix the architecture smell</t>
+  </si>
+  <si>
+    <t>Arcan, Architecture Smell</t>
+  </si>
+  <si>
+    <t>Taxonomy of ATD</t>
+  </si>
+  <si>
+    <t>Yes, using quality model to check increasing or decreasing of ATD accumulation</t>
   </si>
 </sst>
 </file>
@@ -4623,7 +4689,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -4750,32 +4816,11 @@
     <xf numFmtId="49" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
@@ -4789,9 +4834,6 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -4800,6 +4842,48 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="85">
@@ -6040,10 +6124,10 @@
   <dimension ref="A1:AI47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="AD2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="AE1" sqref="AE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -6090,7 +6174,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="37" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="E1" s="37" t="s">
         <v>3</v>
@@ -6126,43 +6210,43 @@
         <v>13</v>
       </c>
       <c r="P1" s="37" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="Q1" s="37" t="s">
+        <v>621</v>
+      </c>
+      <c r="R1" s="37" t="s">
+        <v>698</v>
+      </c>
+      <c r="S1" s="37" t="s">
         <v>622</v>
       </c>
-      <c r="R1" s="37" t="s">
+      <c r="T1" s="37" t="s">
         <v>699</v>
       </c>
-      <c r="S1" s="37" t="s">
-        <v>623</v>
-      </c>
-      <c r="T1" s="37" t="s">
+      <c r="U1" s="37" t="s">
         <v>700</v>
       </c>
-      <c r="U1" s="37" t="s">
-        <v>701</v>
-      </c>
       <c r="V1" s="37" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="W1" s="37" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="X1" s="37" t="s">
+        <v>727</v>
+      </c>
+      <c r="Y1" s="37" t="s">
+        <v>728</v>
+      </c>
+      <c r="Z1" s="37" t="s">
         <v>729</v>
       </c>
-      <c r="Y1" s="37" t="s">
+      <c r="AA1" s="37" t="s">
         <v>730</v>
       </c>
-      <c r="Z1" s="37" t="s">
-        <v>731</v>
-      </c>
-      <c r="AA1" s="37" t="s">
-        <v>732</v>
-      </c>
       <c r="AB1" s="37" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="AC1" s="37" t="s">
         <v>14</v>
@@ -6171,10 +6255,10 @@
         <v>15</v>
       </c>
       <c r="AE1" s="37" t="s">
+        <v>696</v>
+      </c>
+      <c r="AF1" s="37" t="s">
         <v>697</v>
-      </c>
-      <c r="AF1" s="37" t="s">
-        <v>698</v>
       </c>
       <c r="AG1" s="37" t="s">
         <v>16</v>
@@ -6183,7 +6267,7 @@
         <v>17</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="2" spans="1:35" ht="160" customHeight="1">
@@ -6209,7 +6293,7 @@
         <v>2019</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>21</v>
@@ -6233,62 +6317,62 @@
         <v>401</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>26</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="V2" s="38" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="W2" s="38" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="X2" s="3" t="s">
+        <v>629</v>
+      </c>
+      <c r="Y2" s="5" t="s">
         <v>630</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="Z2" s="5" t="s">
+        <v>537</v>
+      </c>
+      <c r="AA2" s="5" t="s">
         <v>631</v>
-      </c>
-      <c r="Z2" s="5" t="s">
-        <v>538</v>
-      </c>
-      <c r="AA2" s="5" t="s">
-        <v>632</v>
       </c>
       <c r="AB2" s="5"/>
       <c r="AC2" s="3" t="s">
         <v>27</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="AE2" s="3" t="s">
         <v>28</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="AG2" s="7" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="AH2" s="3" t="s">
         <v>29</v>
       </c>
       <c r="AI2" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="3" spans="1:35" ht="301" customHeight="1">
@@ -6329,62 +6413,62 @@
         <v>36</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="N3" s="10">
         <v>16</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="P3" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="R3" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S3" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T3" s="11" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="U3" s="11" t="s">
         <v>37</v>
       </c>
       <c r="V3" s="11" t="s">
+        <v>623</v>
+      </c>
+      <c r="W3" s="11" t="s">
+        <v>753</v>
+      </c>
+      <c r="X3" s="11" t="s">
         <v>624</v>
       </c>
-      <c r="W3" s="11" t="s">
-        <v>755</v>
-      </c>
-      <c r="X3" s="11" t="s">
+      <c r="Y3" s="11" t="s">
         <v>625</v>
       </c>
-      <c r="Y3" s="11" t="s">
+      <c r="Z3" s="11" t="s">
+        <v>741</v>
+      </c>
+      <c r="AA3" s="9" t="s">
         <v>626</v>
-      </c>
-      <c r="Z3" s="11" t="s">
-        <v>743</v>
-      </c>
-      <c r="AA3" s="9" t="s">
-        <v>627</v>
       </c>
       <c r="AB3" s="9"/>
       <c r="AC3" s="12" t="s">
+        <v>627</v>
+      </c>
+      <c r="AD3" s="12" t="s">
         <v>628</v>
       </c>
-      <c r="AD3" s="12" t="s">
-        <v>629</v>
-      </c>
       <c r="AE3" s="9" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="AF3" s="9" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="AG3" s="9" t="s">
         <v>38</v>
@@ -6393,7 +6477,7 @@
         <v>26</v>
       </c>
       <c r="AI3" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="4" spans="1:35" ht="310" customHeight="1">
@@ -6440,65 +6524,65 @@
         <v>9</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="P4" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="Q4" s="9" t="s">
         <v>26</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="S4" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T4" s="11" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="U4" s="11" t="s">
         <v>46</v>
       </c>
       <c r="V4" s="11" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="W4" s="11" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="X4" s="11" t="s">
+        <v>634</v>
+      </c>
+      <c r="Y4" s="11" t="s">
         <v>635</v>
       </c>
-      <c r="Y4" s="11" t="s">
-        <v>636</v>
-      </c>
       <c r="Z4" s="11" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="AA4" s="11" t="s">
         <v>26</v>
       </c>
       <c r="AB4" s="11"/>
       <c r="AC4" s="13" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="AD4" s="13" t="s">
         <v>47</v>
       </c>
       <c r="AE4" s="11" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="AF4" s="11" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AG4" s="11" t="s">
+        <v>636</v>
+      </c>
+      <c r="AH4" s="11" t="s">
         <v>637</v>
       </c>
-      <c r="AH4" s="11" t="s">
-        <v>638</v>
-      </c>
       <c r="AI4" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="5" spans="1:35" ht="216" customHeight="1">
@@ -6512,7 +6596,7 @@
         <v>400</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>50</v>
@@ -6548,53 +6632,53 @@
         <v>402</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="R5" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S5" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T5" s="11" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="U5" s="9" t="s">
+        <v>639</v>
+      </c>
+      <c r="V5" s="11" t="s">
+        <v>623</v>
+      </c>
+      <c r="W5" s="11" t="s">
+        <v>753</v>
+      </c>
+      <c r="X5" s="9" t="s">
         <v>640</v>
       </c>
-      <c r="V5" s="11" t="s">
-        <v>624</v>
-      </c>
-      <c r="W5" s="11" t="s">
-        <v>755</v>
-      </c>
-      <c r="X5" s="9" t="s">
+      <c r="Y5" s="11" t="s">
         <v>641</v>
       </c>
-      <c r="Y5" s="11" t="s">
+      <c r="Z5" s="9" t="s">
+        <v>539</v>
+      </c>
+      <c r="AA5" s="11" t="s">
         <v>642</v>
-      </c>
-      <c r="Z5" s="9" t="s">
-        <v>540</v>
-      </c>
-      <c r="AA5" s="11" t="s">
-        <v>643</v>
       </c>
       <c r="AB5" s="11"/>
       <c r="AC5" s="11" t="s">
         <v>54</v>
       </c>
       <c r="AD5" s="11" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="AE5" s="11" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="AF5" s="11" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="AG5" s="11" t="s">
         <v>55</v>
@@ -6603,7 +6687,7 @@
         <v>56</v>
       </c>
       <c r="AI5" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="6" spans="1:35" ht="231" customHeight="1">
@@ -6638,7 +6722,7 @@
         <v>61</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="L6" s="11" t="s">
         <v>44</v>
@@ -6653,62 +6737,62 @@
         <v>403</v>
       </c>
       <c r="P6" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="Q6" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="R6" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S6" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T6" s="11" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="U6" s="9" t="s">
         <v>63</v>
       </c>
       <c r="V6" s="11" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="W6" s="11" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="X6" s="9" t="s">
+        <v>644</v>
+      </c>
+      <c r="Y6" s="9" t="s">
+        <v>486</v>
+      </c>
+      <c r="Z6" s="13" t="s">
         <v>645</v>
       </c>
-      <c r="Y6" s="9" t="s">
-        <v>487</v>
-      </c>
-      <c r="Z6" s="13" t="s">
+      <c r="AA6" s="11" t="s">
         <v>646</v>
-      </c>
-      <c r="AA6" s="11" t="s">
-        <v>647</v>
       </c>
       <c r="AB6" s="11"/>
       <c r="AC6" s="13" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="AD6" s="13" t="s">
         <v>250</v>
       </c>
       <c r="AE6" s="13" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AF6" s="13" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="AG6" s="13" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="AH6" s="13" t="s">
         <v>26</v>
       </c>
       <c r="AI6" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="7" spans="1:35" ht="231" customHeight="1">
@@ -6722,7 +6806,7 @@
         <v>49</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>65</v>
@@ -6758,62 +6842,62 @@
         <v>72</v>
       </c>
       <c r="P7" s="11" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="Q7" s="11" t="s">
         <v>26</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="S7" s="11" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T7" s="11" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="U7" s="9" t="s">
         <v>73</v>
       </c>
       <c r="V7" s="11" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="W7" s="11" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="X7" s="9" t="s">
+        <v>648</v>
+      </c>
+      <c r="Y7" s="11" t="s">
         <v>649</v>
       </c>
-      <c r="Y7" s="11" t="s">
+      <c r="Z7" s="9" t="s">
+        <v>559</v>
+      </c>
+      <c r="AA7" s="11" t="s">
         <v>650</v>
-      </c>
-      <c r="Z7" s="9" t="s">
-        <v>560</v>
-      </c>
-      <c r="AA7" s="11" t="s">
-        <v>651</v>
       </c>
       <c r="AB7" s="11"/>
       <c r="AC7" s="13" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="AD7" s="13" t="s">
+        <v>489</v>
+      </c>
+      <c r="AE7" s="13" t="s">
         <v>490</v>
       </c>
-      <c r="AE7" s="13" t="s">
-        <v>491</v>
-      </c>
       <c r="AF7" s="13" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="AG7" s="13" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="AH7" s="13" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="AI7" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="8" spans="1:35" ht="255" customHeight="1">
@@ -6863,62 +6947,62 @@
         <v>404</v>
       </c>
       <c r="P8" s="11" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="Q8" s="11" t="s">
         <v>26</v>
       </c>
       <c r="R8" s="11" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="S8" s="11" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T8" s="11" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="U8" s="11" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="V8" s="11" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="W8" s="11" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="X8" s="11" t="s">
+        <v>652</v>
+      </c>
+      <c r="Y8" s="11" t="s">
         <v>653</v>
       </c>
-      <c r="Y8" s="11" t="s">
+      <c r="Z8" s="13" t="s">
+        <v>743</v>
+      </c>
+      <c r="AA8" s="11" t="s">
         <v>654</v>
-      </c>
-      <c r="Z8" s="13" t="s">
-        <v>745</v>
-      </c>
-      <c r="AA8" s="11" t="s">
-        <v>655</v>
       </c>
       <c r="AB8" s="11"/>
       <c r="AC8" s="13" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="AD8" s="13" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="AE8" s="13" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AF8" s="13" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="AG8" s="13" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="AH8" s="13" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="AI8" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="9" spans="1:35" ht="226" customHeight="1">
@@ -6959,7 +7043,7 @@
         <v>88</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="N9" s="10">
         <v>10</v>
@@ -6968,28 +7052,28 @@
         <v>89</v>
       </c>
       <c r="P9" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="Q9" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="R9" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S9" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T9" s="11" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="U9" s="9" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="V9" s="11" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="W9" s="11" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="X9" s="9" t="s">
         <v>90</v>
@@ -6998,32 +7082,32 @@
         <v>91</v>
       </c>
       <c r="Z9" s="11" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="AA9" s="11" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="AB9" s="11"/>
       <c r="AC9" s="13" t="s">
+        <v>481</v>
+      </c>
+      <c r="AD9" s="13" t="s">
+        <v>480</v>
+      </c>
+      <c r="AE9" s="13" t="s">
+        <v>478</v>
+      </c>
+      <c r="AF9" s="13" t="s">
+        <v>567</v>
+      </c>
+      <c r="AG9" s="13" t="s">
+        <v>479</v>
+      </c>
+      <c r="AH9" s="13" t="s">
         <v>482</v>
       </c>
-      <c r="AD9" s="13" t="s">
-        <v>481</v>
-      </c>
-      <c r="AE9" s="13" t="s">
-        <v>479</v>
-      </c>
-      <c r="AF9" s="13" t="s">
-        <v>568</v>
-      </c>
-      <c r="AG9" s="13" t="s">
-        <v>480</v>
-      </c>
-      <c r="AH9" s="13" t="s">
-        <v>483</v>
-      </c>
       <c r="AI9" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="10" spans="1:35" ht="409.5" customHeight="1">
@@ -7070,65 +7154,65 @@
         <v>11</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="P10" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="Q10" s="9" t="s">
         <v>26</v>
       </c>
       <c r="R10" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="S10" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T10" s="9" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="U10" s="9" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="V10" s="9" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="W10" s="9" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="X10" s="9" t="s">
+        <v>657</v>
+      </c>
+      <c r="Y10" s="11" t="s">
         <v>658</v>
       </c>
-      <c r="Y10" s="11" t="s">
+      <c r="Z10" s="9" t="s">
+        <v>541</v>
+      </c>
+      <c r="AA10" s="11" t="s">
         <v>659</v>
-      </c>
-      <c r="Z10" s="9" t="s">
-        <v>542</v>
-      </c>
-      <c r="AA10" s="11" t="s">
-        <v>660</v>
       </c>
       <c r="AB10" s="11"/>
       <c r="AC10" s="13" t="s">
+        <v>505</v>
+      </c>
+      <c r="AD10" s="13" t="s">
         <v>506</v>
       </c>
-      <c r="AD10" s="13" t="s">
-        <v>507</v>
-      </c>
       <c r="AE10" s="13" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="AF10" s="13" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="AG10" s="13" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="AH10" s="13" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="AI10" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="11" spans="1:35" ht="175" customHeight="1">
@@ -7190,25 +7274,25 @@
         <v>26</v>
       </c>
       <c r="T11" s="11" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="U11" s="9" t="s">
         <v>108</v>
       </c>
       <c r="V11" s="11" t="s">
+        <v>660</v>
+      </c>
+      <c r="W11" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="X11" s="9" t="s">
         <v>661</v>
       </c>
-      <c r="W11" s="11" t="s">
-        <v>686</v>
-      </c>
-      <c r="X11" s="9" t="s">
-        <v>662</v>
-      </c>
       <c r="Y11" s="11" t="s">
         <v>26</v>
       </c>
       <c r="Z11" s="11" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="AA11" s="11" t="s">
         <v>26</v>
@@ -7224,16 +7308,16 @@
         <v>111</v>
       </c>
       <c r="AF11" s="11" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="AG11" s="11" t="s">
         <v>112</v>
       </c>
       <c r="AH11" s="11" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="AI11" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="12" spans="1:35" ht="171" customHeight="1">
@@ -7253,7 +7337,7 @@
         <v>114</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="G12" s="8">
         <v>2019</v>
@@ -7295,25 +7379,25 @@
         <v>26</v>
       </c>
       <c r="T12" s="11" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="U12" s="11" t="s">
         <v>118</v>
       </c>
       <c r="V12" s="11" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="W12" s="11" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="X12" s="11" t="s">
+        <v>663</v>
+      </c>
+      <c r="Y12" s="11" t="s">
         <v>664</v>
       </c>
-      <c r="Y12" s="11" t="s">
-        <v>665</v>
-      </c>
       <c r="Z12" s="11" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="AA12" s="11" t="s">
         <v>26</v>
@@ -7323,41 +7407,41 @@
         <v>120</v>
       </c>
       <c r="AD12" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="AE12" s="11" t="s">
         <v>121</v>
       </c>
       <c r="AF12" s="11" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="AG12" s="11" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="AH12" s="11" t="s">
         <v>26</v>
       </c>
       <c r="AI12" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
-    <row r="13" spans="1:35" s="43" customFormat="1" ht="291" customHeight="1">
-      <c r="A13" s="39">
+    <row r="13" spans="1:35" s="55" customFormat="1" ht="291" customHeight="1">
+      <c r="A13" s="51">
         <v>16</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="53" t="s">
         <v>122</v>
       </c>
       <c r="C13" s="39">
         <v>14</v>
       </c>
-      <c r="D13" s="39">
+      <c r="D13" s="51">
         <v>2017</v>
       </c>
-      <c r="E13" s="40" t="s">
+      <c r="E13" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="F13" s="41" t="s">
+      <c r="F13" s="52" t="s">
         <v>123</v>
       </c>
       <c r="G13" s="39">
@@ -7376,7 +7460,7 @@
         <v>124</v>
       </c>
       <c r="L13" s="40" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="M13" s="40" t="s">
         <v>406</v>
@@ -7384,42 +7468,60 @@
       <c r="N13" s="39">
         <v>18</v>
       </c>
-      <c r="O13" s="40" t="s">
+      <c r="O13" s="53" t="s">
+        <v>666</v>
+      </c>
+      <c r="P13" s="53" t="s">
+        <v>620</v>
+      </c>
+      <c r="Q13" s="53" t="s">
+        <v>620</v>
+      </c>
+      <c r="R13" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="S13" s="53" t="s">
+        <v>620</v>
+      </c>
+      <c r="T13" s="53" t="s">
+        <v>314</v>
+      </c>
+      <c r="U13" s="53" t="s">
+        <v>734</v>
+      </c>
+      <c r="V13" s="53" t="s">
+        <v>623</v>
+      </c>
+      <c r="W13" s="53" t="s">
+        <v>685</v>
+      </c>
+      <c r="X13" s="53" t="s">
         <v>667</v>
       </c>
-      <c r="P13" s="40"/>
-      <c r="Q13" s="40"/>
-      <c r="R13" s="40"/>
-      <c r="S13" s="40"/>
-      <c r="T13" s="40" t="s">
-        <v>314</v>
-      </c>
-      <c r="U13" s="40" t="s">
-        <v>736</v>
-      </c>
-      <c r="V13" s="40"/>
-      <c r="W13" s="40"/>
-      <c r="X13" s="40" t="s">
+      <c r="Y13" s="53" t="s">
         <v>668</v>
       </c>
-      <c r="Y13" s="40" t="s">
-        <v>669</v>
-      </c>
-      <c r="Z13" s="40" t="s">
-        <v>751</v>
-      </c>
-      <c r="AA13" s="40" t="s">
+      <c r="Z13" s="53" t="s">
+        <v>749</v>
+      </c>
+      <c r="AA13" s="53" t="s">
         <v>125</v>
       </c>
-      <c r="AB13" s="40"/>
-      <c r="AC13" s="42"/>
-      <c r="AD13" s="42"/>
-      <c r="AE13" s="42"/>
-      <c r="AF13" s="42"/>
-      <c r="AG13" s="42"/>
-      <c r="AH13" s="42"/>
-      <c r="AI13" s="43" t="s">
-        <v>728</v>
+      <c r="AB13" s="53" t="s">
+        <v>776</v>
+      </c>
+      <c r="AC13" s="54"/>
+      <c r="AD13" s="54"/>
+      <c r="AE13" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF13" s="54" t="s">
+        <v>777</v>
+      </c>
+      <c r="AG13" s="54"/>
+      <c r="AH13" s="54"/>
+      <c r="AI13" s="55" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="14" spans="1:35" ht="234" customHeight="1">
@@ -7466,31 +7568,31 @@
         <v>3</v>
       </c>
       <c r="O14" s="9" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="P14" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="Q14" s="9" t="s">
         <v>26</v>
       </c>
       <c r="R14" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="S14" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T14" s="11" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="U14" s="9" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="V14" s="11" t="s">
         <v>26</v>
       </c>
       <c r="W14" s="11" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="X14" s="9" t="s">
         <v>26</v>
@@ -7499,7 +7601,7 @@
         <v>26</v>
       </c>
       <c r="Z14" s="11" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="AA14" s="11" t="s">
         <v>26</v>
@@ -7511,13 +7613,13 @@
         <v>135</v>
       </c>
       <c r="AD14" s="24" t="s">
+        <v>669</v>
+      </c>
+      <c r="AE14" s="24" t="s">
         <v>670</v>
       </c>
-      <c r="AE14" s="24" t="s">
+      <c r="AF14" s="24" t="s">
         <v>671</v>
-      </c>
-      <c r="AF14" s="24" t="s">
-        <v>672</v>
       </c>
       <c r="AG14" s="24" t="s">
         <v>136</v>
@@ -7525,8 +7627,8 @@
       <c r="AH14" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="AI14" s="54" t="s">
-        <v>727</v>
+      <c r="AI14" s="47" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="15" spans="1:35" ht="267" customHeight="1">
@@ -7539,7 +7641,7 @@
       <c r="C15" s="19">
         <v>36</v>
       </c>
-      <c r="D15" s="57">
+      <c r="D15" s="49">
         <v>2015</v>
       </c>
       <c r="E15" s="18" t="s">
@@ -7573,65 +7675,65 @@
         <v>10</v>
       </c>
       <c r="O15" s="9" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="P15" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="Q15" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="R15" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S15" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T15" s="11" t="s">
         <v>314</v>
       </c>
       <c r="U15" s="11" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="V15" s="11" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="W15" s="11" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="X15" s="11" t="s">
+        <v>673</v>
+      </c>
+      <c r="Y15" s="11" t="s">
         <v>674</v>
       </c>
-      <c r="Y15" s="11" t="s">
-        <v>675</v>
-      </c>
       <c r="Z15" s="11" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="AA15" s="11" t="s">
         <v>146</v>
       </c>
       <c r="AB15" s="11"/>
       <c r="AC15" s="13" t="s">
+        <v>471</v>
+      </c>
+      <c r="AD15" s="13" t="s">
         <v>472</v>
-      </c>
-      <c r="AD15" s="13" t="s">
-        <v>473</v>
       </c>
       <c r="AE15" s="13" t="s">
         <v>28</v>
       </c>
       <c r="AF15" s="13" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="AG15" s="13" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="AH15" s="13" t="s">
-        <v>470</v>
-      </c>
-      <c r="AI15" s="54" t="s">
-        <v>727</v>
+        <v>469</v>
+      </c>
+      <c r="AI15" s="47" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="16" spans="1:35" ht="224" customHeight="1">
@@ -7678,47 +7780,47 @@
         <v>8</v>
       </c>
       <c r="O16" s="11" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="P16" s="11" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="Q16" s="11" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="R16" s="11" t="s">
         <v>26</v>
       </c>
       <c r="S16" s="11" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T16" s="11" t="s">
         <v>314</v>
       </c>
       <c r="U16" s="11" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="V16" s="11" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="W16" s="11" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="X16" s="11" t="s">
+        <v>676</v>
+      </c>
+      <c r="Y16" s="11" t="s">
         <v>677</v>
       </c>
-      <c r="Y16" s="11" t="s">
+      <c r="Z16" s="11" t="s">
+        <v>546</v>
+      </c>
+      <c r="AA16" s="11" t="s">
         <v>678</v>
-      </c>
-      <c r="Z16" s="11" t="s">
-        <v>547</v>
-      </c>
-      <c r="AA16" s="11" t="s">
-        <v>679</v>
       </c>
       <c r="AB16" s="11"/>
       <c r="AC16" s="13" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="AD16" s="13" t="s">
         <v>228</v>
@@ -7727,16 +7829,16 @@
         <v>377</v>
       </c>
       <c r="AF16" s="13" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="AG16" s="13" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="AH16" s="13" t="s">
         <v>399</v>
       </c>
-      <c r="AI16" s="54" t="s">
-        <v>727</v>
+      <c r="AI16" s="47" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="17" spans="1:35" ht="291" customHeight="1">
@@ -7777,7 +7879,7 @@
         <v>88</v>
       </c>
       <c r="M17" s="9" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="N17" s="8">
         <v>8</v>
@@ -7786,81 +7888,81 @@
         <v>157</v>
       </c>
       <c r="P17" s="11" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="Q17" s="11" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="R17" s="11" t="s">
         <v>26</v>
       </c>
       <c r="S17" s="11" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T17" s="11" t="s">
         <v>314</v>
       </c>
       <c r="U17" s="11" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="V17" s="11" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="W17" s="11" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="X17" s="11" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="Y17" s="11" t="s">
         <v>158</v>
       </c>
       <c r="Z17" s="11" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="AA17" s="11" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="AB17" s="11"/>
       <c r="AC17" s="13" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="AD17" s="13" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="AE17" s="13" t="s">
         <v>377</v>
       </c>
       <c r="AF17" s="13" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="AG17" s="13" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="AH17" s="29" t="s">
-        <v>450</v>
-      </c>
-      <c r="AI17" s="54" t="s">
-        <v>727</v>
+        <v>449</v>
+      </c>
+      <c r="AI17" s="47" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="18" spans="1:35" ht="199" customHeight="1">
-      <c r="A18" s="39">
+      <c r="A18" s="51">
         <v>30</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="53" t="s">
         <v>159</v>
       </c>
       <c r="C18" s="39">
         <v>13</v>
       </c>
-      <c r="D18" s="39">
+      <c r="D18" s="51">
         <v>2018</v>
       </c>
-      <c r="E18" s="40" t="s">
+      <c r="E18" s="53" t="s">
         <v>160</v>
       </c>
-      <c r="F18" s="40" t="s">
+      <c r="F18" s="53" t="s">
         <v>161</v>
       </c>
       <c r="G18" s="39">
@@ -7887,107 +7989,159 @@
       <c r="N18" s="39">
         <v>16</v>
       </c>
-      <c r="O18" s="40" t="s">
-        <v>407</v>
-      </c>
-      <c r="P18" s="40"/>
-      <c r="Q18" s="40"/>
-      <c r="R18" s="40"/>
-      <c r="S18" s="40"/>
-      <c r="T18" s="40" t="s">
+      <c r="O18" s="53" t="s">
+        <v>775</v>
+      </c>
+      <c r="P18" s="53" t="s">
+        <v>620</v>
+      </c>
+      <c r="Q18" s="53" t="s">
+        <v>620</v>
+      </c>
+      <c r="R18" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="S18" s="53" t="s">
+        <v>620</v>
+      </c>
+      <c r="T18" s="53" t="s">
         <v>314</v>
       </c>
-      <c r="U18" s="40" t="s">
-        <v>737</v>
-      </c>
-      <c r="V18" s="40"/>
-      <c r="W18" s="40"/>
-      <c r="X18" s="40"/>
-      <c r="Y18" s="41"/>
-      <c r="Z18" s="40"/>
-      <c r="AA18" s="40"/>
-      <c r="AB18" s="40"/>
-      <c r="AC18" s="42"/>
-      <c r="AD18" s="42"/>
-      <c r="AE18" s="42"/>
-      <c r="AF18" s="42"/>
-      <c r="AG18" s="42"/>
-      <c r="AH18" s="42"/>
+      <c r="U18" s="53" t="s">
+        <v>735</v>
+      </c>
+      <c r="V18" s="53" t="s">
+        <v>623</v>
+      </c>
+      <c r="W18" s="53" t="s">
+        <v>687</v>
+      </c>
+      <c r="X18" s="53" t="s">
+        <v>620</v>
+      </c>
+      <c r="Y18" s="52" t="s">
+        <v>396</v>
+      </c>
+      <c r="Z18" s="53" t="s">
+        <v>779</v>
+      </c>
+      <c r="AA18" s="53" t="s">
+        <v>778</v>
+      </c>
+      <c r="AB18" s="53" t="s">
+        <v>776</v>
+      </c>
+      <c r="AC18" s="54"/>
+      <c r="AD18" s="54"/>
+      <c r="AE18" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF18" s="54" t="s">
+        <v>777</v>
+      </c>
+      <c r="AG18" s="54"/>
+      <c r="AH18" s="54"/>
       <c r="AI18" s="1" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="19" spans="1:35" ht="220" customHeight="1">
-      <c r="A19" s="39">
+      <c r="A19" s="51">
         <v>38</v>
       </c>
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="53" t="s">
         <v>165</v>
       </c>
-      <c r="C19" s="39">
+      <c r="C19" s="51">
         <v>3</v>
       </c>
-      <c r="D19" s="39">
+      <c r="D19" s="51">
         <v>2016</v>
       </c>
-      <c r="E19" s="40" t="s">
+      <c r="E19" s="53" t="s">
         <v>384</v>
       </c>
-      <c r="F19" s="40" t="s">
+      <c r="F19" s="53" t="s">
         <v>166</v>
       </c>
-      <c r="G19" s="39">
+      <c r="G19" s="51">
         <v>2016</v>
       </c>
-      <c r="H19" s="40" t="s">
+      <c r="H19" s="53" t="s">
+        <v>407</v>
+      </c>
+      <c r="I19" s="53" t="s">
+        <v>167</v>
+      </c>
+      <c r="J19" s="53" t="s">
+        <v>168</v>
+      </c>
+      <c r="K19" s="53" t="s">
+        <v>169</v>
+      </c>
+      <c r="L19" s="53" t="s">
+        <v>520</v>
+      </c>
+      <c r="M19" s="53" t="s">
+        <v>170</v>
+      </c>
+      <c r="N19" s="51">
+        <v>4</v>
+      </c>
+      <c r="O19" s="53" t="s">
         <v>408</v>
       </c>
-      <c r="I19" s="40" t="s">
-        <v>167</v>
-      </c>
-      <c r="J19" s="40" t="s">
-        <v>168</v>
-      </c>
-      <c r="K19" s="40" t="s">
-        <v>169</v>
-      </c>
-      <c r="L19" s="40" t="s">
-        <v>521</v>
-      </c>
-      <c r="M19" s="40" t="s">
-        <v>170</v>
-      </c>
-      <c r="N19" s="39">
-        <v>4</v>
-      </c>
-      <c r="O19" s="40" t="s">
-        <v>409</v>
-      </c>
-      <c r="P19" s="40"/>
-      <c r="Q19" s="40"/>
-      <c r="R19" s="40"/>
-      <c r="S19" s="40"/>
-      <c r="T19" s="40" t="s">
-        <v>704</v>
-      </c>
-      <c r="U19" s="40" t="s">
-        <v>738</v>
-      </c>
-      <c r="V19" s="40"/>
-      <c r="W19" s="40"/>
-      <c r="X19" s="40"/>
-      <c r="Y19" s="41"/>
-      <c r="Z19" s="40"/>
-      <c r="AA19" s="40"/>
-      <c r="AB19" s="40"/>
-      <c r="AC19" s="42"/>
-      <c r="AD19" s="42"/>
-      <c r="AE19" s="42"/>
-      <c r="AF19" s="42"/>
-      <c r="AG19" s="42"/>
-      <c r="AH19" s="42"/>
-      <c r="AI19" s="1" t="s">
-        <v>728</v>
+      <c r="P19" s="53" t="s">
+        <v>620</v>
+      </c>
+      <c r="Q19" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="R19" s="53" t="s">
+        <v>620</v>
+      </c>
+      <c r="S19" s="53" t="s">
+        <v>620</v>
+      </c>
+      <c r="T19" s="53" t="s">
+        <v>703</v>
+      </c>
+      <c r="U19" s="53" t="s">
+        <v>736</v>
+      </c>
+      <c r="V19" s="53" t="s">
+        <v>638</v>
+      </c>
+      <c r="W19" s="53" t="s">
+        <v>687</v>
+      </c>
+      <c r="X19" s="53" t="s">
+        <v>640</v>
+      </c>
+      <c r="Y19" s="52" t="s">
+        <v>766</v>
+      </c>
+      <c r="Z19" s="53" t="s">
+        <v>767</v>
+      </c>
+      <c r="AA19" s="53" t="s">
+        <v>768</v>
+      </c>
+      <c r="AB19" s="53" t="s">
+        <v>769</v>
+      </c>
+      <c r="AC19" s="54"/>
+      <c r="AD19" s="54"/>
+      <c r="AE19" s="54" t="s">
+        <v>475</v>
+      </c>
+      <c r="AF19" s="54" t="s">
+        <v>770</v>
+      </c>
+      <c r="AG19" s="54"/>
+      <c r="AH19" s="54"/>
+      <c r="AI19" s="55" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="20" spans="1:35" ht="408" customHeight="1">
@@ -8033,66 +8187,66 @@
       <c r="N20" s="8">
         <v>10</v>
       </c>
-      <c r="O20" s="58" t="s">
-        <v>681</v>
+      <c r="O20" s="50" t="s">
+        <v>680</v>
       </c>
       <c r="P20" s="11" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="Q20" s="11" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="R20" s="11" t="s">
         <v>26</v>
       </c>
       <c r="S20" s="11" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T20" s="11" t="s">
         <v>314</v>
       </c>
       <c r="U20" s="9" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="V20" s="11" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="W20" s="11" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="X20" s="9" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="Y20" s="11" t="s">
         <v>179</v>
       </c>
       <c r="Z20" s="11" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="AA20" s="11" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="AB20" s="11"/>
       <c r="AC20" s="13" t="s">
+        <v>498</v>
+      </c>
+      <c r="AD20" s="13" t="s">
         <v>499</v>
       </c>
-      <c r="AD20" s="13" t="s">
-        <v>500</v>
-      </c>
       <c r="AE20" s="13" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="AF20" s="13" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="AG20" s="13" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="AH20" s="13" t="s">
-        <v>498</v>
-      </c>
-      <c r="AI20" s="54" t="s">
-        <v>727</v>
+        <v>497</v>
+      </c>
+      <c r="AI20" s="47" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="21" spans="1:35" ht="198" customHeight="1">
@@ -8118,7 +8272,7 @@
         <v>2015</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="I21" s="11" t="s">
         <v>21</v>
@@ -8139,31 +8293,31 @@
         <v>8</v>
       </c>
       <c r="O21" s="11" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="P21" s="11" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="Q21" s="11" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="R21" s="11" t="s">
         <v>26</v>
       </c>
       <c r="S21" s="11" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T21" s="11" t="s">
         <v>314</v>
       </c>
       <c r="U21" s="11" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="V21" s="11" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="W21" s="11" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="X21" s="11" t="s">
         <v>26</v>
@@ -8172,32 +8326,32 @@
         <v>26</v>
       </c>
       <c r="Z21" s="13" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="AA21" s="11" t="s">
         <v>26</v>
       </c>
       <c r="AB21" s="11"/>
       <c r="AC21" s="13" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="AD21" s="13" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="AE21" s="13" t="s">
         <v>373</v>
       </c>
       <c r="AF21" s="13" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="AG21" s="13" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="AH21" s="13" t="s">
-        <v>454</v>
-      </c>
-      <c r="AI21" s="54" t="s">
-        <v>727</v>
+        <v>453</v>
+      </c>
+      <c r="AI21" s="47" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="22" spans="1:35" ht="272" customHeight="1">
@@ -8238,46 +8392,46 @@
         <v>144</v>
       </c>
       <c r="M22" s="11" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="N22" s="8">
         <v>8</v>
       </c>
       <c r="O22" s="11" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="P22" s="11" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="Q22" s="11" t="s">
         <v>26</v>
       </c>
       <c r="R22" s="11" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="S22" s="11" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T22" s="13" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="U22" s="13" t="s">
         <v>395</v>
       </c>
       <c r="V22" s="13" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="W22" s="13" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="X22" s="13" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="Y22" s="11" t="s">
         <v>396</v>
       </c>
       <c r="Z22" s="13" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="AA22" s="11" t="s">
         <v>26</v>
@@ -8293,7 +8447,7 @@
         <v>300</v>
       </c>
       <c r="AF22" s="13" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="AG22" s="13" t="s">
         <v>398</v>
@@ -8301,8 +8455,8 @@
       <c r="AH22" s="13" t="s">
         <v>394</v>
       </c>
-      <c r="AI22" s="54" t="s">
-        <v>727</v>
+      <c r="AI22" s="47" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="23" spans="1:35" ht="250" customHeight="1">
@@ -8352,28 +8506,28 @@
         <v>197</v>
       </c>
       <c r="P23" s="11" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="Q23" s="11" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="R23" s="11" t="s">
         <v>26</v>
       </c>
       <c r="S23" s="11" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T23" s="22" t="s">
         <v>314</v>
       </c>
       <c r="U23" s="11" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="V23" s="22" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="W23" s="22" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="X23" s="11" t="s">
         <v>198</v>
@@ -8382,32 +8536,32 @@
         <v>396</v>
       </c>
       <c r="Z23" s="13" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="AA23" s="13" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="AB23" s="13"/>
       <c r="AC23" s="13" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="AD23" s="13" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="AE23" s="13" t="s">
         <v>293</v>
       </c>
       <c r="AF23" s="13" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="AG23" s="13" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="AH23" s="13" t="s">
-        <v>501</v>
-      </c>
-      <c r="AI23" s="54" t="s">
-        <v>727</v>
+        <v>500</v>
+      </c>
+      <c r="AI23" s="47" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="24" spans="1:35" ht="217" customHeight="1">
@@ -8433,7 +8587,7 @@
         <v>2019</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="I24" s="9" t="s">
         <v>21</v>
@@ -8469,16 +8623,16 @@
         <v>26</v>
       </c>
       <c r="T24" s="11" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="U24" s="11" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="V24" s="11" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="W24" s="11" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="X24" s="11" t="s">
         <v>26</v>
@@ -8500,10 +8654,10 @@
         <v>207</v>
       </c>
       <c r="AE24" s="11" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="AF24" s="11" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="AG24" s="11" t="s">
         <v>208</v>
@@ -8511,8 +8665,8 @@
       <c r="AH24" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="AI24" s="54" t="s">
-        <v>727</v>
+      <c r="AI24" s="47" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="25" spans="1:35" ht="231" customHeight="1">
@@ -8559,40 +8713,40 @@
         <v>4</v>
       </c>
       <c r="O25" s="9" t="s">
+        <v>605</v>
+      </c>
+      <c r="P25" s="9" t="s">
+        <v>620</v>
+      </c>
+      <c r="Q25" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="R25" s="9" t="s">
+        <v>620</v>
+      </c>
+      <c r="S25" s="9" t="s">
+        <v>620</v>
+      </c>
+      <c r="T25" s="11" t="s">
+        <v>703</v>
+      </c>
+      <c r="U25" s="11" t="s">
         <v>606</v>
       </c>
-      <c r="P25" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="Q25" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="R25" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="S25" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="T25" s="11" t="s">
-        <v>704</v>
-      </c>
-      <c r="U25" s="11" t="s">
-        <v>607</v>
-      </c>
       <c r="V25" s="11" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="W25" s="11" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="X25" s="11" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="Y25" s="11" t="s">
         <v>26</v>
       </c>
       <c r="Z25" s="9" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="AA25" s="11" t="s">
         <v>26</v>
@@ -8608,7 +8762,7 @@
         <v>377</v>
       </c>
       <c r="AF25" s="11" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="AG25" s="11" t="s">
         <v>218</v>
@@ -8616,8 +8770,8 @@
       <c r="AH25" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="AI25" s="54" t="s">
-        <v>727</v>
+      <c r="AI25" s="47" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="26" spans="1:35" ht="301" customHeight="1">
@@ -8658,37 +8812,37 @@
         <v>24</v>
       </c>
       <c r="M26" s="9" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="N26" s="10">
         <v>8</v>
       </c>
       <c r="O26" s="9" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="P26" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="Q26" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="R26" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S26" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T26" s="11" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="U26" s="11" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="V26" s="11" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="W26" s="11" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="X26" s="11" t="s">
         <v>225</v>
@@ -8697,7 +8851,7 @@
         <v>226</v>
       </c>
       <c r="Z26" s="9" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="AA26" s="11" t="s">
         <v>225</v>
@@ -8713,7 +8867,7 @@
         <v>377</v>
       </c>
       <c r="AF26" s="11" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="AG26" s="11" t="s">
         <v>229</v>
@@ -8721,8 +8875,8 @@
       <c r="AH26" s="11" t="s">
         <v>230</v>
       </c>
-      <c r="AI26" s="54" t="s">
-        <v>727</v>
+      <c r="AI26" s="47" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="27" spans="1:35" ht="223" customHeight="1">
@@ -8769,7 +8923,7 @@
         <v>4</v>
       </c>
       <c r="O27" s="9" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="P27" s="9" t="s">
         <v>26</v>
@@ -8784,16 +8938,16 @@
         <v>26</v>
       </c>
       <c r="T27" s="11" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="U27" s="11" t="s">
         <v>235</v>
       </c>
       <c r="V27" s="11" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="W27" s="11" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="X27" s="11" t="s">
         <v>26</v>
@@ -8802,7 +8956,7 @@
         <v>26</v>
       </c>
       <c r="Z27" s="9" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="AA27" s="11" t="s">
         <v>26</v>
@@ -8818,7 +8972,7 @@
         <v>373</v>
       </c>
       <c r="AF27" s="11" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="AG27" s="11" t="s">
         <v>238</v>
@@ -8826,8 +8980,8 @@
       <c r="AH27" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="AI27" s="54" t="s">
-        <v>727</v>
+      <c r="AI27" s="47" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="28" spans="1:35" ht="187" customHeight="1">
@@ -8853,7 +9007,7 @@
         <v>2016</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="I28" s="9" t="s">
         <v>34</v>
@@ -8868,37 +9022,37 @@
         <v>245</v>
       </c>
       <c r="M28" s="9" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="N28" s="10">
         <v>13</v>
       </c>
       <c r="O28" s="9" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="P28" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="Q28" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="R28" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S28" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T28" s="11" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="U28" s="11" t="s">
         <v>246</v>
       </c>
       <c r="V28" s="11" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="W28" s="11" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="X28" s="11" t="s">
         <v>247</v>
@@ -8907,7 +9061,7 @@
         <v>26</v>
       </c>
       <c r="Z28" s="9" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="AA28" s="11" t="s">
         <v>248</v>
@@ -8923,7 +9077,7 @@
         <v>28</v>
       </c>
       <c r="AF28" s="11" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="AG28" s="11" t="s">
         <v>251</v>
@@ -8931,8 +9085,8 @@
       <c r="AH28" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="AI28" s="54" t="s">
-        <v>727</v>
+      <c r="AI28" s="47" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="29" spans="1:35" ht="195" customHeight="1">
@@ -8979,40 +9133,40 @@
         <v>11</v>
       </c>
       <c r="O29" s="9" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="P29" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="Q29" s="9" t="s">
         <v>26</v>
       </c>
       <c r="R29" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="S29" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T29" s="11" t="s">
         <v>314</v>
       </c>
       <c r="U29" s="11" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="V29" s="11" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="W29" s="11" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="X29" s="11" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="Y29" s="11" t="s">
         <v>261</v>
       </c>
       <c r="Z29" s="9" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="AA29" s="11" t="s">
         <v>26</v>
@@ -9028,7 +9182,7 @@
         <v>28</v>
       </c>
       <c r="AF29" s="11" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="AG29" s="11" t="s">
         <v>264</v>
@@ -9036,8 +9190,8 @@
       <c r="AH29" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="AI29" s="54" t="s">
-        <v>727</v>
+      <c r="AI29" s="47" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="30" spans="1:35" ht="317" customHeight="1">
@@ -9083,20 +9237,20 @@
       <c r="N30" s="10">
         <v>8</v>
       </c>
-      <c r="O30" s="52" t="s">
-        <v>414</v>
+      <c r="O30" s="45" t="s">
+        <v>413</v>
       </c>
       <c r="P30" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="Q30" s="9" t="s">
         <v>26</v>
       </c>
       <c r="R30" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="S30" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T30" s="11" t="s">
         <v>314</v>
@@ -9105,13 +9259,13 @@
         <v>271</v>
       </c>
       <c r="V30" s="11" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="W30" s="11" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="X30" s="11" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="Y30" s="11" t="s">
         <v>26</v>
@@ -9133,7 +9287,7 @@
         <v>28</v>
       </c>
       <c r="AF30" s="13" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="AG30" s="13" t="s">
         <v>393</v>
@@ -9141,81 +9295,103 @@
       <c r="AH30" s="13" t="s">
         <v>390</v>
       </c>
-      <c r="AI30" s="54" t="s">
-        <v>727</v>
+      <c r="AI30" s="47" t="s">
+        <v>726</v>
       </c>
     </row>
-    <row r="31" spans="1:35" ht="238" customHeight="1">
-      <c r="A31" s="39">
+    <row r="31" spans="1:35" s="55" customFormat="1" ht="238" customHeight="1">
+      <c r="A31" s="51">
         <v>63</v>
       </c>
-      <c r="B31" s="41" t="s">
+      <c r="B31" s="52" t="s">
         <v>272</v>
       </c>
       <c r="C31" s="39">
         <v>4</v>
       </c>
-      <c r="D31" s="39">
+      <c r="D31" s="51">
         <v>2019</v>
       </c>
-      <c r="E31" s="41" t="s">
+      <c r="E31" s="52" t="s">
         <v>386</v>
       </c>
-      <c r="F31" s="40" t="s">
+      <c r="F31" s="53" t="s">
         <v>273</v>
       </c>
       <c r="G31" s="39">
         <v>2019</v>
       </c>
-      <c r="H31" s="51" t="s">
+      <c r="H31" s="44" t="s">
         <v>274</v>
       </c>
-      <c r="I31" s="53" t="s">
+      <c r="I31" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="J31" s="53" t="s">
+      <c r="J31" s="46" t="s">
         <v>275</v>
       </c>
-      <c r="K31" s="53" t="s">
+      <c r="K31" s="46" t="s">
         <v>275</v>
       </c>
       <c r="L31" s="40" t="s">
         <v>88</v>
       </c>
       <c r="M31" s="41" t="s">
+        <v>419</v>
+      </c>
+      <c r="N31" s="42">
+        <v>31</v>
+      </c>
+      <c r="O31" s="52" t="s">
         <v>420</v>
       </c>
-      <c r="N31" s="45">
-        <v>31</v>
-      </c>
-      <c r="O31" s="41" t="s">
-        <v>421</v>
-      </c>
-      <c r="P31" s="41"/>
-      <c r="Q31" s="41"/>
-      <c r="R31" s="41"/>
-      <c r="S31" s="41"/>
-      <c r="T31" s="40" t="s">
-        <v>609</v>
-      </c>
-      <c r="U31" s="40" t="s">
+      <c r="P31" s="52" t="s">
+        <v>620</v>
+      </c>
+      <c r="Q31" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="R31" s="52" t="s">
+        <v>620</v>
+      </c>
+      <c r="S31" s="52" t="s">
+        <v>620</v>
+      </c>
+      <c r="T31" s="53" t="s">
+        <v>314</v>
+      </c>
+      <c r="U31" s="53" t="s">
         <v>276</v>
       </c>
-      <c r="V31" s="40"/>
-      <c r="W31" s="40"/>
-      <c r="X31" s="40"/>
-      <c r="Y31" s="40"/>
-      <c r="Z31" s="42"/>
-      <c r="AA31" s="42"/>
-      <c r="AB31" s="42"/>
-      <c r="AC31" s="42"/>
-      <c r="AD31" s="42"/>
-      <c r="AE31" s="42"/>
-      <c r="AF31" s="42"/>
-      <c r="AG31" s="42"/>
-      <c r="AH31" s="42"/>
-      <c r="AI31" s="1" t="s">
-        <v>728</v>
+      <c r="V31" s="53" t="s">
+        <v>638</v>
+      </c>
+      <c r="W31" s="53" t="s">
+        <v>754</v>
+      </c>
+      <c r="X31" s="53" t="s">
+        <v>758</v>
+      </c>
+      <c r="Y31" s="53" t="s">
+        <v>396</v>
+      </c>
+      <c r="Z31" s="54" t="s">
+        <v>759</v>
+      </c>
+      <c r="AA31" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB31" s="54" t="s">
+        <v>760</v>
+      </c>
+      <c r="AC31" s="54"/>
+      <c r="AD31" s="54"/>
+      <c r="AE31" s="54"/>
+      <c r="AF31" s="54"/>
+      <c r="AG31" s="54"/>
+      <c r="AH31" s="54"/>
+      <c r="AI31" s="55" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="32" spans="1:35" ht="226" customHeight="1">
@@ -9232,7 +9408,7 @@
         <v>2018</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F32" s="11" t="s">
         <v>278</v>
@@ -9247,22 +9423,22 @@
         <v>21</v>
       </c>
       <c r="J32" s="26" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="K32" s="26" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="L32" s="11" t="s">
         <v>24</v>
       </c>
       <c r="M32" s="9" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="N32" s="10">
         <v>5</v>
       </c>
       <c r="O32" s="9" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="P32" s="9" t="s">
         <v>26</v>
@@ -9277,16 +9453,16 @@
         <v>26</v>
       </c>
       <c r="T32" s="11" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="U32" s="11" t="s">
         <v>280</v>
       </c>
       <c r="V32" s="11" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="W32" s="11" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="X32" s="11" t="s">
         <v>281</v>
@@ -9295,10 +9471,10 @@
         <v>26</v>
       </c>
       <c r="Z32" s="9" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="AA32" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="AB32" s="11"/>
       <c r="AC32" s="11" t="s">
@@ -9311,7 +9487,7 @@
         <v>284</v>
       </c>
       <c r="AF32" s="11" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="AG32" s="11" t="s">
         <v>285</v>
@@ -9319,8 +9495,8 @@
       <c r="AH32" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="AI32" s="54" t="s">
-        <v>727</v>
+      <c r="AI32" s="47" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="33" spans="1:35" ht="274" customHeight="1">
@@ -9337,7 +9513,7 @@
         <v>2017</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F33" s="27" t="s">
         <v>287</v>
@@ -9352,10 +9528,10 @@
         <v>21</v>
       </c>
       <c r="J33" s="26" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="K33" s="26" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="L33" s="11" t="s">
         <v>259</v>
@@ -9366,20 +9542,20 @@
       <c r="N33" s="10">
         <v>11</v>
       </c>
-      <c r="O33" s="52" t="s">
-        <v>429</v>
+      <c r="O33" s="45" t="s">
+        <v>428</v>
       </c>
       <c r="P33" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="Q33" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="R33" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S33" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T33" s="11" t="s">
         <v>290</v>
@@ -9388,10 +9564,10 @@
         <v>290</v>
       </c>
       <c r="V33" s="11" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="W33" s="11" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="X33" s="11" t="s">
         <v>26</v>
@@ -9416,16 +9592,16 @@
         <v>293</v>
       </c>
       <c r="AF33" s="11" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="AG33" s="11" t="s">
         <v>294</v>
       </c>
       <c r="AH33" s="11" t="s">
-        <v>616</v>
-      </c>
-      <c r="AI33" s="54" t="s">
-        <v>727</v>
+        <v>615</v>
+      </c>
+      <c r="AI33" s="47" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="34" spans="1:35" ht="235" customHeight="1">
@@ -9457,46 +9633,46 @@
         <v>167</v>
       </c>
       <c r="J34" s="26" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="K34" s="26" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="L34" s="11" t="s">
         <v>24</v>
       </c>
       <c r="M34" s="9" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="N34" s="10">
         <v>8</v>
       </c>
       <c r="O34" s="9" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="P34" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="Q34" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="R34" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S34" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T34" s="11" t="s">
         <v>314</v>
       </c>
       <c r="U34" s="11" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="V34" s="11" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="W34" s="11" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="X34" s="11" t="s">
         <v>26</v>
@@ -9505,7 +9681,7 @@
         <v>26</v>
       </c>
       <c r="Z34" s="11" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="AA34" s="11" t="s">
         <v>26</v>
@@ -9521,7 +9697,7 @@
         <v>300</v>
       </c>
       <c r="AF34" s="11" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="AG34" s="11" t="s">
         <v>301</v>
@@ -9529,8 +9705,8 @@
       <c r="AH34" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="AI34" s="54" t="s">
-        <v>727</v>
+      <c r="AI34" s="47" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="35" spans="1:35" ht="270" customHeight="1">
@@ -9547,7 +9723,7 @@
         <v>2016</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F35" s="28" t="s">
         <v>303</v>
@@ -9556,7 +9732,7 @@
         <v>2016</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="I35" s="26" t="s">
         <v>21</v>
@@ -9577,31 +9753,31 @@
         <v>8</v>
       </c>
       <c r="O35" s="9" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="P35" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="Q35" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="R35" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S35" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T35" s="11" t="s">
         <v>314</v>
       </c>
       <c r="U35" s="11" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="V35" s="11" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="W35" s="11" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="X35" s="11" t="s">
         <v>26</v>
@@ -9626,7 +9802,7 @@
         <v>293</v>
       </c>
       <c r="AF35" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="AG35" s="13" t="s">
         <v>381</v>
@@ -9634,8 +9810,8 @@
       <c r="AH35" s="13" t="s">
         <v>383</v>
       </c>
-      <c r="AI35" s="54" t="s">
-        <v>727</v>
+      <c r="AI35" s="47" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="36" spans="1:35" ht="202" customHeight="1">
@@ -9652,7 +9828,7 @@
         <v>2017</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="F36" s="28" t="s">
         <v>307</v>
@@ -9685,28 +9861,28 @@
         <v>313</v>
       </c>
       <c r="P36" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="Q36" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="R36" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S36" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T36" s="11" t="s">
         <v>314</v>
       </c>
       <c r="U36" s="11" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="V36" s="11" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="W36" s="11" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="X36" s="11" t="s">
         <v>26</v>
@@ -9722,51 +9898,51 @@
       </c>
       <c r="AB36" s="11"/>
       <c r="AC36" s="13" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="AD36" s="13" t="s">
+        <v>493</v>
+      </c>
+      <c r="AE36" s="13" t="s">
+        <v>495</v>
+      </c>
+      <c r="AF36" s="13" t="s">
+        <v>587</v>
+      </c>
+      <c r="AG36" s="13" t="s">
         <v>494</v>
       </c>
-      <c r="AE36" s="13" t="s">
-        <v>496</v>
-      </c>
-      <c r="AF36" s="13" t="s">
-        <v>588</v>
-      </c>
-      <c r="AG36" s="13" t="s">
-        <v>495</v>
-      </c>
       <c r="AH36" s="30" t="s">
-        <v>493</v>
-      </c>
-      <c r="AI36" s="54" t="s">
-        <v>727</v>
+        <v>492</v>
+      </c>
+      <c r="AI36" s="47" t="s">
+        <v>726</v>
       </c>
     </row>
-    <row r="37" spans="1:35" ht="225" customHeight="1">
-      <c r="A37" s="39">
+    <row r="37" spans="1:35" s="55" customFormat="1" ht="225" customHeight="1">
+      <c r="A37" s="51">
         <v>35</v>
       </c>
-      <c r="B37" s="41" t="s">
+      <c r="B37" s="52" t="s">
         <v>315</v>
       </c>
       <c r="C37" s="39">
         <v>65</v>
       </c>
-      <c r="D37" s="39">
+      <c r="D37" s="51">
         <v>2015</v>
       </c>
-      <c r="E37" s="41" t="s">
-        <v>415</v>
-      </c>
-      <c r="F37" s="41" t="s">
+      <c r="E37" s="52" t="s">
+        <v>414</v>
+      </c>
+      <c r="F37" s="52" t="s">
         <v>316</v>
       </c>
       <c r="G37" s="8">
         <v>2015</v>
       </c>
       <c r="H37" s="9" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I37" s="26" t="s">
         <v>34</v>
@@ -9781,118 +9957,162 @@
         <v>311</v>
       </c>
       <c r="M37" s="9" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="N37" s="10">
         <v>17</v>
       </c>
-      <c r="O37" s="41" t="s">
-        <v>537</v>
-      </c>
-      <c r="P37" s="41" t="s">
-        <v>621</v>
-      </c>
-      <c r="Q37" s="41" t="s">
-        <v>621</v>
-      </c>
-      <c r="R37" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="S37" s="41" t="s">
-        <v>621</v>
-      </c>
-      <c r="T37" s="40" t="s">
+      <c r="O37" s="52" t="s">
+        <v>536</v>
+      </c>
+      <c r="P37" s="52" t="s">
+        <v>620</v>
+      </c>
+      <c r="Q37" s="52" t="s">
+        <v>620</v>
+      </c>
+      <c r="R37" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="S37" s="52" t="s">
+        <v>620</v>
+      </c>
+      <c r="T37" s="53" t="s">
         <v>314</v>
       </c>
-      <c r="U37" s="40" t="s">
-        <v>723</v>
-      </c>
-      <c r="V37" s="40" t="s">
-        <v>624</v>
-      </c>
-      <c r="W37" s="40"/>
-      <c r="X37" s="40"/>
-      <c r="Y37" s="42"/>
-      <c r="Z37" s="42"/>
-      <c r="AA37" s="42"/>
-      <c r="AB37" s="42"/>
-      <c r="AC37" s="42"/>
-      <c r="AD37" s="42"/>
-      <c r="AE37" s="42"/>
-      <c r="AF37" s="42"/>
-      <c r="AG37" s="42"/>
-      <c r="AH37" s="42"/>
-      <c r="AI37" s="1" t="s">
-        <v>728</v>
+      <c r="U37" s="53" t="s">
+        <v>722</v>
+      </c>
+      <c r="V37" s="53" t="s">
+        <v>623</v>
+      </c>
+      <c r="W37" s="53" t="s">
+        <v>685</v>
+      </c>
+      <c r="X37" s="53" t="s">
+        <v>620</v>
+      </c>
+      <c r="Y37" s="54" t="s">
+        <v>620</v>
+      </c>
+      <c r="Z37" s="54" t="s">
+        <v>780</v>
+      </c>
+      <c r="AA37" s="54" t="s">
+        <v>781</v>
+      </c>
+      <c r="AB37" s="54" t="s">
+        <v>769</v>
+      </c>
+      <c r="AC37" s="54"/>
+      <c r="AD37" s="54"/>
+      <c r="AE37" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF37" s="54" t="s">
+        <v>774</v>
+      </c>
+      <c r="AG37" s="54"/>
+      <c r="AH37" s="54"/>
+      <c r="AI37" s="55" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="38" spans="1:35" ht="270" customHeight="1">
-      <c r="A38" s="39">
+      <c r="A38" s="51">
         <v>24</v>
       </c>
-      <c r="B38" s="41" t="s">
+      <c r="B38" s="52" t="s">
         <v>318</v>
       </c>
-      <c r="C38" s="39">
+      <c r="C38" s="51">
         <v>15</v>
       </c>
-      <c r="D38" s="39">
+      <c r="D38" s="51">
         <v>2018</v>
       </c>
-      <c r="E38" s="41" t="s">
+      <c r="E38" s="52" t="s">
+        <v>433</v>
+      </c>
+      <c r="F38" s="52" t="s">
+        <v>319</v>
+      </c>
+      <c r="G38" s="51">
+        <v>2018</v>
+      </c>
+      <c r="H38" s="52" t="s">
+        <v>616</v>
+      </c>
+      <c r="I38" s="59" t="s">
+        <v>21</v>
+      </c>
+      <c r="J38" s="59" t="s">
+        <v>320</v>
+      </c>
+      <c r="K38" s="59" t="s">
+        <v>321</v>
+      </c>
+      <c r="L38" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="M38" s="52" t="s">
         <v>434</v>
       </c>
-      <c r="F38" s="41" t="s">
-        <v>319</v>
-      </c>
-      <c r="G38" s="39">
-        <v>2018</v>
-      </c>
-      <c r="H38" s="41" t="s">
-        <v>617</v>
-      </c>
-      <c r="I38" s="44" t="s">
-        <v>21</v>
-      </c>
-      <c r="J38" s="44" t="s">
-        <v>320</v>
-      </c>
-      <c r="K38" s="44" t="s">
-        <v>321</v>
-      </c>
-      <c r="L38" s="40" t="s">
-        <v>88</v>
-      </c>
-      <c r="M38" s="41" t="s">
-        <v>435</v>
-      </c>
-      <c r="N38" s="45">
+      <c r="N38" s="60">
         <v>27</v>
       </c>
-      <c r="O38" s="41" t="s">
-        <v>611</v>
-      </c>
-      <c r="P38" s="41"/>
-      <c r="Q38" s="41"/>
-      <c r="R38" s="41"/>
-      <c r="S38" s="41"/>
-      <c r="T38" s="40"/>
-      <c r="U38" s="42"/>
-      <c r="V38" s="40"/>
-      <c r="W38" s="40"/>
-      <c r="X38" s="42"/>
-      <c r="Y38" s="42"/>
-      <c r="Z38" s="42"/>
-      <c r="AA38" s="42"/>
-      <c r="AB38" s="42"/>
-      <c r="AC38" s="42"/>
-      <c r="AD38" s="42"/>
-      <c r="AE38" s="42"/>
-      <c r="AF38" s="42"/>
-      <c r="AG38" s="42"/>
-      <c r="AH38" s="42"/>
+      <c r="O38" s="52" t="s">
+        <v>610</v>
+      </c>
+      <c r="P38" s="52" t="s">
+        <v>620</v>
+      </c>
+      <c r="Q38" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="R38" s="52" t="s">
+        <v>620</v>
+      </c>
+      <c r="S38" s="52" t="s">
+        <v>620</v>
+      </c>
+      <c r="T38" s="53" t="s">
+        <v>702</v>
+      </c>
+      <c r="U38" s="54"/>
+      <c r="V38" s="53" t="s">
+        <v>771</v>
+      </c>
+      <c r="W38" s="53" t="s">
+        <v>687</v>
+      </c>
+      <c r="X38" s="54" t="s">
+        <v>640</v>
+      </c>
+      <c r="Y38" s="54" t="s">
+        <v>396</v>
+      </c>
+      <c r="Z38" s="54" t="s">
+        <v>773</v>
+      </c>
+      <c r="AA38" s="54" t="s">
+        <v>772</v>
+      </c>
+      <c r="AB38" s="54" t="s">
+        <v>620</v>
+      </c>
+      <c r="AC38" s="54"/>
+      <c r="AD38" s="54"/>
+      <c r="AE38" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF38" s="54" t="s">
+        <v>579</v>
+      </c>
+      <c r="AG38" s="54"/>
+      <c r="AH38" s="54"/>
       <c r="AI38" s="1" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="39" spans="1:35" ht="243" customHeight="1">
@@ -9918,7 +10138,7 @@
         <v>2019</v>
       </c>
       <c r="H39" s="9" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="I39" s="9" t="s">
         <v>21</v>
@@ -9933,37 +10153,37 @@
         <v>259</v>
       </c>
       <c r="M39" s="9" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N39" s="10">
         <v>11</v>
       </c>
       <c r="O39" s="9" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="P39" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="Q39" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="R39" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S39" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T39" s="11" t="s">
         <v>290</v>
       </c>
       <c r="U39" s="13" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="V39" s="11" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="W39" s="11" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="X39" s="13" t="s">
         <v>26</v>
@@ -9979,25 +10199,25 @@
       </c>
       <c r="AB39" s="13"/>
       <c r="AC39" s="13" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="AD39" s="13" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="AE39" s="13" t="s">
         <v>373</v>
       </c>
       <c r="AF39" s="13" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="AG39" s="13" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="AH39" s="13" t="s">
-        <v>508</v>
-      </c>
-      <c r="AI39" s="54" t="s">
-        <v>727</v>
+        <v>507</v>
+      </c>
+      <c r="AI39" s="47" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="40" spans="1:35" ht="220" customHeight="1">
@@ -10017,7 +10237,7 @@
         <v>328</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G40" s="8">
         <v>2017</v>
@@ -10029,22 +10249,22 @@
         <v>21</v>
       </c>
       <c r="J40" s="9" t="s">
+        <v>438</v>
+      </c>
+      <c r="K40" s="9" t="s">
         <v>439</v>
-      </c>
-      <c r="K40" s="9" t="s">
-        <v>440</v>
       </c>
       <c r="L40" s="11" t="s">
         <v>88</v>
       </c>
       <c r="M40" s="9" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="N40" s="10">
         <v>5</v>
       </c>
       <c r="O40" s="9" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="P40" s="9" t="s">
         <v>26</v>
@@ -10059,16 +10279,16 @@
         <v>26</v>
       </c>
       <c r="T40" s="11" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="U40" s="11" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="V40" s="11" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="W40" s="11" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="X40" s="13" t="s">
         <v>26</v>
@@ -10077,7 +10297,7 @@
         <v>26</v>
       </c>
       <c r="Z40" s="13" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="AA40" s="13" t="s">
         <v>26</v>
@@ -10093,7 +10313,7 @@
         <v>373</v>
       </c>
       <c r="AF40" s="13" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="AG40" s="13" t="s">
         <v>371</v>
@@ -10101,8 +10321,8 @@
       <c r="AH40" s="13" t="s">
         <v>372</v>
       </c>
-      <c r="AI40" s="54" t="s">
-        <v>727</v>
+      <c r="AI40" s="47" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="41" spans="1:35" ht="227" customHeight="1">
@@ -10128,7 +10348,7 @@
         <v>2012</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="I41" s="9" t="s">
         <v>34</v>
@@ -10149,138 +10369,164 @@
         <v>9</v>
       </c>
       <c r="O41" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="P41" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="Q41" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="R41" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S41" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T41" s="11" t="s">
         <v>314</v>
       </c>
       <c r="U41" s="11" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="V41" s="11" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="W41" s="11" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="X41" s="11" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="Y41" s="13" t="s">
         <v>26</v>
       </c>
       <c r="Z41" s="13" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="AA41" s="13" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="AB41" s="13"/>
       <c r="AC41" s="13" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="AD41" s="13" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="AE41" s="13" t="s">
         <v>373</v>
       </c>
       <c r="AF41" s="13" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="AG41" s="13" t="s">
+        <v>461</v>
+      </c>
+      <c r="AH41" s="13" t="s">
         <v>462</v>
       </c>
-      <c r="AH41" s="13" t="s">
-        <v>463</v>
-      </c>
-      <c r="AI41" s="54" t="s">
-        <v>727</v>
+      <c r="AI41" s="47" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="42" spans="1:35" ht="205" customHeight="1">
-      <c r="A42" s="39">
+      <c r="A42" s="51">
         <v>85</v>
       </c>
-      <c r="B42" s="41" t="s">
+      <c r="B42" s="52" t="s">
         <v>334</v>
       </c>
       <c r="C42" s="39">
         <v>1</v>
       </c>
-      <c r="D42" s="55">
+      <c r="D42" s="56">
         <v>2018</v>
       </c>
-      <c r="E42" s="46" t="s">
+      <c r="E42" s="57" t="s">
         <v>335</v>
       </c>
-      <c r="F42" s="47" t="s">
+      <c r="F42" s="58" t="s">
         <v>336</v>
       </c>
-      <c r="G42" s="48">
+      <c r="G42" s="43">
         <v>2018</v>
       </c>
       <c r="H42" s="41" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="I42" s="41" t="s">
         <v>337</v>
       </c>
       <c r="J42" s="41" t="s">
+        <v>442</v>
+      </c>
+      <c r="K42" s="41" t="s">
         <v>443</v>
-      </c>
-      <c r="K42" s="41" t="s">
-        <v>444</v>
       </c>
       <c r="L42" s="40" t="s">
         <v>338</v>
       </c>
       <c r="M42" s="41" t="s">
-        <v>530</v>
-      </c>
-      <c r="N42" s="45">
+        <v>529</v>
+      </c>
+      <c r="N42" s="42">
         <v>13</v>
       </c>
-      <c r="O42" s="41" t="s">
-        <v>445</v>
-      </c>
-      <c r="P42" s="41"/>
-      <c r="Q42" s="41"/>
-      <c r="R42" s="41"/>
-      <c r="S42" s="41"/>
-      <c r="T42" s="40" t="s">
+      <c r="O42" s="52" t="s">
+        <v>444</v>
+      </c>
+      <c r="P42" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q42" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="R42" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="S42" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="T42" s="53" t="s">
         <v>314</v>
       </c>
-      <c r="U42" s="40" t="s">
+      <c r="U42" s="53" t="s">
         <v>314</v>
       </c>
-      <c r="V42" s="40"/>
-      <c r="W42" s="40"/>
-      <c r="X42" s="40"/>
-      <c r="Y42" s="42"/>
-      <c r="Z42" s="42"/>
-      <c r="AA42" s="42"/>
-      <c r="AB42" s="42"/>
-      <c r="AC42" s="42"/>
-      <c r="AD42" s="42"/>
-      <c r="AE42" s="42"/>
-      <c r="AF42" s="42"/>
-      <c r="AG42" s="42"/>
-      <c r="AH42" s="42"/>
+      <c r="V42" s="53" t="s">
+        <v>660</v>
+      </c>
+      <c r="W42" s="53" t="s">
+        <v>755</v>
+      </c>
+      <c r="X42" s="53" t="s">
+        <v>764</v>
+      </c>
+      <c r="Y42" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z42" s="54" t="s">
+        <v>292</v>
+      </c>
+      <c r="AA42" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB42" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC42" s="54"/>
+      <c r="AD42" s="54"/>
+      <c r="AE42" s="54" t="s">
+        <v>284</v>
+      </c>
+      <c r="AF42" s="54" t="s">
+        <v>765</v>
+      </c>
+      <c r="AG42" s="54"/>
+      <c r="AH42" s="54"/>
       <c r="AI42" s="1" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="43" spans="1:35" ht="276" customHeight="1">
@@ -10293,7 +10539,7 @@
       <c r="C43" s="8">
         <v>2</v>
       </c>
-      <c r="D43" s="56">
+      <c r="D43" s="48">
         <v>2019</v>
       </c>
       <c r="E43" s="36" t="s">
@@ -10306,7 +10552,7 @@
         <v>2019</v>
       </c>
       <c r="H43" s="9" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I43" s="9" t="s">
         <v>21</v>
@@ -10327,40 +10573,40 @@
         <v>5</v>
       </c>
       <c r="O43" s="9" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="P43" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="Q43" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="R43" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S43" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T43" s="11" t="s">
         <v>314</v>
       </c>
       <c r="U43" s="11" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="V43" s="11" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="W43" s="11" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="X43" s="11" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="Y43" s="11" t="s">
         <v>26</v>
       </c>
       <c r="Z43" s="9" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="AA43" s="11" t="s">
         <v>26</v>
@@ -10376,7 +10622,7 @@
         <v>377</v>
       </c>
       <c r="AF43" s="13" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="AG43" s="13" t="s">
         <v>378</v>
@@ -10384,8 +10630,8 @@
       <c r="AH43" s="13" t="s">
         <v>379</v>
       </c>
-      <c r="AI43" s="54" t="s">
-        <v>727</v>
+      <c r="AI43" s="47" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="44" spans="1:35" ht="231" customHeight="1">
@@ -10398,7 +10644,7 @@
       <c r="C44" s="8">
         <v>6</v>
       </c>
-      <c r="D44" s="56">
+      <c r="D44" s="48">
         <v>2019</v>
       </c>
       <c r="E44" s="36" t="s">
@@ -10420,7 +10666,7 @@
         <v>347</v>
       </c>
       <c r="K44" s="9" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="L44" s="11" t="s">
         <v>88</v>
@@ -10432,31 +10678,31 @@
         <v>10</v>
       </c>
       <c r="O44" s="9" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="P44" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="Q44" s="9" t="s">
         <v>26</v>
       </c>
       <c r="R44" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="S44" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T44" s="11" t="s">
         <v>314</v>
       </c>
       <c r="U44" s="11" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="V44" s="11" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="W44" s="11" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="X44" s="11" t="s">
         <v>26</v>
@@ -10465,32 +10711,32 @@
         <v>26</v>
       </c>
       <c r="Z44" s="13" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="AA44" s="11" t="s">
         <v>26</v>
       </c>
       <c r="AB44" s="11"/>
       <c r="AC44" s="13" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD44" s="13" t="s">
+        <v>477</v>
+      </c>
+      <c r="AE44" s="13" t="s">
         <v>475</v>
       </c>
-      <c r="AD44" s="13" t="s">
-        <v>478</v>
-      </c>
-      <c r="AE44" s="13" t="s">
+      <c r="AF44" s="13" t="s">
+        <v>592</v>
+      </c>
+      <c r="AG44" s="13" t="s">
         <v>476</v>
       </c>
-      <c r="AF44" s="13" t="s">
-        <v>593</v>
-      </c>
-      <c r="AG44" s="13" t="s">
-        <v>477</v>
-      </c>
       <c r="AH44" s="13" t="s">
-        <v>474</v>
-      </c>
-      <c r="AI44" s="54" t="s">
-        <v>727</v>
+        <v>473</v>
+      </c>
+      <c r="AI44" s="47" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="45" spans="1:35" ht="268" customHeight="1">
@@ -10503,14 +10749,14 @@
       <c r="C45" s="8">
         <v>10</v>
       </c>
-      <c r="D45" s="56">
+      <c r="D45" s="48">
         <v>2018</v>
       </c>
       <c r="E45" s="36" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="F45" s="33" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="G45" s="21">
         <v>2018</v>
@@ -10522,10 +10768,10 @@
         <v>21</v>
       </c>
       <c r="J45" s="9" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="K45" s="9" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="L45" s="11" t="s">
         <v>24</v>
@@ -10537,65 +10783,65 @@
         <v>9</v>
       </c>
       <c r="O45" s="9" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="P45" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="Q45" s="9" t="s">
         <v>26</v>
       </c>
       <c r="R45" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="S45" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T45" s="11" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="U45" s="11" t="s">
         <v>290</v>
       </c>
       <c r="V45" s="11" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="W45" s="11" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="X45" s="11" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="Y45" s="11" t="s">
         <v>26</v>
       </c>
       <c r="Z45" s="9" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="AA45" s="13" t="s">
         <v>26</v>
       </c>
       <c r="AB45" s="13"/>
       <c r="AC45" s="13" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="AD45" s="13" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AE45" s="13" t="s">
         <v>373</v>
       </c>
       <c r="AF45" s="13" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="AG45" s="13" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="AH45" s="13" t="s">
-        <v>465</v>
-      </c>
-      <c r="AI45" s="54" t="s">
-        <v>727</v>
+        <v>464</v>
+      </c>
+      <c r="AI45" s="47" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="46" spans="1:35" ht="159" customHeight="1">
@@ -10608,7 +10854,7 @@
       <c r="C46" s="8">
         <v>0</v>
       </c>
-      <c r="D46" s="56">
+      <c r="D46" s="48">
         <v>2017</v>
       </c>
       <c r="E46" s="36" t="s">
@@ -10642,7 +10888,7 @@
         <v>4</v>
       </c>
       <c r="O46" s="9" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="P46" s="9" t="s">
         <v>26</v>
@@ -10657,16 +10903,16 @@
         <v>26</v>
       </c>
       <c r="T46" s="11" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="U46" s="11" t="s">
         <v>359</v>
       </c>
       <c r="V46" s="11" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="W46" s="11" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="X46" s="11" t="s">
         <v>26</v>
@@ -10682,16 +10928,16 @@
       </c>
       <c r="AB46" s="11"/>
       <c r="AC46" s="11" t="s">
+        <v>694</v>
+      </c>
+      <c r="AD46" s="11" t="s">
         <v>695</v>
-      </c>
-      <c r="AD46" s="11" t="s">
-        <v>696</v>
       </c>
       <c r="AE46" s="11" t="s">
         <v>360</v>
       </c>
       <c r="AF46" s="11" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="AG46" s="11" t="s">
         <v>361</v>
@@ -10699,83 +10945,107 @@
       <c r="AH46" s="11" t="s">
         <v>362</v>
       </c>
-      <c r="AI46" s="54" t="s">
-        <v>727</v>
+      <c r="AI46" s="47" t="s">
+        <v>726</v>
       </c>
     </row>
-    <row r="47" spans="1:35" ht="283" customHeight="1">
-      <c r="A47" s="39">
+    <row r="47" spans="1:35" s="55" customFormat="1" ht="283" customHeight="1">
+      <c r="A47" s="51">
         <v>40</v>
       </c>
-      <c r="B47" s="41" t="s">
+      <c r="B47" s="52" t="s">
         <v>363</v>
       </c>
-      <c r="C47" s="39">
+      <c r="C47" s="51">
         <v>3</v>
       </c>
-      <c r="D47" s="55">
+      <c r="D47" s="56">
         <v>2019</v>
       </c>
-      <c r="E47" s="49" t="s">
+      <c r="E47" s="61" t="s">
         <v>364</v>
       </c>
-      <c r="F47" s="50" t="s">
+      <c r="F47" s="62" t="s">
         <v>365</v>
       </c>
-      <c r="G47" s="48">
+      <c r="G47" s="63">
         <v>2019</v>
       </c>
-      <c r="H47" s="51" t="s">
+      <c r="H47" s="64" t="s">
         <v>366</v>
       </c>
-      <c r="I47" s="41" t="s">
+      <c r="I47" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="J47" s="41" t="s">
+      <c r="J47" s="52" t="s">
         <v>367</v>
       </c>
-      <c r="K47" s="41" t="s">
+      <c r="K47" s="52" t="s">
         <v>368</v>
       </c>
-      <c r="L47" s="40" t="s">
+      <c r="L47" s="53" t="s">
         <v>369</v>
       </c>
-      <c r="M47" s="41" t="s">
+      <c r="M47" s="52" t="s">
         <v>370</v>
       </c>
-      <c r="N47" s="45">
+      <c r="N47" s="60">
         <v>18</v>
       </c>
-      <c r="O47" s="41" t="s">
-        <v>449</v>
-      </c>
-      <c r="P47" s="41"/>
-      <c r="Q47" s="41"/>
-      <c r="R47" s="41"/>
-      <c r="S47" s="41"/>
-      <c r="T47" s="42"/>
-      <c r="U47" s="40" t="s">
+      <c r="O47" s="52" t="s">
+        <v>448</v>
+      </c>
+      <c r="P47" s="52" t="s">
+        <v>620</v>
+      </c>
+      <c r="Q47" s="52" t="s">
+        <v>620</v>
+      </c>
+      <c r="R47" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="S47" s="52" t="s">
+        <v>620</v>
+      </c>
+      <c r="T47" s="54" t="s">
+        <v>702</v>
+      </c>
+      <c r="U47" s="53" t="s">
         <v>314</v>
       </c>
-      <c r="V47" s="42"/>
-      <c r="W47" s="42"/>
-      <c r="X47" s="40"/>
-      <c r="Y47" s="42"/>
-      <c r="Z47" s="42"/>
-      <c r="AA47" s="42"/>
-      <c r="AB47" s="42"/>
-      <c r="AC47" s="42"/>
-      <c r="AD47" s="42"/>
-      <c r="AE47" s="42"/>
-      <c r="AF47" s="42"/>
-      <c r="AG47" s="42"/>
-      <c r="AH47" s="42"/>
-      <c r="AI47" s="1" t="s">
-        <v>728</v>
+      <c r="V47" s="54" t="s">
+        <v>623</v>
+      </c>
+      <c r="W47" s="54" t="s">
+        <v>685</v>
+      </c>
+      <c r="X47" s="53" t="s">
+        <v>761</v>
+      </c>
+      <c r="Y47" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z47" s="54" t="s">
+        <v>763</v>
+      </c>
+      <c r="AA47" s="54" t="s">
+        <v>762</v>
+      </c>
+      <c r="AB47" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC47" s="54"/>
+      <c r="AD47" s="54"/>
+      <c r="AE47" s="54"/>
+      <c r="AF47" s="54"/>
+      <c r="AG47" s="54"/>
+      <c r="AH47" s="54"/>
+      <c r="AI47" s="55" t="s">
+        <v>726</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:B47"/>
+  <autoFilter ref="AI1:AI47"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" display="A Proposed Model-driven Approach to Manage Architectural Technical Debt Life Cycle _x000a_"/>

</xml_diff>

<commit_message>
Updating scripts to get tools and methods from dataset
</commit_message>
<xml_diff>
--- a/dataset/Extraction_form_basic.xlsx
+++ b/dataset/Extraction_form_basic.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Folha 1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1345" uniqueCount="781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1346" uniqueCount="781">
   <si>
     <t>Paper Id</t>
   </si>
@@ -4017,9 +4017,6 @@
     <t xml:space="preserve">we study architecture evolution by identifying the major design decisions that were introduced along a number of the most significant releases (see Section 4). Such design decisions are mainly: (a) architecture components, including their interfaces, such as the kernel, shells, and libraries; (b) architecture connectors such as pipes and C header files; (c) architecture patterns [71] that were applied in the system, such as layering and reflection; and (d) the princi- ples that guide the system architecture, such as modularity and separation of concerns. A quantitative point of view. Specifically we look at how metrics of size and complexity evolve over time; these metrics concern system features (e.g. number of user commands or system calls), as determined by the Unix reference documentation </t>
   </si>
   <si>
-    <t>analysis of unix documentation, analysis of repository of unix history, souce code analysis, measure complexity, calculate cyclomatic complexity, component level, Constant Comparison, Another major force that has been driving the software architecture is portability.</t>
-  </si>
-  <si>
     <t>The architecture technical debt is systematically paid back despite increasing system size and complexity; identified, repayment, monitored</t>
   </si>
   <si>
@@ -4041,9 +4038,6 @@
     <t>Tracking architecture roots, architecutre flaws and Decopling Level for each version analysed by Titan tool</t>
   </si>
   <si>
-    <t>Titan, architecture smells, Decopling Level, DRSpace, Propagation Cost, DSM</t>
-  </si>
-  <si>
     <t>Yes, using a owner formula to calculate the effort to fix the architecture smell</t>
   </si>
   <si>
@@ -4057,9 +4051,6 @@
   </si>
   <si>
     <t>Yes, using a owner formula to calculate the effort to fix the architecture root</t>
-  </si>
-  <si>
-    <t>DRSpace, Architectural Root, Architecture Smell, DSM, DRH, Coupling, latix, source code analysis</t>
   </si>
   <si>
     <t>Good</t>
@@ -4087,13 +4078,22 @@
     <t>Yes, using a owner formula to calculate the tim effort to fix the architecture smell</t>
   </si>
   <si>
-    <t>Arcan, Architecture Smell</t>
-  </si>
-  <si>
-    <t>Taxonomy of ATD</t>
-  </si>
-  <si>
     <t>Yes, using quality model to check increasing or decreasing of ATD accumulation</t>
+  </si>
+  <si>
+    <t>general:# approuch: ' Architecture Smell'#tools: 'Arcan'</t>
+  </si>
+  <si>
+    <t>general: # approuch: architecture smells, Decopling Level, DRSpace, Propagation Cost, DSM# tools: 'Titan'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">general: # appouch: analysis of unix documentation, analysis of repository of unix history, souce code analysis, measure complexity, calculate cyclomatic complexity, component level, Constant Comparison, Another major force that has been driving the software architecture is portability# tools: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">general: # approuch: 'Taxonomy of ATD'# tools: </t>
+  </si>
+  <si>
+    <t>general: # approuch: 'DRSpace, Architectural Root, Architecture Smell, DSM, DRH, Coupling, source code analysis'# tools: latix</t>
   </si>
 </sst>
 </file>
@@ -4429,8 +4429,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="85">
+  <cellStyleXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4883,7 +4886,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="85">
+  <cellStyles count="86">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -4968,6 +4971,7 @@
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6121,10 +6125,10 @@
   <dimension ref="A1:AI47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="U36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V44" sqref="V44"/>
+      <selection pane="bottomRight" activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -6542,7 +6546,7 @@
         <v>46</v>
       </c>
       <c r="V4" s="11" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="W4" s="11" t="s">
         <v>686</v>
@@ -6857,7 +6861,7 @@
         <v>73</v>
       </c>
       <c r="V7" s="11" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="W7" s="11" t="s">
         <v>753</v>
@@ -6962,7 +6966,7 @@
         <v>599</v>
       </c>
       <c r="V8" s="11" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="W8" s="11" t="s">
         <v>754</v>
@@ -7172,7 +7176,7 @@
         <v>704</v>
       </c>
       <c r="V10" s="9" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="W10" s="9" t="s">
         <v>686</v>
@@ -7505,7 +7509,7 @@
         <v>125</v>
       </c>
       <c r="AB13" s="53" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="AC13" s="54"/>
       <c r="AD13" s="54"/>
@@ -7513,7 +7517,7 @@
         <v>28</v>
       </c>
       <c r="AF13" s="54" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="AG13" s="54"/>
       <c r="AH13" s="54"/>
@@ -7987,7 +7991,7 @@
         <v>16</v>
       </c>
       <c r="O18" s="53" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="P18" s="53" t="s">
         <v>620</v>
@@ -8020,13 +8024,13 @@
         <v>396</v>
       </c>
       <c r="Z18" s="53" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="AA18" s="53" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="AB18" s="53" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="AC18" s="54"/>
       <c r="AD18" s="54"/>
@@ -8034,7 +8038,7 @@
         <v>28</v>
       </c>
       <c r="AF18" s="54" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="AG18" s="54"/>
       <c r="AH18" s="54"/>
@@ -8107,7 +8111,7 @@
         <v>735</v>
       </c>
       <c r="V19" s="53" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="W19" s="53" t="s">
         <v>686</v>
@@ -8116,16 +8120,16 @@
         <v>639</v>
       </c>
       <c r="Y19" s="52" t="s">
+        <v>764</v>
+      </c>
+      <c r="Z19" s="53" t="s">
+        <v>777</v>
+      </c>
+      <c r="AA19" s="53" t="s">
         <v>765</v>
       </c>
-      <c r="Z19" s="53" t="s">
+      <c r="AB19" s="53" t="s">
         <v>766</v>
-      </c>
-      <c r="AA19" s="53" t="s">
-        <v>767</v>
-      </c>
-      <c r="AB19" s="53" t="s">
-        <v>768</v>
       </c>
       <c r="AC19" s="54"/>
       <c r="AD19" s="54"/>
@@ -8133,7 +8137,7 @@
         <v>475</v>
       </c>
       <c r="AF19" s="54" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="AG19" s="54"/>
       <c r="AH19" s="54"/>
@@ -8416,7 +8420,7 @@
         <v>395</v>
       </c>
       <c r="V22" s="13" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="W22" s="13" t="s">
         <v>686</v>
@@ -8731,7 +8735,7 @@
         <v>606</v>
       </c>
       <c r="V25" s="11" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="W25" s="11" t="s">
         <v>753</v>
@@ -9151,7 +9155,7 @@
         <v>717</v>
       </c>
       <c r="V29" s="11" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="W29" s="11" t="s">
         <v>686</v>
@@ -9256,7 +9260,7 @@
         <v>271</v>
       </c>
       <c r="V30" s="11" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="W30" s="11" t="s">
         <v>686</v>
@@ -9361,7 +9365,7 @@
         <v>276</v>
       </c>
       <c r="V31" s="53" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="W31" s="53" t="s">
         <v>753</v>
@@ -9373,13 +9377,13 @@
         <v>396</v>
       </c>
       <c r="Z31" s="54" t="s">
+        <v>778</v>
+      </c>
+      <c r="AA31" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB31" s="54" t="s">
         <v>758</v>
-      </c>
-      <c r="AA31" s="54" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB31" s="54" t="s">
-        <v>759</v>
       </c>
       <c r="AC31" s="54"/>
       <c r="AD31" s="54"/>
@@ -9876,7 +9880,7 @@
         <v>608</v>
       </c>
       <c r="V36" s="11" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="W36" s="11" t="s">
         <v>755</v>
@@ -9996,10 +10000,10 @@
         <v>779</v>
       </c>
       <c r="AA37" s="54" t="s">
-        <v>780</v>
+        <v>775</v>
       </c>
       <c r="AB37" s="54" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="AC37" s="54"/>
       <c r="AD37" s="54"/>
@@ -10007,7 +10011,7 @@
         <v>28</v>
       </c>
       <c r="AF37" s="54" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="AG37" s="54"/>
       <c r="AH37" s="54"/>
@@ -10078,7 +10082,7 @@
       </c>
       <c r="U38" s="54"/>
       <c r="V38" s="53" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="W38" s="53" t="s">
         <v>686</v>
@@ -10090,10 +10094,10 @@
         <v>396</v>
       </c>
       <c r="Z38" s="54" t="s">
-        <v>772</v>
+        <v>780</v>
       </c>
       <c r="AA38" s="54" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="AB38" s="54" t="s">
         <v>620</v>
@@ -10498,13 +10502,13 @@
         <v>754</v>
       </c>
       <c r="X42" s="53" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="Y42" s="54" t="s">
         <v>26</v>
       </c>
       <c r="Z42" s="54" t="s">
-        <v>292</v>
+        <v>26</v>
       </c>
       <c r="AA42" s="54" t="s">
         <v>26</v>
@@ -10518,7 +10522,7 @@
         <v>284</v>
       </c>
       <c r="AF42" s="54" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="AG42" s="54"/>
       <c r="AH42" s="54"/>
@@ -10696,7 +10700,7 @@
         <v>607</v>
       </c>
       <c r="V44" s="11" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="W44" s="11" t="s">
         <v>684</v>
@@ -11017,22 +11021,24 @@
         <v>684</v>
       </c>
       <c r="X47" s="53" t="s">
+        <v>759</v>
+      </c>
+      <c r="Y47" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z47" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA47" s="54" t="s">
         <v>760</v>
       </c>
-      <c r="Y47" s="54" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z47" s="54" t="s">
-        <v>762</v>
-      </c>
-      <c r="AA47" s="54" t="s">
+      <c r="AB47" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC47" s="54"/>
+      <c r="AD47" s="54" t="s">
         <v>761</v>
       </c>
-      <c r="AB47" s="54" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC47" s="54"/>
-      <c r="AD47" s="54"/>
       <c r="AE47" s="54"/>
       <c r="AF47" s="54"/>
       <c r="AG47" s="54"/>
@@ -11053,6 +11059,7 @@
     <hyperlink ref="O41" r:id="rId6" display="Analyse a set of application from Cast database system tWe analyzed these applications us- ing CAST’s Application Intelligence Platform (AIP),7 which analyzes an en- tire application using more than 1,200 rules to detect violations of good ar- chitectural and coding practice. We drew these rules from software engi- neering literature, repositories such as the Common Weakness Enumeration (CWE; cwe.mitre.org), online discus- sion groups of structural quality prob- lems, and customer experience as re- ported from defect logs and application architects. As an example, security- related violations would include SQL injection, cross-site scripting, buffer overflows, and other violations from the CWE. _x000a_"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Refactoring scripts to generate the tables with extra papers
</commit_message>
<xml_diff>
--- a/dataset/Extraction_form_basic.xlsx
+++ b/dataset/Extraction_form_basic.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000"/>
   </bookViews>
   <sheets>
     <sheet name="Folha 1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1346" uniqueCount="781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1662" uniqueCount="861">
   <si>
     <t>Paper Id</t>
   </si>
@@ -4095,12 +4095,275 @@
   <si>
     <t>general: # approuch: 'DRSpace, Architectural Root, Architecture Smell, DSM, DRH, Coupling, source code analysis'# tools: latix</t>
   </si>
+  <si>
+    <t>Architectural Technical Debt: A Grounded Theory</t>
+  </si>
+  <si>
+    <t>Skuld: a self-learning tool for impact-driven technical debt management</t>
+  </si>
+  <si>
+    <t>Long-Term Evaluation of Technical Debt in Open-Source Software</t>
+  </si>
+  <si>
+    <t>Towards an Approach to Identify Obsolete Features based on Importance and Technical Debt</t>
+  </si>
+  <si>
+    <t>Software Architecture Reconstruction via a Genetic Algorithm: Applying the Move Class Refactoring</t>
+  </si>
+  <si>
+    <t>Characterizing Architectural Drifts of Adaptive Systems</t>
+  </si>
+  <si>
+    <t>Improving agility by managing shared libraries in microservices</t>
+  </si>
+  <si>
+    <t>A modeling method for systematic architecture reconstruction of microservice-based software systems</t>
+  </si>
+  <si>
+    <t>Managing security debt across PLC phases in a VSE context</t>
+  </si>
+  <si>
+    <t>A preliminary analysis of self-adaptive systems according to different issues</t>
+  </si>
+  <si>
+    <t>An empirical investigation on the relationship between design and architecture smells</t>
+  </si>
+  <si>
+    <t>Verdechia, Kruchten and Lago 2020</t>
+  </si>
+  <si>
+    <t>Roberto Verdecchia, Philippe Kruchten, Patricia Lago</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Architectural technical debt in a software-intensive system is driven by design decisions about its structure, frameworks, technologies, languages, etc. Unlike code-level technical debt, which can be readily detected by static analysers, and can often be refactored with minimal efforts, architectural debt is hard to detect, and its remediation is wide- ranging, daunting, and often avoided. The objective of this study is to develop a better understanding of how software development organisations conceptualize their architectural debt, and how they deal with it, if at all. We used a grounded theory method, eliciting qualitative data from software architects and senior technical staff from a wide range of software development organizations. The result of the study, i.e., the theory emerging from the collected data, constitutes an encompassing conceptual theory of architectural debt, identifying and relating concepts such as symptoms, causes, consequences, and management strategies. By grounding the findings in empirical data, the theory provides researchers and practitioners with evidence of which crucial factors of architectural technical debt are experienced in industrial contexts.</t>
+  </si>
+  <si>
+    <t>Software Architecture: 14th European Conference, ECSA 2020</t>
+  </si>
+  <si>
+    <t>Software Architecture, Technical Debt, Grounded Theory</t>
+  </si>
+  <si>
+    <t>As the development progresses, software projects tend to accumulate Technical Debt and become harder to maintain. Multiple tools exist with the mission to help practitioners to better manage Technical Debt. Despite this progress, there is a lack of tools providing actionable and self-learned suggestions to practitioners aimed at mitigating the impact of Technical Debt in real projects. We aim to create a data-driven, lightweight, and self-learning tool positioning highly impactful refactoring proposals on a Jira backlog. Bearing this goal in mind, the first two authors have founded a startup, called Skuld.ai, with the vision of becoming the go-to software renovation company. In this tool paper, we present the software architecture and demonstrate the main functionalities of our tool. It has been showcased to practitioners, receiving positive feedback. Currently, its release to the market is underway thanks to an industry-research institute collaboration with Fraunhofer IESE to incorporate self-learning technical debt capabilities.</t>
+  </si>
+  <si>
+    <t>Technical Debt, Project Management, Tool, Data-Driven Development</t>
+  </si>
+  <si>
+    <t>Create a tool to monitor Technical Debt information over the repository and issue tracker using a self-learing method to predict Technical Debt.</t>
+  </si>
+  <si>
+    <t>Josep Burgaya Pujols ,Pieter Bas Pieter Bas, Silverio Martínez-Fernández,Antonio Martini,Adam Trendowicz</t>
+  </si>
+  <si>
+    <t>Tushar Sharma, Paramvir Singh, Diomidis Spinellis</t>
+  </si>
+  <si>
+    <t>Context: Architecture of a software system represents the key design decisions and there- fore its quality plays an important role to keep the software maintainable. Code smells are indicators of quality issues in a software system and are classified based on their granular- ity, scope, and impact. Despite a plethora of existing work on smells, a detailed exploration of architecture smells, their characteristics, and their relationships with smells in other granularities is missing.
+Objective: The paper aims to study architecture smells characteristics, investigate correla- tion, collocation, and causation relationships between architecture and design smells.
+Method: We implement smell detection support for seven architecture smells. We mine 3073 open-source repositories containing more than 118 million lines of C# code and empirically investigate the relationships between seven architecture and 19 design smells.
+Results: Wefindthatsmelldensitydoesnotdependonrepositorysize.Cumulatively,archi- tecture smells are highly correlated with design smells. Our collocation analysis finds that the majority of design and architecture smell pairs do not exhibit collocation. Finally, our causality analysis reveals that design smells cause architecture smells.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empirical Software Engineering </t>
+  </si>
+  <si>
+    <t>Empirical Software Engineering</t>
+  </si>
+  <si>
+    <t>Maintainability,Code quality,Code smells,Architecture smells,Design smells,Inter-smell relationships,Collocation,Correlation,Causality,Refactoring</t>
+  </si>
+  <si>
+    <t>Experiment</t>
+  </si>
+  <si>
+    <t>Incomplete</t>
+  </si>
+  <si>
+    <t>Claudia Raibulet1,Francesca Arcelli Fontana,Simone Carettoni</t>
+  </si>
+  <si>
+    <t>Self-adaptive systems dynamically change their structure and behavior in response to changes in their execution environment to ensure the quality of the services they provide. Self-adaptive systems are usually built of a managed part, which implements their func- tionality, and a managing part, which implements the self-adaptive mechanisms. Hence, the complexity of self-adaptive systems results also from the existence of the managing part and the interaction between the managed and the managing parts. The available evalua- tion approaches of self-adaptive systems focus on their performances, i.e., on the benefits (e.g., degree of autonomy, support for detecting anomalous behavior, adaptivity time, qual- ity of response) achieved through the self-adaptive mechanisms of the managing part. In this paper, we evaluate the quality of the design of self-adaptive systems (including the managed and the managing parts) as it is done in traditional software engineering. We are interested in the internal software quality of self-adaptive systems, as the existence of the managing part and its interaction with the managed part leads to a tightly coupled system. We analyze the self-adaptive systems through the detection of different issues such as architectural and code smells and the detection of design patterns. The smells provide some hints on possible design and implementation problems, and help software engineers to improve the quality of the systems. While, design patterns are usually indicators of the application of good prac- tices in the software development and allow to capture part of the design rationale. In this way, they can help software engineers to understand, reuse, and extend self-adaptive sys- tems. In this paper, we have considered the detection of 3 architectural smells, 18 code smells, and 15 design patterns in 11 self-adaptive systems written in the Java programming language. The results indicate that the 3 architectural smells, 9 out of the 18 code smells, and the 15 design patterns have been detected in all the analyzed self-adaptive systems. We also discuss the possible reasons behind the presence of these quality issues, and provide our lessons learned.</t>
+  </si>
+  <si>
+    <t>Software Quality Journal</t>
+  </si>
+  <si>
+    <t>Software Quality</t>
+  </si>
+  <si>
+    <t>Self-adaptive systems,Software quality,Architectural smells,Code smells,Design patterns</t>
+  </si>
+  <si>
+    <t>Background: A consistent body of research and practice have iden- tified that technical debt provides valuable and actionable insight into the design and implementation deficiencies of complex soft- ware systems. Existing software tools enable characterizing and measuring the amount of technical debt at selective granularity lev- els; by providing a computational model, they enable stakeholders to measure and ultimately control this phenomenon. Aims: In this paper we aim to study the evolution and characteristics of technical debt in open-source software. For this, we carry out a longitudi- nal study that covers the entire development history of several complex applications. The goal is to improve our understanding of how the amount and composition of technical debt changes in evolving software. We also study how new technical debt is in- troduced in software, as well as identify how developers handle its accumulation over the long term. Method: We carried out our evaluation using three complex, open-source Java applications. All 110 released versions, covering more than 10 years of development history for each application were analyzed using SonarQube. We studied how the amount, composition and history of technical debt changed during development, compared our results across the studied applications and present our most important findings. Results: For each application, we identified key versions during which large amounts of technical debt were added, removed or both. This had significantly more impact when compared to the lines of code or class count increases that generally occurred during devel- opment. However, within each version, we found high correlation between file lines of code and technical debt. We observed that the Pareto principle was satisfied for the studied applications, as 20% of issue types generated around 80% of total technical debt. Interest- ingly, there was a large degree of overlap between the issues that generated most of the debt across the studied applications. Conclu- sions: Early application versions showed greater fluctuation in the amount of existing technical debt. We found application size to be an unreliable predictor for the quantity of technical debt. Most debt was introduced in applications as part of milestone releases that expanded their feature set; likewise, we identified releases where extensive refactoring significantly reduced the level of debt. also discovered that technical debt issues persist for a long time in source code, and their removal did not appear to be prioritized according to type or severity.</t>
+  </si>
+  <si>
+    <t>International Symposium on Empirical Software Engineering and Measurement</t>
+  </si>
+  <si>
+    <t>software evolution, software maintenance, technical debt, static analysis, open-source</t>
+  </si>
+  <si>
+    <t>Arthur-Jozsef Molnar,Simona  Motogna</t>
+  </si>
+  <si>
+    <t>Andrea Janes, Valentina Lenarduzzi</t>
+  </si>
+  <si>
+    <t>Many of today’s software systems are maintained over years or even decades. To ensure that software remains useful, new features have to be added or old features have to be adapted to respond to new or changed requirements. As time goes on, some of the features become obsolete, i.e., are not needed anymore. Typically, these features are not removed because of various reasons, e.g., because removing them might be considered too costly, the costs of keeping unused features is considered low, or because of the “sunk cost fallacy”, i.e., that a feature is considered worth to keep because of the previously invested resources (time, money or effort) to build it. The consequences of keeping unused source code can impact maintainability, technical debt, performance, and extensibility of the system. This can lead to lower development productivity and to a reduced innovation ability, consequently reducing competitiveness on the market. This paper aims to present an approach to identify features based on their value and on costs for keeping or removing them.</t>
+  </si>
+  <si>
+    <t>2020 46th Euromicro Conference on Software Engineering and Advanced Applications (SEAA)</t>
+  </si>
+  <si>
+    <t>Feature importance, Technical Debt, Maintenance</t>
+  </si>
+  <si>
+    <t>Modularity is one of the four key principles of software design and architecture. According to this principle, software should be organized into modules that are tightly linked internally (high cohe- sion), whereas at the same time as independent from other modules as possible (low coupling). However, in practice, this principle is violated due to poor architecting design decisions, lack of time, or coding shortcuts, leading to a phenomenon termed as architectural technical debt (ATD). To alleviate this problem (lack of architec- tural modularity), the most common solution is the application of a software refactoring, namely Move Class—i.e., moving classes (the core artifact in object-oriented systems) from one module to another. To identify Move Class refactoring opportunities, we em- ploy a search-based optimization process, relying on optimization metrics, through which optimal moves are derived. Given the ex- tensive search space required for applying a brute-force search strategy, in this paper, we propose the use of a genetic algorithm that re-arranges existing software classes into existing or new mod- ules (software packages in Java, or folders in C++). To validate the usefulness of the proposed refactorings, we performed an indus- trial case study on three projects (from the Aviation, Healthcare, and Manufacturing application domains). The results of the study indicate that the proposed architecture reconstruction is able to improve modularity, improving both coupling and cohesion. The obtained results can be useful to practitioners through an open source tool; whereas at the same point, they open interesting future work directions.</t>
+  </si>
+  <si>
+    <t>Architecture reconstruction, coupling, cohesion, move class</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>An adaptive system (AS) evaluates its own behavior and changes it when the evaluation indicates that the system is not accomplishing what it is intended to do, or when better functionality or performance is possible. MAPE-K is a reference model that prescribes the adaptation mechanism of ASs by means of high-level abstractions such as Monitors, Analyzers, Planners and Executors and the relationships among them. Since the abstractions and the relationships provided by MAPE-K are generic, other reference models were proposed focusing on providing lower level abstractions to support software engineers in a more suitable way. However, after the analysis of seven representative ASs, we realized the abstractions prescribed by the existing reference models are not properly implemented, thus leading to architectural drifts. Therefore, in this paper we characterized three of these drifts by describing them with a template and showing practical examples. The three architectural drifts of ASs are Scattered Reference Inputs, Mixed Executors and Effectors, and Obscure Alternatives. We expect that by identifying and characterizing these drifts, we can help software architects improve their design and, as a consequence, increase the reliability of this type of systems.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">architectural drifts, adaptive system, mainte- nance
+</t>
+  </si>
+  <si>
+    <t>Using microservices is a way of supporting an agile architecture. However, if the microservices development is not properly managed, the teams’ development velocity may be affected, reducing agility and increasing architectural technical debt. This paper investigates how to manage the use of shared libraries in microservices to improve agility during development. We interviewed practitioners from four large international companies involved in microservices projects to identify problems when using shared libraries. Our results show that the participating companies had issues with shared libraries as follows: coupling among teams, delays on fixes due to overhead on libraries development teams, and need to maintain many versions of the libraries. Our results highlight that the use of shared libraries may hinder agility on microservices. Thus, their use should be restricted to situations where shared libraries cannot be replaced by a microservice and the costs of replicating the code on each service is very high.</t>
+  </si>
+  <si>
+    <t>International Conference on Agile Software Development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cross-company study, Multiple-case study,Software quality, Qualitative analysis, Architectural technical debt </t>
+  </si>
+  <si>
+    <t>Microservice Architecture (MSA) is an approach to architecting service- based software systems, which aims for decreasing service coupling to enable independent service development and deployment. Consequently, the adoption of MSA is expected to particularly benefit the scalability, maintainability, and reliability of monolithic systems. However, MSA adoption also increases architectural complexity in service design, implementation, and operation. As a result, Software Architecture Reconstruction (SAR) of microservice architectures is aggravated. This paper presents a modeling method that systematizes SAR of microservice architectures with the goal to facilitate its execution. The method yields reconstruction models for certain architecture viewpoints in MSA to enable efficient architecture analysis. We validate the methodʼs applicability by means of a case study architecture and the assessment of its risk in technical debt using derived reconstruction models.</t>
+  </si>
+  <si>
+    <t>International Conference on Evaluation and Modeling Methods for Systems Analysis and Development</t>
+  </si>
+  <si>
+    <t>Systems Modeling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microservice architecture, Software Architecture,Reconstruction,Model-driven engineering, Modeling languages </t>
+  </si>
+  <si>
+    <t>Nowadays, security and safety aspects are two of the major concerns for any soft- ware system development, especially while developing safety critical systems. This is especially relevant for very small entities because they have a limited amount of resources for dealing with all these aspects at the same time. In addition, these sys- tems are highly regulated domains, and they involve a huge set of standards focused on safety and security‐related issues. Therefore, these small entities are not only fac- ing hurdles related to technical aspects but also from the so‐called technical debt when overarching a critical development. This paper extends the assurance cases approach by integrating security aspects within the life cycle, and it proposes a frame- work for managing the associated security technical debt for very small entities. A tool chain is outlined, and the approach is illustrated with an industrial use case.</t>
+  </si>
+  <si>
+    <t>assurance case, ISO/IEC 29110, safety, security, technical debt</t>
+  </si>
+  <si>
+    <t>Pujols, Josep Burgaya, et al. 2020</t>
+  </si>
+  <si>
+    <t>Molnar, Arthur-Jozsef, and Simona Motogna 2020</t>
+  </si>
+  <si>
+    <t>Janes, Andrea, and Valentina Lenarduzzi 2020</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Maikantis, Theodoros, et al. 2020</t>
+  </si>
+  <si>
+    <t>Theodoros Maikantis,Angeliki Agathi Tsintzira,Apostolos Ampatzoglou,Elvira Maria Arvanitou,Alexander Chatzigeorgiou,Ioannis G Stamelos</t>
+  </si>
+  <si>
+    <t>24th Pan-Hellenic Conference on Informatics</t>
+  </si>
+  <si>
+    <t>Pan-Hellenic Conference on Informatics</t>
+  </si>
+  <si>
+    <t>Informatics</t>
+  </si>
+  <si>
+    <t>Daniel San Martín, Bento Siqueira, Valter Vieira de Camargo, Fabiano Ferrari</t>
+  </si>
+  <si>
+    <t>San Martín, Daniel, et al 2020</t>
+  </si>
+  <si>
+    <t>IEEE 27th International Conference on Software Analysis, Evolution and Reengineering (SANER)</t>
+  </si>
+  <si>
+    <t>International Conference on Software Analysis, Evolution and Reengineering (SANER)</t>
+  </si>
+  <si>
+    <t>Saulo S. de Toledo, Antonio Martini, Dag I. K. Sjoberg</t>
+  </si>
+  <si>
+    <t>de Toledo, Saulo S., Antonio Martini, and Dag IK Sjoberg 2020</t>
+  </si>
+  <si>
+    <t>Florian Rademacher, Sabine Sachweh, Albert Zündorf</t>
+  </si>
+  <si>
+    <t>Rademacher, Florian, Sabine Sachweh, and Albert Zundorf 2020</t>
+  </si>
+  <si>
+    <t>Xabier Larrucea, Izaskun Santamaria, Borja Fernandez‐Gauna</t>
+  </si>
+  <si>
+    <t>Larrucea, Xabier, Izaskun Santamaria, and Borja Fernandez‐Gauna 2020</t>
+  </si>
+  <si>
+    <t>Raibulet, Claudia, Francesca Arcelli Fontana, and Simone Carettoni 2020</t>
+  </si>
+  <si>
+    <t>Tushar Sharma, Paramvir Singh and Diomidis Spinellis 2020</t>
+  </si>
+  <si>
+    <t>general:""
+# 
+approuch:""
+#
+tools:"Arcan"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">general:""
+# 
+approuch:""
+#
+tools:"proprietary"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">general:""
+# 
+approuch:""
+#
+tools:"Sonarqube"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">general:""
+# 
+approuch:""
+#
+tools:"Skuld"
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -4227,6 +4490,17 @@
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="8"/>
+      <name val="LykrxsHpbcsdDmthxtLstjsxMyriadP"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -4254,7 +4528,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -4428,8 +4702,75 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="thin">
+        <color indexed="17"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="thin">
+        <color indexed="17"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="86">
+  <cellStyleXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -4688,8 +5029,101 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -4873,20 +5307,62 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="86">
+  <cellStyles count="117">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -4972,6 +5448,37 @@
     <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6122,29 +6629,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI47"/>
+  <dimension ref="A1:AI58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F46" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="H50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A47" sqref="A47"/>
+      <selection pane="bottomRight" activeCell="J57" sqref="J57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="5.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="7.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="36.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="64.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="11" width="33.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="19" style="1" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="37.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="16" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="78.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="64.6640625" style="1" customWidth="1"/>
+    <col min="9" max="11" width="33.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="19" style="1" customWidth="1"/>
+    <col min="13" max="13" width="37.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="16" style="1" customWidth="1"/>
     <col min="15" max="15" width="76.1640625" style="1" customWidth="1"/>
     <col min="16" max="19" width="13.5" style="1" customWidth="1"/>
     <col min="20" max="20" width="27.83203125" style="1" customWidth="1"/>
@@ -10951,100 +11457,1227 @@
       </c>
     </row>
     <row r="47" spans="1:35" s="55" customFormat="1" ht="283" customHeight="1">
-      <c r="A47" s="51">
+      <c r="A47" s="61">
         <v>40</v>
       </c>
-      <c r="B47" s="52" t="s">
+      <c r="B47" s="62" t="s">
         <v>363</v>
       </c>
-      <c r="C47" s="51">
+      <c r="C47" s="61">
         <v>3</v>
       </c>
       <c r="D47" s="56">
         <v>2019</v>
       </c>
-      <c r="E47" s="61" t="s">
+      <c r="E47" s="63" t="s">
         <v>364</v>
       </c>
-      <c r="F47" s="62" t="s">
+      <c r="F47" s="64" t="s">
         <v>365</v>
       </c>
-      <c r="G47" s="63">
+      <c r="G47" s="65">
         <v>2019</v>
       </c>
-      <c r="H47" s="64" t="s">
+      <c r="H47" s="66" t="s">
         <v>366</v>
       </c>
-      <c r="I47" s="52" t="s">
+      <c r="I47" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="J47" s="52" t="s">
+      <c r="J47" s="62" t="s">
         <v>367</v>
       </c>
-      <c r="K47" s="52" t="s">
+      <c r="K47" s="62" t="s">
         <v>368</v>
       </c>
-      <c r="L47" s="53" t="s">
+      <c r="L47" s="67" t="s">
         <v>369</v>
       </c>
-      <c r="M47" s="52" t="s">
+      <c r="M47" s="62" t="s">
         <v>370</v>
       </c>
-      <c r="N47" s="60">
+      <c r="N47" s="68">
         <v>18</v>
       </c>
-      <c r="O47" s="52" t="s">
+      <c r="O47" s="62" t="s">
         <v>448</v>
       </c>
-      <c r="P47" s="52" t="s">
-        <v>620</v>
-      </c>
-      <c r="Q47" s="52" t="s">
-        <v>620</v>
-      </c>
-      <c r="R47" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="S47" s="52" t="s">
-        <v>620</v>
-      </c>
-      <c r="T47" s="54" t="s">
+      <c r="P47" s="62" t="s">
+        <v>620</v>
+      </c>
+      <c r="Q47" s="62" t="s">
+        <v>620</v>
+      </c>
+      <c r="R47" s="62" t="s">
+        <v>26</v>
+      </c>
+      <c r="S47" s="62" t="s">
+        <v>620</v>
+      </c>
+      <c r="T47" s="69" t="s">
         <v>701</v>
       </c>
-      <c r="U47" s="53" t="s">
+      <c r="U47" s="67" t="s">
         <v>314</v>
       </c>
-      <c r="V47" s="54" t="s">
+      <c r="V47" s="69" t="s">
         <v>623</v>
       </c>
-      <c r="W47" s="54" t="s">
+      <c r="W47" s="69" t="s">
         <v>684</v>
       </c>
-      <c r="X47" s="53" t="s">
+      <c r="X47" s="67" t="s">
         <v>759</v>
       </c>
-      <c r="Y47" s="54" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z47" s="54" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA47" s="54" t="s">
+      <c r="Y47" s="69" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z47" s="69" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA47" s="69" t="s">
         <v>760</v>
       </c>
-      <c r="AB47" s="54" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC47" s="54"/>
-      <c r="AD47" s="54" t="s">
+      <c r="AB47" s="69" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC47" s="69"/>
+      <c r="AD47" s="69" t="s">
         <v>761</v>
       </c>
-      <c r="AE47" s="54"/>
-      <c r="AF47" s="54"/>
-      <c r="AG47" s="54"/>
-      <c r="AH47" s="54"/>
+      <c r="AE47" s="69"/>
+      <c r="AF47" s="69"/>
+      <c r="AG47" s="69"/>
+      <c r="AH47" s="69"/>
       <c r="AI47" s="55" t="s">
         <v>725</v>
+      </c>
+    </row>
+    <row r="48" spans="1:35" ht="46" customHeight="1">
+      <c r="A48" s="70">
+        <v>106</v>
+      </c>
+      <c r="B48" s="71" t="s">
+        <v>792</v>
+      </c>
+      <c r="C48" s="72"/>
+      <c r="D48" s="70">
+        <v>2020</v>
+      </c>
+      <c r="E48" s="73" t="s">
+        <v>793</v>
+      </c>
+      <c r="F48" s="74" t="s">
+        <v>781</v>
+      </c>
+      <c r="G48" s="72">
+        <v>2020</v>
+      </c>
+      <c r="H48" s="75" t="s">
+        <v>794</v>
+      </c>
+      <c r="I48" s="72" t="s">
+        <v>21</v>
+      </c>
+      <c r="J48" s="72" t="s">
+        <v>795</v>
+      </c>
+      <c r="K48" s="72" t="s">
+        <v>270</v>
+      </c>
+      <c r="L48" s="72" t="s">
+        <v>144</v>
+      </c>
+      <c r="M48" s="72" t="s">
+        <v>796</v>
+      </c>
+      <c r="N48" s="72">
+        <v>17</v>
+      </c>
+      <c r="O48" s="72"/>
+      <c r="P48" s="72" t="s">
+        <v>620</v>
+      </c>
+      <c r="Q48" s="72" t="s">
+        <v>620</v>
+      </c>
+      <c r="R48" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="S48" s="72" t="s">
+        <v>620</v>
+      </c>
+      <c r="T48" s="76" t="s">
+        <v>718</v>
+      </c>
+      <c r="U48" s="72" t="s">
+        <v>359</v>
+      </c>
+      <c r="V48" s="72" t="s">
+        <v>692</v>
+      </c>
+      <c r="W48" s="72" t="s">
+        <v>684</v>
+      </c>
+      <c r="X48" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y48" s="72" t="s">
+        <v>620</v>
+      </c>
+      <c r="Z48" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA48" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB48" s="72"/>
+      <c r="AC48" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD48" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE48" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF48" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG48" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH48" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI48" s="1" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="49" spans="1:35" ht="145" customHeight="1">
+      <c r="A49" s="72">
+        <v>107</v>
+      </c>
+      <c r="B49" s="72" t="s">
+        <v>836</v>
+      </c>
+      <c r="C49" s="72"/>
+      <c r="D49" s="72">
+        <v>2020</v>
+      </c>
+      <c r="E49" s="73" t="s">
+        <v>800</v>
+      </c>
+      <c r="F49" s="74" t="s">
+        <v>782</v>
+      </c>
+      <c r="G49" s="72">
+        <v>2020</v>
+      </c>
+      <c r="H49" s="75" t="s">
+        <v>797</v>
+      </c>
+      <c r="I49" s="72" t="s">
+        <v>21</v>
+      </c>
+      <c r="J49" s="72" t="s">
+        <v>23</v>
+      </c>
+      <c r="K49" s="72" t="s">
+        <v>23</v>
+      </c>
+      <c r="L49" s="72" t="s">
+        <v>24</v>
+      </c>
+      <c r="M49" s="72" t="s">
+        <v>798</v>
+      </c>
+      <c r="N49" s="72">
+        <v>2</v>
+      </c>
+      <c r="O49" s="72" t="s">
+        <v>799</v>
+      </c>
+      <c r="P49" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q49" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="R49" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="S49" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="T49" s="72"/>
+      <c r="U49" s="76" t="s">
+        <v>611</v>
+      </c>
+      <c r="V49" s="72" t="s">
+        <v>768</v>
+      </c>
+      <c r="W49" s="72" t="s">
+        <v>686</v>
+      </c>
+      <c r="X49" s="72" t="s">
+        <v>620</v>
+      </c>
+      <c r="Y49" s="72" t="s">
+        <v>620</v>
+      </c>
+      <c r="Z49" s="72" t="s">
+        <v>860</v>
+      </c>
+      <c r="AA49" s="72" t="s">
+        <v>620</v>
+      </c>
+      <c r="AB49" s="72" t="s">
+        <v>620</v>
+      </c>
+      <c r="AC49" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD49" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE49" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF49" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG49" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH49" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI49" s="1" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="50" spans="1:35" ht="130" customHeight="1">
+      <c r="A50" s="72">
+        <v>108</v>
+      </c>
+      <c r="B50" s="72" t="s">
+        <v>837</v>
+      </c>
+      <c r="C50" s="72"/>
+      <c r="D50" s="72">
+        <v>2020</v>
+      </c>
+      <c r="E50" s="73" t="s">
+        <v>816</v>
+      </c>
+      <c r="F50" s="74" t="s">
+        <v>783</v>
+      </c>
+      <c r="G50" s="72">
+        <v>2020</v>
+      </c>
+      <c r="H50" s="75" t="s">
+        <v>813</v>
+      </c>
+      <c r="I50" s="72" t="s">
+        <v>130</v>
+      </c>
+      <c r="J50" s="72" t="s">
+        <v>814</v>
+      </c>
+      <c r="K50" s="72" t="s">
+        <v>814</v>
+      </c>
+      <c r="L50" s="72" t="s">
+        <v>177</v>
+      </c>
+      <c r="M50" s="72" t="s">
+        <v>815</v>
+      </c>
+      <c r="N50" s="72">
+        <v>9</v>
+      </c>
+      <c r="O50" s="72"/>
+      <c r="P50" s="72" t="s">
+        <v>620</v>
+      </c>
+      <c r="Q50" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="R50" s="72" t="s">
+        <v>620</v>
+      </c>
+      <c r="S50" s="72" t="s">
+        <v>620</v>
+      </c>
+      <c r="T50" s="72" t="s">
+        <v>806</v>
+      </c>
+      <c r="U50" s="72" t="s">
+        <v>806</v>
+      </c>
+      <c r="V50" s="72" t="s">
+        <v>768</v>
+      </c>
+      <c r="W50" s="72" t="s">
+        <v>753</v>
+      </c>
+      <c r="X50" s="72" t="s">
+        <v>620</v>
+      </c>
+      <c r="Y50" s="72" t="s">
+        <v>620</v>
+      </c>
+      <c r="Z50" s="72" t="s">
+        <v>859</v>
+      </c>
+      <c r="AA50" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB50" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC50" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD50" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE50" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF50" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG50" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH50" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI50" s="1" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="51" spans="1:35" ht="20" customHeight="1">
+      <c r="A51" s="72">
+        <v>109</v>
+      </c>
+      <c r="B51" s="72" t="s">
+        <v>838</v>
+      </c>
+      <c r="C51" s="72"/>
+      <c r="D51" s="72">
+        <v>2020</v>
+      </c>
+      <c r="E51" s="73" t="s">
+        <v>817</v>
+      </c>
+      <c r="F51" s="74" t="s">
+        <v>784</v>
+      </c>
+      <c r="G51" s="72">
+        <v>2020</v>
+      </c>
+      <c r="H51" s="75" t="s">
+        <v>818</v>
+      </c>
+      <c r="I51" s="72" t="s">
+        <v>21</v>
+      </c>
+      <c r="J51" s="72" t="s">
+        <v>819</v>
+      </c>
+      <c r="K51" s="72" t="s">
+        <v>43</v>
+      </c>
+      <c r="L51" s="72" t="s">
+        <v>177</v>
+      </c>
+      <c r="M51" s="72" t="s">
+        <v>820</v>
+      </c>
+      <c r="N51" s="72">
+        <v>5</v>
+      </c>
+      <c r="O51" s="72"/>
+      <c r="P51" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q51" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="R51" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="S51" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="T51" s="72" t="s">
+        <v>839</v>
+      </c>
+      <c r="U51" s="72" t="s">
+        <v>839</v>
+      </c>
+      <c r="V51" s="72" t="s">
+        <v>692</v>
+      </c>
+      <c r="W51" s="72" t="s">
+        <v>753</v>
+      </c>
+      <c r="X51" s="72" t="s">
+        <v>620</v>
+      </c>
+      <c r="Y51" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z51" s="72" t="s">
+        <v>859</v>
+      </c>
+      <c r="AA51" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB51" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC51" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD51" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE51" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF51" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG51" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH51" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI51" s="1" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="52" spans="1:35" ht="88" customHeight="1">
+      <c r="A52" s="72">
+        <v>110</v>
+      </c>
+      <c r="B52" s="72" t="s">
+        <v>840</v>
+      </c>
+      <c r="C52" s="72"/>
+      <c r="D52" s="72">
+        <v>2020</v>
+      </c>
+      <c r="E52" s="72" t="s">
+        <v>841</v>
+      </c>
+      <c r="F52" s="74" t="s">
+        <v>785</v>
+      </c>
+      <c r="G52" s="72">
+        <v>2020</v>
+      </c>
+      <c r="H52" s="75" t="s">
+        <v>821</v>
+      </c>
+      <c r="I52" s="72" t="s">
+        <v>21</v>
+      </c>
+      <c r="J52" s="72" t="s">
+        <v>842</v>
+      </c>
+      <c r="K52" s="72" t="s">
+        <v>843</v>
+      </c>
+      <c r="L52" s="72" t="s">
+        <v>844</v>
+      </c>
+      <c r="M52" s="72" t="s">
+        <v>822</v>
+      </c>
+      <c r="N52" s="72">
+        <v>5</v>
+      </c>
+      <c r="O52" s="72"/>
+      <c r="P52" s="72" t="s">
+        <v>823</v>
+      </c>
+      <c r="Q52" s="72" t="s">
+        <v>823</v>
+      </c>
+      <c r="R52" s="72" t="s">
+        <v>824</v>
+      </c>
+      <c r="S52" s="72" t="s">
+        <v>823</v>
+      </c>
+      <c r="T52" s="72" t="s">
+        <v>806</v>
+      </c>
+      <c r="U52" s="72" t="s">
+        <v>806</v>
+      </c>
+      <c r="V52" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="W52" s="72" t="s">
+        <v>753</v>
+      </c>
+      <c r="X52" s="72" t="s">
+        <v>823</v>
+      </c>
+      <c r="Y52" s="72" t="s">
+        <v>824</v>
+      </c>
+      <c r="Z52" s="72" t="s">
+        <v>858</v>
+      </c>
+      <c r="AA52" s="72" t="s">
+        <v>824</v>
+      </c>
+      <c r="AB52" s="72" t="s">
+        <v>824</v>
+      </c>
+      <c r="AC52" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD52" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE52" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF52" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG52" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH52" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI52" s="1" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="53" spans="1:35" ht="20" customHeight="1">
+      <c r="A53" s="72">
+        <v>111</v>
+      </c>
+      <c r="B53" s="78" t="s">
+        <v>846</v>
+      </c>
+      <c r="C53" s="72"/>
+      <c r="D53" s="72">
+        <v>2020</v>
+      </c>
+      <c r="E53" s="72" t="s">
+        <v>845</v>
+      </c>
+      <c r="F53" s="74" t="s">
+        <v>786</v>
+      </c>
+      <c r="G53" s="72">
+        <v>2020</v>
+      </c>
+      <c r="H53" s="75" t="s">
+        <v>825</v>
+      </c>
+      <c r="I53" s="72" t="s">
+        <v>21</v>
+      </c>
+      <c r="J53" s="72" t="s">
+        <v>847</v>
+      </c>
+      <c r="K53" s="72" t="s">
+        <v>848</v>
+      </c>
+      <c r="L53" s="72" t="s">
+        <v>177</v>
+      </c>
+      <c r="M53" s="72" t="s">
+        <v>826</v>
+      </c>
+      <c r="N53" s="72">
+        <v>11</v>
+      </c>
+      <c r="O53" s="72"/>
+      <c r="P53" s="72" t="s">
+        <v>823</v>
+      </c>
+      <c r="Q53" s="72" t="s">
+        <v>824</v>
+      </c>
+      <c r="R53" s="72" t="s">
+        <v>823</v>
+      </c>
+      <c r="S53" s="72" t="s">
+        <v>823</v>
+      </c>
+      <c r="T53" s="72" t="s">
+        <v>806</v>
+      </c>
+      <c r="U53" s="72" t="s">
+        <v>806</v>
+      </c>
+      <c r="V53" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="W53" s="72" t="s">
+        <v>753</v>
+      </c>
+      <c r="X53" s="72" t="s">
+        <v>823</v>
+      </c>
+      <c r="Y53" s="72" t="s">
+        <v>824</v>
+      </c>
+      <c r="Z53" s="72" t="s">
+        <v>858</v>
+      </c>
+      <c r="AA53" s="72" t="s">
+        <v>824</v>
+      </c>
+      <c r="AB53" s="72" t="s">
+        <v>824</v>
+      </c>
+      <c r="AC53" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD53" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE53" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF53" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG53" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH53" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI53" s="1" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="54" spans="1:35" ht="20" customHeight="1">
+      <c r="A54" s="72">
+        <v>112</v>
+      </c>
+      <c r="B54" s="72" t="s">
+        <v>850</v>
+      </c>
+      <c r="C54" s="72"/>
+      <c r="D54" s="72">
+        <v>2020</v>
+      </c>
+      <c r="E54" s="73" t="s">
+        <v>849</v>
+      </c>
+      <c r="F54" s="74" t="s">
+        <v>787</v>
+      </c>
+      <c r="G54" s="72">
+        <v>2020</v>
+      </c>
+      <c r="H54" s="75" t="s">
+        <v>827</v>
+      </c>
+      <c r="I54" s="72" t="s">
+        <v>21</v>
+      </c>
+      <c r="J54" s="72" t="s">
+        <v>828</v>
+      </c>
+      <c r="K54" s="72" t="s">
+        <v>828</v>
+      </c>
+      <c r="L54" s="72" t="s">
+        <v>177</v>
+      </c>
+      <c r="M54" s="72" t="s">
+        <v>829</v>
+      </c>
+      <c r="N54" s="72">
+        <v>9</v>
+      </c>
+      <c r="O54" s="72"/>
+      <c r="P54" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q54" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="R54" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="S54" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="T54" s="72"/>
+      <c r="U54" s="72"/>
+      <c r="V54" s="72" t="s">
+        <v>768</v>
+      </c>
+      <c r="W54" s="72" t="s">
+        <v>752</v>
+      </c>
+      <c r="X54" s="72" t="s">
+        <v>823</v>
+      </c>
+      <c r="Y54" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z54" s="72" t="s">
+        <v>858</v>
+      </c>
+      <c r="AA54" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB54" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC54" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD54" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE54" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF54" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG54" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH54" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI54" s="1" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="55" spans="1:35" ht="20" customHeight="1">
+      <c r="A55" s="72">
+        <v>113</v>
+      </c>
+      <c r="B55" s="72" t="s">
+        <v>852</v>
+      </c>
+      <c r="C55" s="72"/>
+      <c r="D55" s="72">
+        <v>2020</v>
+      </c>
+      <c r="E55" s="72" t="s">
+        <v>851</v>
+      </c>
+      <c r="F55" s="74" t="s">
+        <v>788</v>
+      </c>
+      <c r="G55" s="72">
+        <v>2020</v>
+      </c>
+      <c r="H55" s="75" t="s">
+        <v>830</v>
+      </c>
+      <c r="I55" s="72" t="s">
+        <v>21</v>
+      </c>
+      <c r="J55" s="72" t="s">
+        <v>831</v>
+      </c>
+      <c r="K55" s="72" t="s">
+        <v>831</v>
+      </c>
+      <c r="L55" s="72" t="s">
+        <v>832</v>
+      </c>
+      <c r="M55" s="72" t="s">
+        <v>833</v>
+      </c>
+      <c r="N55" s="72">
+        <v>12</v>
+      </c>
+      <c r="O55" s="72"/>
+      <c r="P55" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q55" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="R55" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="S55" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="T55" s="72" t="s">
+        <v>806</v>
+      </c>
+      <c r="U55" s="72" t="s">
+        <v>806</v>
+      </c>
+      <c r="V55" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="W55" s="72" t="s">
+        <v>752</v>
+      </c>
+      <c r="X55" s="72" t="s">
+        <v>823</v>
+      </c>
+      <c r="Y55" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z55" s="72" t="s">
+        <v>858</v>
+      </c>
+      <c r="AA55" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB55" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC55" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD55" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE55" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF55" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG55" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH55" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI55" s="1" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="56" spans="1:35" ht="20" customHeight="1">
+      <c r="A56" s="72">
+        <v>114</v>
+      </c>
+      <c r="B56" s="72" t="s">
+        <v>854</v>
+      </c>
+      <c r="C56" s="72"/>
+      <c r="D56" s="72">
+        <v>2020</v>
+      </c>
+      <c r="E56" s="72" t="s">
+        <v>853</v>
+      </c>
+      <c r="F56" s="74" t="s">
+        <v>789</v>
+      </c>
+      <c r="G56" s="72">
+        <v>2020</v>
+      </c>
+      <c r="H56" s="75" t="s">
+        <v>834</v>
+      </c>
+      <c r="I56" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="J56" s="72" t="s">
+        <v>124</v>
+      </c>
+      <c r="K56" s="72" t="s">
+        <v>124</v>
+      </c>
+      <c r="L56" s="72" t="s">
+        <v>177</v>
+      </c>
+      <c r="M56" s="72" t="s">
+        <v>835</v>
+      </c>
+      <c r="N56" s="72">
+        <v>14</v>
+      </c>
+      <c r="O56" s="72"/>
+      <c r="P56" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q56" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="R56" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="S56" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="T56" s="72" t="s">
+        <v>806</v>
+      </c>
+      <c r="U56" s="72" t="s">
+        <v>806</v>
+      </c>
+      <c r="V56" s="72" t="s">
+        <v>659</v>
+      </c>
+      <c r="W56" s="72" t="s">
+        <v>684</v>
+      </c>
+      <c r="X56" s="72" t="s">
+        <v>620</v>
+      </c>
+      <c r="Y56" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z56" s="72" t="s">
+        <v>858</v>
+      </c>
+      <c r="AA56" s="72" t="s">
+        <v>620</v>
+      </c>
+      <c r="AB56" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC56" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD56" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE56" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF56" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG56" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH56" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI56" s="1" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="57" spans="1:35" ht="113" customHeight="1">
+      <c r="A57" s="72">
+        <v>115</v>
+      </c>
+      <c r="B57" s="72" t="s">
+        <v>855</v>
+      </c>
+      <c r="C57" s="72"/>
+      <c r="D57" s="72">
+        <v>2020</v>
+      </c>
+      <c r="E57" s="73" t="s">
+        <v>808</v>
+      </c>
+      <c r="F57" s="74" t="s">
+        <v>790</v>
+      </c>
+      <c r="G57" s="72">
+        <v>2020</v>
+      </c>
+      <c r="H57" s="75" t="s">
+        <v>809</v>
+      </c>
+      <c r="I57" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="J57" s="72" t="s">
+        <v>810</v>
+      </c>
+      <c r="K57" s="72" t="s">
+        <v>810</v>
+      </c>
+      <c r="L57" s="72" t="s">
+        <v>811</v>
+      </c>
+      <c r="M57" s="72" t="s">
+        <v>812</v>
+      </c>
+      <c r="N57" s="72">
+        <v>31</v>
+      </c>
+      <c r="O57" s="72"/>
+      <c r="P57" s="72" t="s">
+        <v>620</v>
+      </c>
+      <c r="Q57" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="R57" s="72" t="s">
+        <v>620</v>
+      </c>
+      <c r="S57" s="72" t="s">
+        <v>620</v>
+      </c>
+      <c r="T57" s="72" t="s">
+        <v>806</v>
+      </c>
+      <c r="U57" s="72" t="s">
+        <v>806</v>
+      </c>
+      <c r="V57" s="72" t="s">
+        <v>768</v>
+      </c>
+      <c r="W57" s="72" t="s">
+        <v>686</v>
+      </c>
+      <c r="X57" s="72" t="s">
+        <v>620</v>
+      </c>
+      <c r="Y57" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z57" s="72" t="s">
+        <v>857</v>
+      </c>
+      <c r="AA57" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB57" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC57" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD57" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE57" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF57" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG57" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH57" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI57" s="1" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="58" spans="1:35" ht="124" customHeight="1">
+      <c r="A58" s="72">
+        <v>116</v>
+      </c>
+      <c r="B58" s="72" t="s">
+        <v>856</v>
+      </c>
+      <c r="C58" s="72"/>
+      <c r="D58" s="72">
+        <v>2020</v>
+      </c>
+      <c r="E58" s="73" t="s">
+        <v>801</v>
+      </c>
+      <c r="F58" s="74" t="s">
+        <v>791</v>
+      </c>
+      <c r="G58" s="72">
+        <v>2020</v>
+      </c>
+      <c r="H58" s="75" t="s">
+        <v>802</v>
+      </c>
+      <c r="I58" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="J58" s="77" t="s">
+        <v>803</v>
+      </c>
+      <c r="K58" s="72" t="s">
+        <v>804</v>
+      </c>
+      <c r="L58" s="72" t="s">
+        <v>177</v>
+      </c>
+      <c r="M58" s="72" t="s">
+        <v>805</v>
+      </c>
+      <c r="N58" s="72">
+        <v>49</v>
+      </c>
+      <c r="O58" s="72"/>
+      <c r="P58" s="72" t="s">
+        <v>620</v>
+      </c>
+      <c r="Q58" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="R58" s="72" t="s">
+        <v>620</v>
+      </c>
+      <c r="S58" s="72" t="s">
+        <v>620</v>
+      </c>
+      <c r="T58" s="72" t="s">
+        <v>806</v>
+      </c>
+      <c r="U58" s="72" t="s">
+        <v>806</v>
+      </c>
+      <c r="V58" s="72" t="s">
+        <v>768</v>
+      </c>
+      <c r="W58" s="72" t="s">
+        <v>686</v>
+      </c>
+      <c r="X58" s="72" t="s">
+        <v>620</v>
+      </c>
+      <c r="Y58" s="72" t="s">
+        <v>620</v>
+      </c>
+      <c r="Z58" s="72" t="s">
+        <v>858</v>
+      </c>
+      <c r="AA58" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB58" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC58" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD58" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE58" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF58" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG58" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH58" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI58" s="1" t="s">
+        <v>807</v>
       </c>
     </row>
   </sheetData>
@@ -11059,7 +12692,6 @@
     <hyperlink ref="O41" r:id="rId6" display="Analyse a set of application from Cast database system tWe analyzed these applications us- ing CAST’s Application Intelligence Platform (AIP),7 which analyzes an en- tire application using more than 1,200 rules to detect violations of good ar- chitectural and coding practice. We drew these rules from software engi- neering literature, repositories such as the Common Weakness Enumeration (CWE; cwe.mitre.org), online discus- sion groups of structural quality prob- lems, and customer experience as re- ported from defect logs and application architects. As an example, security- related violations would include SQL injection, cross-site scripting, buffer overflows, and other violations from the CWE. _x000a_"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Updating measures of ATD
</commit_message>
<xml_diff>
--- a/dataset/Extraction_form_basic.xlsx
+++ b/dataset/Extraction_form_basic.xlsx
@@ -6643,10 +6643,10 @@
   <dimension ref="A1:AI58"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="V31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A57" sqref="A57"/>
+      <selection pane="bottomRight" activeCell="X31" sqref="X31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Updating monitoring of ATD
</commit_message>
<xml_diff>
--- a/dataset/Extraction_form_basic.xlsx
+++ b/dataset/Extraction_form_basic.xlsx
@@ -1991,12 +1991,6 @@
     </r>
   </si>
   <si>
-    <t>Context: A known problem in large software companies is to balance the prioritization of short-term with long-term feature delivery speed. Specifically, Architecture Technical Debt is regarded as sub-optimal architectural solutions taken to deliver fast that might hinder future feature development, which, in turn, would hinder agility. 
-Objective: This paper aims at improving software management by shedding light on the current factors responsible for the accumulation of Architectural Technical Debt and to understand how it evolves over time.
-Method: We conducted an exploratory multiple-case embedded case study in 7 sites at 5 large compa- nies. We evaluated the results with additional cross-company interviews and an in-depth, company-specific case study in which we initially evaluate factors and models. 
-Results: We compiled a taxonomy of the factors and their influence in the accumulation of Architectural Technical Debt, and we provide two qualitative models of how the debt is accumulated and refactored over time in the studied companies. We also list a set of exploratory propositions on possible refactoring strategies that can be useful as insights for practitioners and as hypotheses for further research. Conclusion: Several factors cause constant and unavoidable accumulation of Architecture Technical Debt, which leads to development crises. Refactorings are often overlooked in prioritization and they are often triggered by development crises, in a reactive fashion. Some of the factors are manageable, while others are external to the companies. ATD needs to be made visible, in order to postpone the crises according to the strategic goals of the companies. There is a need for practices and automated tools to proactively manage ATD</t>
-  </si>
-  <si>
     <t xml:space="preserve">Yuanfang Cai, Lu Xiao, Rick Kazman, Ran Mo, Qiong Feng 
 </t>
   </si>
@@ -4364,6 +4358,12 @@
       <t xml:space="preserve">erent ways by exploiting several tools with the aim to identify architectural violations, architectural smells or other relevant features. In this paper, we provide our experience report in using three known tools to capture in- formation that can be useful to identify and evaluate the architectural debt of an application. We outline the main diferences among these tools and the results they produce. 
 </t>
     </r>
+  </si>
+  <si>
+    <t>Context: A known problem in large software companies is to balance the prioritization of short-term with long-term feature delivery speed. Specifically, Architecture Technical Debt is regarded as sub-optimal architectural solutions taken to deliver fast that might hinder future feature development, which, in turn, would hinder agility. 
+Objective: This paper aims at improving software management by shedding light on the current factors responsible for the accumulation of Architectural Technical Debt and to understand how it evolves over time.
+Method: We conducted an exploratory multiple-case embedded case study in 7 sites at 5 large companies. We evaluated the results with additional cross-company interviews and an in-depth, company-specific case study in which we initially evaluate factors and models. 
+Results: We compiled a taxonomy of the factors and their influence in the accumulation of Architectural Technical Debt, and we provide two qualitative models of how the debt is accumulated and refactored over time in the studied companies. We also list a set of exploratory propositions on possible refactoring strategies that can be useful as insights for practitioners and as hypotheses for further research. Conclusion: Several factors cause constant and unavoidable accumulation of Architecture Technical Debt, which leads to development crises. Refactorings are often overlooked in prioritization and they are often triggered by development crises, in a reactive fashion. Some of the factors are manageable, while others are external to the companies. ATD needs to be made visible, in order to postpone the crises according to the strategic goals of the companies. There is a need for practices and automated tools to proactively manage ATD</t>
   </si>
 </sst>
 </file>
@@ -6643,10 +6643,10 @@
   <dimension ref="A1:AI58"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="V31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X31" sqref="X31"/>
+      <selection pane="bottomRight" activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -6693,7 +6693,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="37" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="E1" s="37" t="s">
         <v>3</v>
@@ -6729,43 +6729,43 @@
         <v>13</v>
       </c>
       <c r="P1" s="37" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="Q1" s="37" t="s">
+        <v>606</v>
+      </c>
+      <c r="R1" s="37" t="s">
+        <v>681</v>
+      </c>
+      <c r="S1" s="37" t="s">
         <v>607</v>
       </c>
-      <c r="R1" s="37" t="s">
+      <c r="T1" s="37" t="s">
         <v>682</v>
       </c>
-      <c r="S1" s="37" t="s">
-        <v>608</v>
-      </c>
-      <c r="T1" s="37" t="s">
+      <c r="U1" s="37" t="s">
         <v>683</v>
       </c>
-      <c r="U1" s="37" t="s">
-        <v>684</v>
-      </c>
       <c r="V1" s="37" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="W1" s="37" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="X1" s="37" t="s">
+        <v>709</v>
+      </c>
+      <c r="Y1" s="37" t="s">
         <v>710</v>
       </c>
-      <c r="Y1" s="37" t="s">
+      <c r="Z1" s="37" t="s">
         <v>711</v>
       </c>
-      <c r="Z1" s="37" t="s">
+      <c r="AA1" s="37" t="s">
         <v>712</v>
       </c>
-      <c r="AA1" s="37" t="s">
-        <v>713</v>
-      </c>
       <c r="AB1" s="37" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="AC1" s="37" t="s">
         <v>14</v>
@@ -6774,10 +6774,10 @@
         <v>15</v>
       </c>
       <c r="AE1" s="37" t="s">
+        <v>679</v>
+      </c>
+      <c r="AF1" s="37" t="s">
         <v>680</v>
-      </c>
-      <c r="AF1" s="37" t="s">
-        <v>681</v>
       </c>
       <c r="AG1" s="37" t="s">
         <v>16</v>
@@ -6786,7 +6786,7 @@
         <v>17</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="2" spans="1:35" ht="160" customHeight="1">
@@ -6812,7 +6812,7 @@
         <v>2019</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>21</v>
@@ -6836,62 +6836,62 @@
         <v>397</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>26</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="V2" s="38" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="W2" s="38" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="X2" s="3" t="s">
+        <v>614</v>
+      </c>
+      <c r="Y2" s="5" t="s">
         <v>615</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="Z2" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="AA2" s="5" t="s">
         <v>616</v>
-      </c>
-      <c r="Z2" s="5" t="s">
-        <v>531</v>
-      </c>
-      <c r="AA2" s="5" t="s">
-        <v>617</v>
       </c>
       <c r="AB2" s="5"/>
       <c r="AC2" s="3" t="s">
         <v>27</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="AE2" s="3" t="s">
         <v>28</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AG2" s="7" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="AH2" s="3" t="s">
         <v>29</v>
       </c>
       <c r="AI2" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="3" spans="1:35" ht="301" customHeight="1">
@@ -6932,62 +6932,62 @@
         <v>36</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="N3" s="10">
         <v>16</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="P3" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="R3" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S3" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T3" s="11" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="U3" s="11" t="s">
         <v>37</v>
       </c>
       <c r="V3" s="11" t="s">
+        <v>608</v>
+      </c>
+      <c r="W3" s="11" t="s">
+        <v>731</v>
+      </c>
+      <c r="X3" s="11" t="s">
         <v>609</v>
       </c>
-      <c r="W3" s="11" t="s">
-        <v>732</v>
-      </c>
-      <c r="X3" s="11" t="s">
+      <c r="Y3" s="11" t="s">
         <v>610</v>
       </c>
-      <c r="Y3" s="11" t="s">
+      <c r="Z3" s="11" t="s">
+        <v>857</v>
+      </c>
+      <c r="AA3" s="9" t="s">
         <v>611</v>
-      </c>
-      <c r="Z3" s="11" t="s">
-        <v>858</v>
-      </c>
-      <c r="AA3" s="9" t="s">
-        <v>612</v>
       </c>
       <c r="AB3" s="9"/>
       <c r="AC3" s="12" t="s">
+        <v>612</v>
+      </c>
+      <c r="AD3" s="12" t="s">
         <v>613</v>
       </c>
-      <c r="AD3" s="12" t="s">
-        <v>614</v>
-      </c>
       <c r="AE3" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="AF3" s="9" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="AG3" s="9" t="s">
         <v>38</v>
@@ -6996,7 +6996,7 @@
         <v>26</v>
       </c>
       <c r="AI3" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="4" spans="1:35" ht="310" customHeight="1">
@@ -7043,65 +7043,65 @@
         <v>9</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P4" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q4" s="9" t="s">
         <v>26</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="S4" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T4" s="11" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="U4" s="11" t="s">
         <v>46</v>
       </c>
       <c r="V4" s="11" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="W4" s="11" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="X4" s="11" t="s">
+        <v>619</v>
+      </c>
+      <c r="Y4" s="11" t="s">
         <v>620</v>
       </c>
-      <c r="Y4" s="11" t="s">
-        <v>621</v>
-      </c>
       <c r="Z4" s="11" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AA4" s="11" t="s">
         <v>26</v>
       </c>
       <c r="AB4" s="11"/>
       <c r="AC4" s="13" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="AD4" s="13" t="s">
         <v>47</v>
       </c>
       <c r="AE4" s="11" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="AF4" s="11" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="AG4" s="11" t="s">
+        <v>621</v>
+      </c>
+      <c r="AH4" s="11" t="s">
         <v>622</v>
       </c>
-      <c r="AH4" s="11" t="s">
-        <v>623</v>
-      </c>
       <c r="AI4" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="5" spans="1:35" ht="216" customHeight="1">
@@ -7115,7 +7115,7 @@
         <v>396</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>50</v>
@@ -7151,53 +7151,53 @@
         <v>398</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="R5" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S5" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T5" s="11" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="U5" s="9" t="s">
+        <v>623</v>
+      </c>
+      <c r="V5" s="11" t="s">
+        <v>608</v>
+      </c>
+      <c r="W5" s="11" t="s">
+        <v>731</v>
+      </c>
+      <c r="X5" s="9" t="s">
         <v>624</v>
       </c>
-      <c r="V5" s="11" t="s">
-        <v>609</v>
-      </c>
-      <c r="W5" s="11" t="s">
-        <v>732</v>
-      </c>
-      <c r="X5" s="9" t="s">
+      <c r="Y5" s="11" t="s">
         <v>625</v>
       </c>
-      <c r="Y5" s="11" t="s">
+      <c r="Z5" s="9" t="s">
+        <v>532</v>
+      </c>
+      <c r="AA5" s="11" t="s">
         <v>626</v>
-      </c>
-      <c r="Z5" s="9" t="s">
-        <v>533</v>
-      </c>
-      <c r="AA5" s="11" t="s">
-        <v>627</v>
       </c>
       <c r="AB5" s="11"/>
       <c r="AC5" s="11" t="s">
         <v>54</v>
       </c>
       <c r="AD5" s="11" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="AE5" s="11" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="AF5" s="11" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="AG5" s="11" t="s">
         <v>55</v>
@@ -7206,7 +7206,7 @@
         <v>56</v>
       </c>
       <c r="AI5" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="6" spans="1:35" ht="231" customHeight="1">
@@ -7241,7 +7241,7 @@
         <v>61</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="L6" s="11" t="s">
         <v>44</v>
@@ -7256,62 +7256,62 @@
         <v>399</v>
       </c>
       <c r="P6" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q6" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="R6" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S6" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T6" s="11" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="U6" s="9" t="s">
         <v>63</v>
       </c>
       <c r="V6" s="11" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="W6" s="11" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="X6" s="9" t="s">
+        <v>628</v>
+      </c>
+      <c r="Y6" s="9" t="s">
+        <v>479</v>
+      </c>
+      <c r="Z6" s="13" t="s">
         <v>629</v>
       </c>
-      <c r="Y6" s="9" t="s">
-        <v>480</v>
-      </c>
-      <c r="Z6" s="13" t="s">
+      <c r="AA6" s="11" t="s">
         <v>630</v>
-      </c>
-      <c r="AA6" s="11" t="s">
-        <v>631</v>
       </c>
       <c r="AB6" s="11"/>
       <c r="AC6" s="13" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="AD6" s="13" t="s">
         <v>248</v>
       </c>
       <c r="AE6" s="13" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="AF6" s="13" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="AG6" s="13" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="AH6" s="13" t="s">
         <v>26</v>
       </c>
       <c r="AI6" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="7" spans="1:35" ht="231" customHeight="1">
@@ -7325,7 +7325,7 @@
         <v>49</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>65</v>
@@ -7361,62 +7361,62 @@
         <v>72</v>
       </c>
       <c r="P7" s="11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q7" s="11" t="s">
         <v>26</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="S7" s="11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T7" s="11" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U7" s="9" t="s">
         <v>73</v>
       </c>
       <c r="V7" s="11" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="W7" s="11" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="X7" s="9" t="s">
+        <v>632</v>
+      </c>
+      <c r="Y7" s="11" t="s">
         <v>633</v>
       </c>
-      <c r="Y7" s="11" t="s">
+      <c r="Z7" s="9" t="s">
+        <v>545</v>
+      </c>
+      <c r="AA7" s="11" t="s">
         <v>634</v>
-      </c>
-      <c r="Z7" s="9" t="s">
-        <v>546</v>
-      </c>
-      <c r="AA7" s="11" t="s">
-        <v>635</v>
       </c>
       <c r="AB7" s="11"/>
       <c r="AC7" s="13" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="AD7" s="13" t="s">
+        <v>482</v>
+      </c>
+      <c r="AE7" s="13" t="s">
         <v>483</v>
       </c>
-      <c r="AE7" s="13" t="s">
-        <v>484</v>
-      </c>
       <c r="AF7" s="13" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="AG7" s="13" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="AH7" s="13" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="AI7" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="8" spans="1:35" ht="255" customHeight="1">
@@ -7466,62 +7466,62 @@
         <v>400</v>
       </c>
       <c r="P8" s="11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q8" s="11" t="s">
         <v>26</v>
       </c>
       <c r="R8" s="11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="S8" s="11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T8" s="11" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="U8" s="11" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="V8" s="11" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="W8" s="11" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="X8" s="11" t="s">
+        <v>636</v>
+      </c>
+      <c r="Y8" s="11" t="s">
         <v>637</v>
       </c>
-      <c r="Y8" s="11" t="s">
+      <c r="Z8" s="13" t="s">
+        <v>724</v>
+      </c>
+      <c r="AA8" s="11" t="s">
         <v>638</v>
-      </c>
-      <c r="Z8" s="13" t="s">
-        <v>725</v>
-      </c>
-      <c r="AA8" s="11" t="s">
-        <v>639</v>
       </c>
       <c r="AB8" s="11"/>
       <c r="AC8" s="13" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="AD8" s="13" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AE8" s="13" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="AF8" s="13" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="AG8" s="13" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AH8" s="13" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="AI8" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="9" spans="1:35" ht="226" customHeight="1">
@@ -7562,7 +7562,7 @@
         <v>88</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="N9" s="10">
         <v>10</v>
@@ -7571,28 +7571,28 @@
         <v>89</v>
       </c>
       <c r="P9" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q9" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="R9" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S9" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T9" s="11" t="s">
+        <v>714</v>
+      </c>
+      <c r="U9" s="9" t="s">
         <v>715</v>
       </c>
-      <c r="U9" s="9" t="s">
-        <v>716</v>
-      </c>
       <c r="V9" s="11" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="W9" s="11" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="X9" s="9" t="s">
         <v>90</v>
@@ -7601,32 +7601,32 @@
         <v>91</v>
       </c>
       <c r="Z9" s="11" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="AA9" s="11" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="AB9" s="11"/>
       <c r="AC9" s="13" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD9" s="13" t="s">
+        <v>473</v>
+      </c>
+      <c r="AE9" s="13" t="s">
+        <v>471</v>
+      </c>
+      <c r="AF9" s="13" t="s">
+        <v>553</v>
+      </c>
+      <c r="AG9" s="13" t="s">
+        <v>472</v>
+      </c>
+      <c r="AH9" s="13" t="s">
         <v>475</v>
       </c>
-      <c r="AD9" s="13" t="s">
-        <v>474</v>
-      </c>
-      <c r="AE9" s="13" t="s">
-        <v>472</v>
-      </c>
-      <c r="AF9" s="13" t="s">
-        <v>554</v>
-      </c>
-      <c r="AG9" s="13" t="s">
-        <v>473</v>
-      </c>
-      <c r="AH9" s="13" t="s">
-        <v>476</v>
-      </c>
       <c r="AI9" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="10" spans="1:35" ht="409.5" customHeight="1">
@@ -7673,65 +7673,65 @@
         <v>11</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="P10" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q10" s="9" t="s">
         <v>26</v>
       </c>
       <c r="R10" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="S10" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T10" s="9" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U10" s="9" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="V10" s="9" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="W10" s="9" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="X10" s="9" t="s">
+        <v>641</v>
+      </c>
+      <c r="Y10" s="11" t="s">
         <v>642</v>
       </c>
-      <c r="Y10" s="11" t="s">
+      <c r="Z10" s="9" t="s">
+        <v>533</v>
+      </c>
+      <c r="AA10" s="11" t="s">
         <v>643</v>
-      </c>
-      <c r="Z10" s="9" t="s">
-        <v>534</v>
-      </c>
-      <c r="AA10" s="11" t="s">
-        <v>644</v>
       </c>
       <c r="AB10" s="11"/>
       <c r="AC10" s="13" t="s">
+        <v>498</v>
+      </c>
+      <c r="AD10" s="13" t="s">
         <v>499</v>
       </c>
-      <c r="AD10" s="13" t="s">
-        <v>500</v>
-      </c>
       <c r="AE10" s="13" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="AF10" s="13" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="AG10" s="13" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="AH10" s="13" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="AI10" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="11" spans="1:35" ht="175" customHeight="1">
@@ -7793,25 +7793,25 @@
         <v>26</v>
       </c>
       <c r="T11" s="11" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="U11" s="9" t="s">
         <v>108</v>
       </c>
       <c r="V11" s="11" t="s">
+        <v>644</v>
+      </c>
+      <c r="W11" s="11" t="s">
+        <v>836</v>
+      </c>
+      <c r="X11" s="9" t="s">
         <v>645</v>
       </c>
-      <c r="W11" s="11" t="s">
-        <v>837</v>
-      </c>
-      <c r="X11" s="9" t="s">
-        <v>646</v>
-      </c>
       <c r="Y11" s="11" t="s">
         <v>26</v>
       </c>
       <c r="Z11" s="11" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="AA11" s="11" t="s">
         <v>26</v>
@@ -7827,16 +7827,16 @@
         <v>111</v>
       </c>
       <c r="AF11" s="11" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="AG11" s="11" t="s">
         <v>112</v>
       </c>
       <c r="AH11" s="11" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="AI11" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="12" spans="1:35" ht="171" customHeight="1">
@@ -7856,7 +7856,7 @@
         <v>114</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="G12" s="8">
         <v>2019</v>
@@ -7898,25 +7898,25 @@
         <v>26</v>
       </c>
       <c r="T12" s="11" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="U12" s="11" t="s">
         <v>118</v>
       </c>
       <c r="V12" s="11" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="W12" s="11" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="X12" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="Y12" s="11" t="s">
         <v>648</v>
       </c>
-      <c r="Y12" s="11" t="s">
-        <v>649</v>
-      </c>
       <c r="Z12" s="11" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="AA12" s="11" t="s">
         <v>26</v>
@@ -7926,22 +7926,22 @@
         <v>120</v>
       </c>
       <c r="AD12" s="11" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="AE12" s="11" t="s">
         <v>121</v>
       </c>
       <c r="AF12" s="11" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="AG12" s="11" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="AH12" s="11" t="s">
         <v>26</v>
       </c>
       <c r="AI12" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="13" spans="1:35" s="55" customFormat="1" ht="291" customHeight="1">
@@ -7979,7 +7979,7 @@
         <v>124</v>
       </c>
       <c r="L13" s="40" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="M13" s="40" t="s">
         <v>402</v>
@@ -7988,46 +7988,46 @@
         <v>18</v>
       </c>
       <c r="O13" s="53" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="P13" s="53" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q13" s="53" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="R13" s="53" t="s">
         <v>26</v>
       </c>
       <c r="S13" s="53" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T13" s="53" t="s">
         <v>311</v>
       </c>
       <c r="U13" s="53" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="V13" s="53" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="W13" s="53" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="X13" s="53" t="s">
+        <v>651</v>
+      </c>
+      <c r="Y13" s="53" t="s">
         <v>652</v>
       </c>
-      <c r="Y13" s="53" t="s">
-        <v>653</v>
-      </c>
       <c r="Z13" s="53" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="AA13" s="53" t="s">
         <v>125</v>
       </c>
       <c r="AB13" s="53" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="AC13" s="54"/>
       <c r="AD13" s="54"/>
@@ -8035,12 +8035,12 @@
         <v>28</v>
       </c>
       <c r="AF13" s="54" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="AG13" s="54"/>
       <c r="AH13" s="54"/>
       <c r="AI13" s="55" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="14" spans="1:35" ht="234" customHeight="1">
@@ -8066,7 +8066,7 @@
         <v>2016</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="I14" s="9" t="s">
         <v>129</v>
@@ -8087,31 +8087,31 @@
         <v>3</v>
       </c>
       <c r="O14" s="9" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="P14" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q14" s="9" t="s">
         <v>26</v>
       </c>
       <c r="R14" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="S14" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T14" s="11" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="U14" s="9" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="V14" s="11" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="W14" s="11" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="X14" s="9" t="s">
         <v>26</v>
@@ -8120,7 +8120,7 @@
         <v>26</v>
       </c>
       <c r="Z14" s="11" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AA14" s="11" t="s">
         <v>26</v>
@@ -8132,13 +8132,13 @@
         <v>134</v>
       </c>
       <c r="AD14" s="24" t="s">
+        <v>653</v>
+      </c>
+      <c r="AE14" s="24" t="s">
         <v>654</v>
       </c>
-      <c r="AE14" s="24" t="s">
+      <c r="AF14" s="24" t="s">
         <v>655</v>
-      </c>
-      <c r="AF14" s="24" t="s">
-        <v>656</v>
       </c>
       <c r="AG14" s="24" t="s">
         <v>135</v>
@@ -8147,7 +8147,7 @@
         <v>136</v>
       </c>
       <c r="AI14" s="47" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="15" spans="1:35" ht="267" customHeight="1">
@@ -8194,65 +8194,65 @@
         <v>10</v>
       </c>
       <c r="O15" s="9" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="P15" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q15" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="R15" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S15" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T15" s="11" t="s">
         <v>311</v>
       </c>
       <c r="U15" s="11" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="V15" s="11" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="W15" s="11" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="X15" s="11" t="s">
+        <v>657</v>
+      </c>
+      <c r="Y15" s="11" t="s">
         <v>658</v>
       </c>
-      <c r="Y15" s="11" t="s">
-        <v>659</v>
-      </c>
       <c r="Z15" s="11" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="AA15" s="11" t="s">
         <v>145</v>
       </c>
       <c r="AB15" s="11"/>
       <c r="AC15" s="13" t="s">
+        <v>464</v>
+      </c>
+      <c r="AD15" s="13" t="s">
         <v>465</v>
-      </c>
-      <c r="AD15" s="13" t="s">
-        <v>466</v>
       </c>
       <c r="AE15" s="13" t="s">
         <v>28</v>
       </c>
       <c r="AF15" s="13" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="AG15" s="13" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="AH15" s="13" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="AI15" s="47" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="16" spans="1:35" ht="224" customHeight="1">
@@ -8299,47 +8299,47 @@
         <v>8</v>
       </c>
       <c r="O16" s="11" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="P16" s="11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q16" s="11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="R16" s="11" t="s">
         <v>26</v>
       </c>
       <c r="S16" s="11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T16" s="11" t="s">
         <v>311</v>
       </c>
       <c r="U16" s="11" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V16" s="11" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="W16" s="11" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="X16" s="11" t="s">
+        <v>660</v>
+      </c>
+      <c r="Y16" s="11" t="s">
         <v>661</v>
       </c>
-      <c r="Y16" s="11" t="s">
+      <c r="Z16" s="11" t="s">
+        <v>538</v>
+      </c>
+      <c r="AA16" s="11" t="s">
         <v>662</v>
-      </c>
-      <c r="Z16" s="11" t="s">
-        <v>539</v>
-      </c>
-      <c r="AA16" s="11" t="s">
-        <v>663</v>
       </c>
       <c r="AB16" s="11"/>
       <c r="AC16" s="13" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="AD16" s="13" t="s">
         <v>226</v>
@@ -8348,16 +8348,16 @@
         <v>373</v>
       </c>
       <c r="AF16" s="13" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="AG16" s="13" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="AH16" s="13" t="s">
         <v>395</v>
       </c>
       <c r="AI16" s="47" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="17" spans="1:35" ht="291" customHeight="1">
@@ -8398,7 +8398,7 @@
         <v>88</v>
       </c>
       <c r="M17" s="9" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="N17" s="8">
         <v>8</v>
@@ -8407,62 +8407,62 @@
         <v>156</v>
       </c>
       <c r="P17" s="11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q17" s="11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="R17" s="11" t="s">
         <v>26</v>
       </c>
       <c r="S17" s="11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T17" s="11" t="s">
         <v>311</v>
       </c>
       <c r="U17" s="11" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="V17" s="11" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="W17" s="11" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="X17" s="11" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="Y17" s="11" t="s">
         <v>157</v>
       </c>
       <c r="Z17" s="11" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="AA17" s="11" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="AB17" s="11"/>
       <c r="AC17" s="13" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="AD17" s="13" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="AE17" s="13" t="s">
         <v>373</v>
       </c>
       <c r="AF17" s="13" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="AG17" s="13" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="AH17" s="29" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="AI17" s="47" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="18" spans="1:35" ht="199" customHeight="1">
@@ -8509,46 +8509,46 @@
         <v>16</v>
       </c>
       <c r="O18" s="53" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="P18" s="53" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q18" s="53" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="R18" s="53" t="s">
         <v>26</v>
       </c>
       <c r="S18" s="53" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T18" s="53" t="s">
         <v>311</v>
       </c>
       <c r="U18" s="53" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="V18" s="53" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="W18" s="53" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="X18" s="53" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Y18" s="52" t="s">
         <v>392</v>
       </c>
       <c r="Z18" s="53" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="AA18" s="53" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="AB18" s="53" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="AC18" s="54"/>
       <c r="AD18" s="54"/>
@@ -8556,12 +8556,12 @@
         <v>28</v>
       </c>
       <c r="AF18" s="54" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="AG18" s="54"/>
       <c r="AH18" s="54"/>
       <c r="AI18" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="19" spans="1:35" ht="220" customHeight="1">
@@ -8599,7 +8599,7 @@
         <v>168</v>
       </c>
       <c r="L19" s="53" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="M19" s="53" t="s">
         <v>169</v>
@@ -8611,56 +8611,56 @@
         <v>404</v>
       </c>
       <c r="P19" s="53" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q19" s="53" t="s">
         <v>26</v>
       </c>
       <c r="R19" s="53" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="S19" s="53" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T19" s="53" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U19" s="53" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="V19" s="53" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="W19" s="53" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="X19" s="53" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="Y19" s="52" t="s">
+        <v>741</v>
+      </c>
+      <c r="Z19" s="53" t="s">
+        <v>751</v>
+      </c>
+      <c r="AA19" s="53" t="s">
+        <v>842</v>
+      </c>
+      <c r="AB19" s="53" t="s">
         <v>742</v>
-      </c>
-      <c r="Z19" s="53" t="s">
-        <v>752</v>
-      </c>
-      <c r="AA19" s="53" t="s">
-        <v>843</v>
-      </c>
-      <c r="AB19" s="53" t="s">
-        <v>743</v>
       </c>
       <c r="AC19" s="54"/>
       <c r="AD19" s="54"/>
       <c r="AE19" s="54" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="AF19" s="54" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="AG19" s="54"/>
       <c r="AH19" s="54"/>
       <c r="AI19" s="55" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="20" spans="1:35" ht="408" customHeight="1">
@@ -8707,65 +8707,65 @@
         <v>10</v>
       </c>
       <c r="O20" s="50" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="P20" s="11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q20" s="11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="R20" s="11" t="s">
         <v>26</v>
       </c>
       <c r="S20" s="11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T20" s="11" t="s">
         <v>311</v>
       </c>
       <c r="U20" s="9" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="V20" s="11" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="W20" s="11" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="X20" s="9" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="Y20" s="11" t="s">
         <v>178</v>
       </c>
       <c r="Z20" s="11" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="AA20" s="11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AB20" s="11"/>
       <c r="AC20" s="13" t="s">
+        <v>491</v>
+      </c>
+      <c r="AD20" s="13" t="s">
         <v>492</v>
       </c>
-      <c r="AD20" s="13" t="s">
-        <v>493</v>
-      </c>
       <c r="AE20" s="13" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="AF20" s="13" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="AG20" s="13" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="AH20" s="13" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="AI20" s="47" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="21" spans="1:35" ht="198" customHeight="1">
@@ -8791,7 +8791,7 @@
         <v>2015</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="I21" s="11" t="s">
         <v>21</v>
@@ -8812,31 +8812,31 @@
         <v>8</v>
       </c>
       <c r="O21" s="11" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="P21" s="11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q21" s="11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="R21" s="11" t="s">
         <v>26</v>
       </c>
       <c r="S21" s="11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T21" s="11" t="s">
         <v>311</v>
       </c>
       <c r="U21" s="11" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="V21" s="11" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="W21" s="11" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="X21" s="11" t="s">
         <v>26</v>
@@ -8845,32 +8845,32 @@
         <v>26</v>
       </c>
       <c r="Z21" s="13" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="AA21" s="11" t="s">
         <v>26</v>
       </c>
       <c r="AB21" s="11"/>
       <c r="AC21" s="13" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="AD21" s="13" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="AE21" s="13" t="s">
         <v>369</v>
       </c>
       <c r="AF21" s="13" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="AG21" s="13" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="AH21" s="13" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="AI21" s="47" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="22" spans="1:35" ht="272" customHeight="1">
@@ -8911,7 +8911,7 @@
         <v>143</v>
       </c>
       <c r="M22" s="11" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="N22" s="8">
         <v>8</v>
@@ -8920,37 +8920,37 @@
         <v>405</v>
       </c>
       <c r="P22" s="11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q22" s="11" t="s">
         <v>26</v>
       </c>
       <c r="R22" s="11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="S22" s="11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T22" s="13" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U22" s="13" t="s">
         <v>391</v>
       </c>
       <c r="V22" s="13" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="W22" s="13" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="X22" s="13" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="Y22" s="11" t="s">
         <v>392</v>
       </c>
       <c r="Z22" s="13" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="AA22" s="11" t="s">
         <v>26</v>
@@ -8966,7 +8966,7 @@
         <v>297</v>
       </c>
       <c r="AF22" s="13" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AG22" s="13" t="s">
         <v>394</v>
@@ -8975,7 +8975,7 @@
         <v>390</v>
       </c>
       <c r="AI22" s="47" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="23" spans="1:35" ht="250" customHeight="1">
@@ -9016,7 +9016,7 @@
         <v>143</v>
       </c>
       <c r="M23" s="11" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="N23" s="8">
         <v>10</v>
@@ -9025,28 +9025,28 @@
         <v>195</v>
       </c>
       <c r="P23" s="11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q23" s="11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="R23" s="11" t="s">
         <v>26</v>
       </c>
       <c r="S23" s="11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T23" s="22" t="s">
         <v>311</v>
       </c>
       <c r="U23" s="11" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="V23" s="22" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="W23" s="22" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="X23" s="11" t="s">
         <v>196</v>
@@ -9055,32 +9055,32 @@
         <v>392</v>
       </c>
       <c r="Z23" s="13" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="AA23" s="13" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="AB23" s="13"/>
       <c r="AC23" s="13" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="AD23" s="13" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="AE23" s="13" t="s">
         <v>291</v>
       </c>
       <c r="AF23" s="13" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="AG23" s="13" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="AH23" s="13" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="AI23" s="47" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="24" spans="1:35" ht="217" customHeight="1">
@@ -9142,16 +9142,16 @@
         <v>26</v>
       </c>
       <c r="T24" s="11" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="U24" s="11" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="V24" s="11" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="W24" s="11" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="X24" s="11" t="s">
         <v>26</v>
@@ -9173,10 +9173,10 @@
         <v>205</v>
       </c>
       <c r="AE24" s="11" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="AF24" s="11" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="AG24" s="11" t="s">
         <v>206</v>
@@ -9185,7 +9185,7 @@
         <v>26</v>
       </c>
       <c r="AI24" s="47" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="25" spans="1:35" ht="231" customHeight="1">
@@ -9232,40 +9232,40 @@
         <v>4</v>
       </c>
       <c r="O25" s="9" t="s">
+        <v>591</v>
+      </c>
+      <c r="P25" s="9" t="s">
+        <v>605</v>
+      </c>
+      <c r="Q25" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="R25" s="9" t="s">
+        <v>605</v>
+      </c>
+      <c r="S25" s="9" t="s">
+        <v>605</v>
+      </c>
+      <c r="T25" s="11" t="s">
+        <v>686</v>
+      </c>
+      <c r="U25" s="11" t="s">
         <v>592</v>
       </c>
-      <c r="P25" s="9" t="s">
-        <v>606</v>
-      </c>
-      <c r="Q25" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="R25" s="9" t="s">
-        <v>606</v>
-      </c>
-      <c r="S25" s="9" t="s">
-        <v>606</v>
-      </c>
-      <c r="T25" s="11" t="s">
-        <v>687</v>
-      </c>
-      <c r="U25" s="11" t="s">
-        <v>593</v>
-      </c>
       <c r="V25" s="11" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="W25" s="11" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="X25" s="11" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="Y25" s="11" t="s">
         <v>26</v>
       </c>
       <c r="Z25" s="9" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="AA25" s="11" t="s">
         <v>26</v>
@@ -9281,7 +9281,7 @@
         <v>373</v>
       </c>
       <c r="AF25" s="11" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="AG25" s="11" t="s">
         <v>216</v>
@@ -9290,7 +9290,7 @@
         <v>26</v>
       </c>
       <c r="AI25" s="47" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="26" spans="1:35" ht="301" customHeight="1">
@@ -9331,7 +9331,7 @@
         <v>24</v>
       </c>
       <c r="M26" s="9" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="N26" s="10">
         <v>8</v>
@@ -9340,28 +9340,28 @@
         <v>411</v>
       </c>
       <c r="P26" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q26" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="R26" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S26" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T26" s="11" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="U26" s="11" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="V26" s="11" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="W26" s="11" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="X26" s="11" t="s">
         <v>223</v>
@@ -9370,7 +9370,7 @@
         <v>224</v>
       </c>
       <c r="Z26" s="9" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="AA26" s="11" t="s">
         <v>223</v>
@@ -9386,7 +9386,7 @@
         <v>373</v>
       </c>
       <c r="AF26" s="11" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="AG26" s="11" t="s">
         <v>227</v>
@@ -9395,7 +9395,7 @@
         <v>228</v>
       </c>
       <c r="AI26" s="47" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="27" spans="1:35" ht="223" customHeight="1">
@@ -9442,7 +9442,7 @@
         <v>4</v>
       </c>
       <c r="O27" s="9" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="P27" s="9" t="s">
         <v>26</v>
@@ -9457,16 +9457,16 @@
         <v>26</v>
       </c>
       <c r="T27" s="11" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="U27" s="11" t="s">
         <v>233</v>
       </c>
       <c r="V27" s="11" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="W27" s="11" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="X27" s="11" t="s">
         <v>26</v>
@@ -9475,7 +9475,7 @@
         <v>26</v>
       </c>
       <c r="Z27" s="9" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="AA27" s="11" t="s">
         <v>26</v>
@@ -9491,7 +9491,7 @@
         <v>369</v>
       </c>
       <c r="AF27" s="11" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="AG27" s="11" t="s">
         <v>236</v>
@@ -9500,7 +9500,7 @@
         <v>237</v>
       </c>
       <c r="AI27" s="47" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="28" spans="1:35" ht="187" customHeight="1">
@@ -9541,7 +9541,7 @@
         <v>243</v>
       </c>
       <c r="M28" s="9" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="N28" s="10">
         <v>13</v>
@@ -9550,28 +9550,28 @@
         <v>413</v>
       </c>
       <c r="P28" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q28" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="R28" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S28" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T28" s="11" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="U28" s="11" t="s">
         <v>244</v>
       </c>
       <c r="V28" s="11" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="W28" s="11" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="X28" s="11" t="s">
         <v>245</v>
@@ -9580,7 +9580,7 @@
         <v>26</v>
       </c>
       <c r="Z28" s="9" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="AA28" s="11" t="s">
         <v>246</v>
@@ -9596,7 +9596,7 @@
         <v>28</v>
       </c>
       <c r="AF28" s="11" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="AG28" s="11" t="s">
         <v>249</v>
@@ -9605,7 +9605,7 @@
         <v>250</v>
       </c>
       <c r="AI28" s="47" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="29" spans="1:35" ht="195" customHeight="1">
@@ -9655,37 +9655,37 @@
         <v>407</v>
       </c>
       <c r="P29" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q29" s="9" t="s">
         <v>26</v>
       </c>
       <c r="R29" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="S29" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T29" s="11" t="s">
         <v>311</v>
       </c>
       <c r="U29" s="11" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="V29" s="11" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="W29" s="11" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="X29" s="11" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="Y29" s="11" t="s">
         <v>259</v>
       </c>
       <c r="Z29" s="9" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="AA29" s="11" t="s">
         <v>26</v>
@@ -9701,7 +9701,7 @@
         <v>28</v>
       </c>
       <c r="AF29" s="11" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="AG29" s="11" t="s">
         <v>262</v>
@@ -9710,7 +9710,7 @@
         <v>263</v>
       </c>
       <c r="AI29" s="47" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="30" spans="1:35" ht="317" customHeight="1">
@@ -9760,16 +9760,16 @@
         <v>408</v>
       </c>
       <c r="P30" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q30" s="9" t="s">
         <v>26</v>
       </c>
       <c r="R30" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="S30" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T30" s="11" t="s">
         <v>311</v>
@@ -9778,13 +9778,13 @@
         <v>269</v>
       </c>
       <c r="V30" s="11" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="W30" s="11" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="X30" s="11" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="Y30" s="11" t="s">
         <v>26</v>
@@ -9806,7 +9806,7 @@
         <v>28</v>
       </c>
       <c r="AF30" s="13" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="AG30" s="13" t="s">
         <v>389</v>
@@ -9815,7 +9815,7 @@
         <v>386</v>
       </c>
       <c r="AI30" s="47" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="31" spans="1:35" s="55" customFormat="1" ht="238" customHeight="1">
@@ -9865,16 +9865,16 @@
         <v>415</v>
       </c>
       <c r="P31" s="52" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q31" s="52" t="s">
         <v>26</v>
       </c>
       <c r="R31" s="52" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="S31" s="52" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T31" s="53" t="s">
         <v>311</v>
@@ -9883,25 +9883,25 @@
         <v>274</v>
       </c>
       <c r="V31" s="53" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="W31" s="53" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="X31" s="53" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="Y31" s="53" t="s">
         <v>392</v>
       </c>
       <c r="Z31" s="54" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="AA31" s="54" t="s">
         <v>26</v>
       </c>
       <c r="AB31" s="54" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="AC31" s="54"/>
       <c r="AD31" s="54"/>
@@ -9910,7 +9910,7 @@
       <c r="AG31" s="54"/>
       <c r="AH31" s="54"/>
       <c r="AI31" s="55" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="32" spans="1:35" ht="226" customHeight="1">
@@ -9945,7 +9945,7 @@
         <v>417</v>
       </c>
       <c r="K32" s="26" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="L32" s="11" t="s">
         <v>24</v>
@@ -9972,16 +9972,16 @@
         <v>26</v>
       </c>
       <c r="T32" s="11" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="U32" s="11" t="s">
         <v>278</v>
       </c>
       <c r="V32" s="11" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="W32" s="11" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="X32" s="11" t="s">
         <v>279</v>
@@ -9990,7 +9990,7 @@
         <v>26</v>
       </c>
       <c r="Z32" s="9" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="AA32" s="11" t="s">
         <v>420</v>
@@ -10006,7 +10006,7 @@
         <v>282</v>
       </c>
       <c r="AF32" s="11" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="AG32" s="11" t="s">
         <v>283</v>
@@ -10015,7 +10015,7 @@
         <v>26</v>
       </c>
       <c r="AI32" s="47" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="33" spans="1:35" ht="274" customHeight="1">
@@ -10065,16 +10065,16 @@
         <v>423</v>
       </c>
       <c r="P33" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q33" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="R33" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S33" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T33" s="11" t="s">
         <v>288</v>
@@ -10083,10 +10083,10 @@
         <v>288</v>
       </c>
       <c r="V33" s="11" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="W33" s="11" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="X33" s="11" t="s">
         <v>26</v>
@@ -10111,16 +10111,16 @@
         <v>291</v>
       </c>
       <c r="AF33" s="11" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="AG33" s="11" t="s">
         <v>292</v>
       </c>
       <c r="AH33" s="11" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="AI33" s="47" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="34" spans="1:35" ht="235" customHeight="1">
@@ -10146,7 +10146,7 @@
         <v>2016</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="I34" s="26" t="s">
         <v>166</v>
@@ -10155,7 +10155,7 @@
         <v>424</v>
       </c>
       <c r="K34" s="26" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="L34" s="11" t="s">
         <v>24</v>
@@ -10167,31 +10167,31 @@
         <v>8</v>
       </c>
       <c r="O34" s="9" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="P34" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q34" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="R34" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S34" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T34" s="11" t="s">
         <v>311</v>
       </c>
       <c r="U34" s="11" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="V34" s="11" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="W34" s="11" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="X34" s="11" t="s">
         <v>26</v>
@@ -10200,7 +10200,7 @@
         <v>26</v>
       </c>
       <c r="Z34" s="11" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="AA34" s="11" t="s">
         <v>26</v>
@@ -10216,7 +10216,7 @@
         <v>297</v>
       </c>
       <c r="AF34" s="11" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="AG34" s="11" t="s">
         <v>298</v>
@@ -10225,7 +10225,7 @@
         <v>26</v>
       </c>
       <c r="AI34" s="47" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="35" spans="1:35" ht="270" customHeight="1">
@@ -10251,7 +10251,7 @@
         <v>2016</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I35" s="26" t="s">
         <v>21</v>
@@ -10272,31 +10272,31 @@
         <v>8</v>
       </c>
       <c r="O35" s="9" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="P35" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q35" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="R35" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S35" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T35" s="11" t="s">
         <v>311</v>
       </c>
       <c r="U35" s="11" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="V35" s="11" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="W35" s="11" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="X35" s="11" t="s">
         <v>26</v>
@@ -10321,7 +10321,7 @@
         <v>291</v>
       </c>
       <c r="AF35" s="13" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="AG35" s="13" t="s">
         <v>377</v>
@@ -10330,7 +10330,7 @@
         <v>379</v>
       </c>
       <c r="AI35" s="47" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="36" spans="1:35" ht="202" customHeight="1">
@@ -10347,7 +10347,7 @@
         <v>2017</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="F36" s="28" t="s">
         <v>304</v>
@@ -10380,28 +10380,28 @@
         <v>310</v>
       </c>
       <c r="P36" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q36" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="R36" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S36" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T36" s="11" t="s">
         <v>311</v>
       </c>
       <c r="U36" s="11" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="V36" s="11" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="W36" s="11" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="X36" s="11" t="s">
         <v>26</v>
@@ -10417,25 +10417,25 @@
       </c>
       <c r="AB36" s="11"/>
       <c r="AC36" s="13" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="AD36" s="13" t="s">
+        <v>486</v>
+      </c>
+      <c r="AE36" s="13" t="s">
+        <v>488</v>
+      </c>
+      <c r="AF36" s="13" t="s">
+        <v>573</v>
+      </c>
+      <c r="AG36" s="13" t="s">
         <v>487</v>
       </c>
-      <c r="AE36" s="13" t="s">
-        <v>489</v>
-      </c>
-      <c r="AF36" s="13" t="s">
-        <v>574</v>
-      </c>
-      <c r="AG36" s="13" t="s">
-        <v>488</v>
-      </c>
       <c r="AH36" s="30" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="AI36" s="47" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="37" spans="1:35" s="55" customFormat="1" ht="225" customHeight="1">
@@ -10461,7 +10461,7 @@
         <v>2015</v>
       </c>
       <c r="H37" s="9" t="s">
-        <v>427</v>
+        <v>861</v>
       </c>
       <c r="I37" s="26" t="s">
         <v>34</v>
@@ -10476,52 +10476,52 @@
         <v>308</v>
       </c>
       <c r="M37" s="9" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="N37" s="10">
         <v>17</v>
       </c>
       <c r="O37" s="52" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="P37" s="52" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q37" s="52" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="R37" s="52" t="s">
         <v>26</v>
       </c>
       <c r="S37" s="52" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T37" s="53" t="s">
         <v>311</v>
       </c>
       <c r="U37" s="53" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="V37" s="53" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="W37" s="53" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="X37" s="53" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Y37" s="54" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Z37" s="54" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="AA37" s="54" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="AB37" s="54" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="AC37" s="54"/>
       <c r="AD37" s="54"/>
@@ -10529,12 +10529,12 @@
         <v>28</v>
       </c>
       <c r="AF37" s="54" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="AG37" s="54"/>
       <c r="AH37" s="54"/>
       <c r="AI37" s="55" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="38" spans="1:35" ht="270" customHeight="1">
@@ -10551,7 +10551,7 @@
         <v>2018</v>
       </c>
       <c r="E38" s="52" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F38" s="52" t="s">
         <v>316</v>
@@ -10560,7 +10560,7 @@
         <v>2018</v>
       </c>
       <c r="H38" s="52" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="I38" s="59" t="s">
         <v>21</v>
@@ -10575,50 +10575,50 @@
         <v>88</v>
       </c>
       <c r="M38" s="52" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="N38" s="60">
         <v>27</v>
       </c>
       <c r="O38" s="52" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="P38" s="52" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q38" s="52" t="s">
         <v>26</v>
       </c>
       <c r="R38" s="52" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="S38" s="52" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T38" s="53" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="U38" s="54"/>
       <c r="V38" s="53" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="W38" s="53" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="X38" s="54" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="Y38" s="54" t="s">
         <v>392</v>
       </c>
       <c r="Z38" s="54" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="AA38" s="54" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="AB38" s="54" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="AC38" s="54"/>
       <c r="AD38" s="54"/>
@@ -10626,12 +10626,12 @@
         <v>28</v>
       </c>
       <c r="AF38" s="54" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="AG38" s="54"/>
       <c r="AH38" s="54"/>
       <c r="AI38" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="39" spans="1:35" ht="243" customHeight="1">
@@ -10657,7 +10657,7 @@
         <v>2019</v>
       </c>
       <c r="H39" s="9" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="I39" s="9" t="s">
         <v>21</v>
@@ -10672,37 +10672,37 @@
         <v>257</v>
       </c>
       <c r="M39" s="9" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="N39" s="10">
         <v>11</v>
       </c>
       <c r="O39" s="9" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="P39" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q39" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="R39" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S39" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T39" s="11" t="s">
         <v>288</v>
       </c>
       <c r="U39" s="13" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="V39" s="11" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="W39" s="11" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="X39" s="13" t="s">
         <v>26</v>
@@ -10718,25 +10718,25 @@
       </c>
       <c r="AB39" s="13"/>
       <c r="AC39" s="13" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="AD39" s="13" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="AE39" s="13" t="s">
         <v>369</v>
       </c>
       <c r="AF39" s="13" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="AG39" s="13" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="AH39" s="13" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="AI39" s="47" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="40" spans="1:35" ht="220" customHeight="1">
@@ -10756,7 +10756,7 @@
         <v>325</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G40" s="8">
         <v>2017</v>
@@ -10768,22 +10768,22 @@
         <v>21</v>
       </c>
       <c r="J40" s="9" t="s">
+        <v>431</v>
+      </c>
+      <c r="K40" s="9" t="s">
         <v>432</v>
-      </c>
-      <c r="K40" s="9" t="s">
-        <v>433</v>
       </c>
       <c r="L40" s="11" t="s">
         <v>88</v>
       </c>
       <c r="M40" s="9" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="N40" s="10">
         <v>5</v>
       </c>
       <c r="O40" s="9" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="P40" s="9" t="s">
         <v>26</v>
@@ -10798,16 +10798,16 @@
         <v>26</v>
       </c>
       <c r="T40" s="11" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="U40" s="11" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="V40" s="11" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="W40" s="11" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="X40" s="13" t="s">
         <v>26</v>
@@ -10816,7 +10816,7 @@
         <v>26</v>
       </c>
       <c r="Z40" s="13" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="AA40" s="13" t="s">
         <v>26</v>
@@ -10832,7 +10832,7 @@
         <v>369</v>
       </c>
       <c r="AF40" s="13" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="AG40" s="13" t="s">
         <v>367</v>
@@ -10841,7 +10841,7 @@
         <v>368</v>
       </c>
       <c r="AI40" s="47" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="41" spans="1:35" ht="227" customHeight="1">
@@ -10867,7 +10867,7 @@
         <v>2012</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="I41" s="9" t="s">
         <v>34</v>
@@ -10888,65 +10888,65 @@
         <v>9</v>
       </c>
       <c r="O41" s="9" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="P41" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q41" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="R41" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S41" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T41" s="11" t="s">
         <v>311</v>
       </c>
       <c r="U41" s="11" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="V41" s="11" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="W41" s="11" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="X41" s="11" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="Y41" s="13" t="s">
         <v>26</v>
       </c>
       <c r="Z41" s="13" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="AA41" s="13" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="AB41" s="13"/>
       <c r="AC41" s="13" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="AD41" s="13" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="AE41" s="13" t="s">
         <v>369</v>
       </c>
       <c r="AF41" s="13" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="AG41" s="13" t="s">
+        <v>454</v>
+      </c>
+      <c r="AH41" s="13" t="s">
         <v>455</v>
       </c>
-      <c r="AH41" s="13" t="s">
-        <v>456</v>
-      </c>
       <c r="AI41" s="47" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="42" spans="1:35" ht="205" customHeight="1">
@@ -10972,28 +10972,28 @@
         <v>2018</v>
       </c>
       <c r="H42" s="41" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="I42" s="41" t="s">
         <v>334</v>
       </c>
       <c r="J42" s="41" t="s">
+        <v>435</v>
+      </c>
+      <c r="K42" s="41" t="s">
         <v>436</v>
-      </c>
-      <c r="K42" s="41" t="s">
-        <v>437</v>
       </c>
       <c r="L42" s="40" t="s">
         <v>335</v>
       </c>
       <c r="M42" s="41" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="N42" s="42">
         <v>13</v>
       </c>
       <c r="O42" s="52" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="P42" s="52" t="s">
         <v>26</v>
@@ -11014,13 +11014,13 @@
         <v>311</v>
       </c>
       <c r="V42" s="53" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="W42" s="53" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="X42" s="53" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="Y42" s="54" t="s">
         <v>26</v>
@@ -11040,12 +11040,12 @@
         <v>282</v>
       </c>
       <c r="AF42" s="54" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="AG42" s="54"/>
       <c r="AH42" s="54"/>
       <c r="AI42" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="43" spans="1:35" ht="276" customHeight="1">
@@ -11071,7 +11071,7 @@
         <v>2019</v>
       </c>
       <c r="H43" s="9" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="I43" s="9" t="s">
         <v>21</v>
@@ -11092,40 +11092,40 @@
         <v>5</v>
       </c>
       <c r="O43" s="9" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="P43" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q43" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="R43" s="9" t="s">
         <v>26</v>
       </c>
       <c r="S43" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T43" s="11" t="s">
         <v>311</v>
       </c>
       <c r="U43" s="11" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="V43" s="11" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="W43" s="11" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="X43" s="11" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="Y43" s="11" t="s">
         <v>26</v>
       </c>
       <c r="Z43" s="9" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="AA43" s="11" t="s">
         <v>26</v>
@@ -11141,7 +11141,7 @@
         <v>373</v>
       </c>
       <c r="AF43" s="13" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="AG43" s="13" t="s">
         <v>374</v>
@@ -11150,7 +11150,7 @@
         <v>375</v>
       </c>
       <c r="AI43" s="47" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="44" spans="1:35" ht="231" customHeight="1">
@@ -11185,7 +11185,7 @@
         <v>344</v>
       </c>
       <c r="K44" s="9" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="L44" s="11" t="s">
         <v>88</v>
@@ -11197,31 +11197,31 @@
         <v>10</v>
       </c>
       <c r="O44" s="9" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="P44" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q44" s="9" t="s">
         <v>26</v>
       </c>
       <c r="R44" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="S44" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T44" s="11" t="s">
         <v>311</v>
       </c>
       <c r="U44" s="11" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="V44" s="11" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="W44" s="11" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="X44" s="11" t="s">
         <v>26</v>
@@ -11230,32 +11230,32 @@
         <v>26</v>
       </c>
       <c r="Z44" s="13" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="AA44" s="11" t="s">
         <v>26</v>
       </c>
       <c r="AB44" s="11"/>
       <c r="AC44" s="13" t="s">
+        <v>467</v>
+      </c>
+      <c r="AD44" s="13" t="s">
+        <v>470</v>
+      </c>
+      <c r="AE44" s="13" t="s">
         <v>468</v>
       </c>
-      <c r="AD44" s="13" t="s">
-        <v>471</v>
-      </c>
-      <c r="AE44" s="13" t="s">
+      <c r="AF44" s="13" t="s">
+        <v>578</v>
+      </c>
+      <c r="AG44" s="13" t="s">
         <v>469</v>
       </c>
-      <c r="AF44" s="13" t="s">
-        <v>579</v>
-      </c>
-      <c r="AG44" s="13" t="s">
-        <v>470</v>
-      </c>
       <c r="AH44" s="13" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AI44" s="47" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="45" spans="1:35" ht="268" customHeight="1">
@@ -11272,25 +11272,25 @@
         <v>2018</v>
       </c>
       <c r="E45" s="36" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F45" s="33" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="G45" s="21">
         <v>2018</v>
       </c>
       <c r="H45" s="9" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="I45" s="9" t="s">
         <v>21</v>
       </c>
       <c r="J45" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="K45" s="9" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="L45" s="11" t="s">
         <v>24</v>
@@ -11302,65 +11302,65 @@
         <v>9</v>
       </c>
       <c r="O45" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="P45" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q45" s="9" t="s">
         <v>26</v>
       </c>
       <c r="R45" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="S45" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T45" s="11" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="U45" s="11" t="s">
         <v>288</v>
       </c>
       <c r="V45" s="11" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="W45" s="11" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="X45" s="11" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="Y45" s="11" t="s">
         <v>26</v>
       </c>
       <c r="Z45" s="9" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="AA45" s="13" t="s">
         <v>26</v>
       </c>
       <c r="AB45" s="13"/>
       <c r="AC45" s="13" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="AD45" s="13" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="AE45" s="13" t="s">
         <v>369</v>
       </c>
       <c r="AF45" s="13" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="AG45" s="13" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="AH45" s="13" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="AI45" s="47" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="46" spans="1:35" ht="159" customHeight="1">
@@ -11422,16 +11422,16 @@
         <v>26</v>
       </c>
       <c r="T46" s="11" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="U46" s="11" t="s">
         <v>355</v>
       </c>
       <c r="V46" s="11" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="W46" s="11" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="X46" s="11" t="s">
         <v>26</v>
@@ -11447,16 +11447,16 @@
       </c>
       <c r="AB46" s="11"/>
       <c r="AC46" s="11" t="s">
+        <v>677</v>
+      </c>
+      <c r="AD46" s="11" t="s">
         <v>678</v>
-      </c>
-      <c r="AD46" s="11" t="s">
-        <v>679</v>
       </c>
       <c r="AE46" s="11" t="s">
         <v>356</v>
       </c>
       <c r="AF46" s="11" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="AG46" s="11" t="s">
         <v>357</v>
@@ -11465,7 +11465,7 @@
         <v>358</v>
       </c>
       <c r="AI46" s="47" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="47" spans="1:35" s="55" customFormat="1" ht="283" customHeight="1">
@@ -11512,34 +11512,34 @@
         <v>18</v>
       </c>
       <c r="O47" s="62" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="P47" s="62" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q47" s="62" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="R47" s="62" t="s">
         <v>26</v>
       </c>
       <c r="S47" s="62" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T47" s="69" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="U47" s="67" t="s">
         <v>311</v>
       </c>
       <c r="V47" s="69" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="W47" s="69" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="X47" s="67" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="Y47" s="69" t="s">
         <v>26</v>
@@ -11548,21 +11548,21 @@
         <v>26</v>
       </c>
       <c r="AA47" s="69" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="AB47" s="69" t="s">
         <v>26</v>
       </c>
       <c r="AC47" s="69"/>
       <c r="AD47" s="69" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="AE47" s="69"/>
       <c r="AF47" s="69"/>
       <c r="AG47" s="69"/>
       <c r="AH47" s="69"/>
       <c r="AI47" s="55" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="48" spans="1:35" ht="46" customHeight="1">
@@ -11570,29 +11570,29 @@
         <v>106</v>
       </c>
       <c r="B48" s="71" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="C48" s="72"/>
       <c r="D48" s="70">
         <v>2020</v>
       </c>
       <c r="E48" s="73" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="F48" s="74" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="G48" s="72">
         <v>2020</v>
       </c>
       <c r="H48" s="75" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="I48" s="72" t="s">
         <v>21</v>
       </c>
       <c r="J48" s="72" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="K48" s="72" t="s">
         <v>268</v>
@@ -11601,41 +11601,41 @@
         <v>143</v>
       </c>
       <c r="M48" s="72" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="N48" s="72">
         <v>17</v>
       </c>
       <c r="O48" s="72"/>
       <c r="P48" s="72" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q48" s="72" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="R48" s="72" t="s">
         <v>26</v>
       </c>
       <c r="S48" s="72" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T48" s="76" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="U48" s="72" t="s">
         <v>355</v>
       </c>
       <c r="V48" s="72" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="W48" s="72" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="X48" s="72" t="s">
         <v>26</v>
       </c>
       <c r="Y48" s="72" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Z48" s="72" t="s">
         <v>26</v>
@@ -11663,7 +11663,7 @@
         <v>49</v>
       </c>
       <c r="AI48" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="49" spans="1:35" ht="145" customHeight="1">
@@ -11671,23 +11671,23 @@
         <v>107</v>
       </c>
       <c r="B49" s="72" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="C49" s="72"/>
       <c r="D49" s="72">
         <v>2020</v>
       </c>
       <c r="E49" s="73" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="F49" s="74" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="G49" s="72">
         <v>2020</v>
       </c>
       <c r="H49" s="75" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="I49" s="72" t="s">
         <v>21</v>
@@ -11702,13 +11702,13 @@
         <v>24</v>
       </c>
       <c r="M49" s="72" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="N49" s="72">
         <v>2</v>
       </c>
       <c r="O49" s="72" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="P49" s="72" t="s">
         <v>26</v>
@@ -11724,28 +11724,28 @@
       </c>
       <c r="T49" s="72"/>
       <c r="U49" s="76" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="V49" s="72" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="W49" s="72" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="X49" s="72" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Y49" s="72" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Z49" s="72" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="AA49" s="72" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="AB49" s="72" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="AC49" s="72" t="s">
         <v>49</v>
@@ -11766,7 +11766,7 @@
         <v>26</v>
       </c>
       <c r="AI49" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="50" spans="1:35" ht="68" customHeight="1">
@@ -11774,75 +11774,75 @@
         <v>108</v>
       </c>
       <c r="B50" s="72" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="C50" s="72"/>
       <c r="D50" s="72">
         <v>2020</v>
       </c>
       <c r="E50" s="73" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="F50" s="74" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="G50" s="72">
         <v>2020</v>
       </c>
       <c r="H50" s="75" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="I50" s="72" t="s">
         <v>129</v>
       </c>
       <c r="J50" s="72" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="K50" s="72" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="L50" s="72" t="s">
         <v>176</v>
       </c>
       <c r="M50" s="72" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="N50" s="72">
         <v>9</v>
       </c>
       <c r="O50" s="72"/>
       <c r="P50" s="72" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q50" s="72" t="s">
         <v>26</v>
       </c>
       <c r="R50" s="72" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="S50" s="72" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T50" s="72" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="U50" s="72" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="V50" s="72" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="W50" s="72" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="X50" s="72" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Y50" s="72" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Z50" s="72" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="AA50" s="72" t="s">
         <v>26</v>
@@ -11869,7 +11869,7 @@
         <v>49</v>
       </c>
       <c r="AI50" s="1" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="51" spans="1:35" ht="66" customHeight="1">
@@ -11877,29 +11877,29 @@
         <v>109</v>
       </c>
       <c r="B51" s="72" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="C51" s="72"/>
       <c r="D51" s="72">
         <v>2020</v>
       </c>
       <c r="E51" s="73" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F51" s="74" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="G51" s="72">
         <v>2020</v>
       </c>
       <c r="H51" s="75" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="I51" s="72" t="s">
         <v>21</v>
       </c>
       <c r="J51" s="72" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="K51" s="72" t="s">
         <v>43</v>
@@ -11908,7 +11908,7 @@
         <v>176</v>
       </c>
       <c r="M51" s="72" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="N51" s="72">
         <v>5</v>
@@ -11927,25 +11927,25 @@
         <v>26</v>
       </c>
       <c r="T51" s="72" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="U51" s="72" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="V51" s="72" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="W51" s="72" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="X51" s="72" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Y51" s="72" t="s">
         <v>26</v>
       </c>
       <c r="Z51" s="72" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="AA51" s="72" t="s">
         <v>26</v>
@@ -11972,7 +11972,7 @@
         <v>49</v>
       </c>
       <c r="AI51" s="1" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="52" spans="1:35" ht="88" customHeight="1">
@@ -11980,81 +11980,81 @@
         <v>110</v>
       </c>
       <c r="B52" s="72" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="C52" s="72"/>
       <c r="D52" s="72">
         <v>2020</v>
       </c>
       <c r="E52" s="72" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="F52" s="74" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="G52" s="72">
         <v>2020</v>
       </c>
       <c r="H52" s="75" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="I52" s="72" t="s">
         <v>21</v>
       </c>
       <c r="J52" s="72" t="s">
+        <v>814</v>
+      </c>
+      <c r="K52" s="72" t="s">
         <v>815</v>
       </c>
-      <c r="K52" s="72" t="s">
+      <c r="L52" s="72" t="s">
         <v>816</v>
       </c>
-      <c r="L52" s="72" t="s">
-        <v>817</v>
-      </c>
       <c r="M52" s="72" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="N52" s="72">
         <v>5</v>
       </c>
       <c r="O52" s="72"/>
       <c r="P52" s="72" t="s">
+        <v>795</v>
+      </c>
+      <c r="Q52" s="72" t="s">
+        <v>795</v>
+      </c>
+      <c r="R52" s="72" t="s">
         <v>796</v>
       </c>
-      <c r="Q52" s="72" t="s">
+      <c r="S52" s="72" t="s">
+        <v>795</v>
+      </c>
+      <c r="T52" s="72" t="s">
+        <v>780</v>
+      </c>
+      <c r="U52" s="72" t="s">
+        <v>780</v>
+      </c>
+      <c r="V52" s="72" t="s">
+        <v>644</v>
+      </c>
+      <c r="W52" s="72" t="s">
+        <v>732</v>
+      </c>
+      <c r="X52" s="72" t="s">
+        <v>795</v>
+      </c>
+      <c r="Y52" s="72" t="s">
         <v>796</v>
       </c>
-      <c r="R52" s="72" t="s">
-        <v>797</v>
-      </c>
-      <c r="S52" s="72" t="s">
+      <c r="Z52" s="72" t="s">
+        <v>830</v>
+      </c>
+      <c r="AA52" s="72" t="s">
         <v>796</v>
       </c>
-      <c r="T52" s="72" t="s">
-        <v>781</v>
-      </c>
-      <c r="U52" s="72" t="s">
-        <v>781</v>
-      </c>
-      <c r="V52" s="72" t="s">
-        <v>645</v>
-      </c>
-      <c r="W52" s="72" t="s">
-        <v>733</v>
-      </c>
-      <c r="X52" s="72" t="s">
+      <c r="AB52" s="72" t="s">
         <v>796</v>
-      </c>
-      <c r="Y52" s="72" t="s">
-        <v>797</v>
-      </c>
-      <c r="Z52" s="72" t="s">
-        <v>831</v>
-      </c>
-      <c r="AA52" s="72" t="s">
-        <v>797</v>
-      </c>
-      <c r="AB52" s="72" t="s">
-        <v>797</v>
       </c>
       <c r="AC52" s="72" t="s">
         <v>49</v>
@@ -12075,7 +12075,7 @@
         <v>49</v>
       </c>
       <c r="AI52" s="1" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="53" spans="1:35" ht="85" customHeight="1">
@@ -12083,81 +12083,81 @@
         <v>111</v>
       </c>
       <c r="B53" s="78" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="C53" s="72"/>
       <c r="D53" s="72">
         <v>2020</v>
       </c>
       <c r="E53" s="72" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="F53" s="74" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="G53" s="72">
         <v>2020</v>
       </c>
       <c r="H53" s="75" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="I53" s="72" t="s">
         <v>21</v>
       </c>
       <c r="J53" s="72" t="s">
+        <v>819</v>
+      </c>
+      <c r="K53" s="72" t="s">
         <v>820</v>
-      </c>
-      <c r="K53" s="72" t="s">
-        <v>821</v>
       </c>
       <c r="L53" s="72" t="s">
         <v>176</v>
       </c>
       <c r="M53" s="72" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="N53" s="72">
         <v>11</v>
       </c>
       <c r="O53" s="72"/>
       <c r="P53" s="72" t="s">
+        <v>795</v>
+      </c>
+      <c r="Q53" s="72" t="s">
         <v>796</v>
       </c>
-      <c r="Q53" s="72" t="s">
-        <v>797</v>
-      </c>
       <c r="R53" s="72" t="s">
+        <v>795</v>
+      </c>
+      <c r="S53" s="72" t="s">
+        <v>795</v>
+      </c>
+      <c r="T53" s="72" t="s">
+        <v>780</v>
+      </c>
+      <c r="U53" s="72" t="s">
+        <v>780</v>
+      </c>
+      <c r="V53" s="72" t="s">
+        <v>644</v>
+      </c>
+      <c r="W53" s="72" t="s">
+        <v>732</v>
+      </c>
+      <c r="X53" s="72" t="s">
+        <v>795</v>
+      </c>
+      <c r="Y53" s="72" t="s">
         <v>796</v>
       </c>
-      <c r="S53" s="72" t="s">
+      <c r="Z53" s="72" t="s">
+        <v>830</v>
+      </c>
+      <c r="AA53" s="72" t="s">
         <v>796</v>
       </c>
-      <c r="T53" s="72" t="s">
-        <v>781</v>
-      </c>
-      <c r="U53" s="72" t="s">
-        <v>781</v>
-      </c>
-      <c r="V53" s="72" t="s">
-        <v>645</v>
-      </c>
-      <c r="W53" s="72" t="s">
-        <v>733</v>
-      </c>
-      <c r="X53" s="72" t="s">
+      <c r="AB53" s="72" t="s">
         <v>796</v>
-      </c>
-      <c r="Y53" s="72" t="s">
-        <v>797</v>
-      </c>
-      <c r="Z53" s="72" t="s">
-        <v>831</v>
-      </c>
-      <c r="AA53" s="72" t="s">
-        <v>797</v>
-      </c>
-      <c r="AB53" s="72" t="s">
-        <v>797</v>
       </c>
       <c r="AC53" s="72" t="s">
         <v>49</v>
@@ -12178,7 +12178,7 @@
         <v>49</v>
       </c>
       <c r="AI53" s="1" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="54" spans="1:35" ht="87" customHeight="1">
@@ -12186,38 +12186,38 @@
         <v>112</v>
       </c>
       <c r="B54" s="72" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="C54" s="72"/>
       <c r="D54" s="72">
         <v>2020</v>
       </c>
       <c r="E54" s="73" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="F54" s="74" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="G54" s="72">
         <v>2020</v>
       </c>
       <c r="H54" s="75" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="I54" s="72" t="s">
         <v>21</v>
       </c>
       <c r="J54" s="72" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="K54" s="72" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="L54" s="72" t="s">
         <v>176</v>
       </c>
       <c r="M54" s="72" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="N54" s="72">
         <v>9</v>
@@ -12238,19 +12238,19 @@
       <c r="T54" s="72"/>
       <c r="U54" s="72"/>
       <c r="V54" s="72" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="W54" s="72" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="X54" s="72" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="Y54" s="72" t="s">
         <v>26</v>
       </c>
       <c r="Z54" s="72" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="AA54" s="72" t="s">
         <v>26</v>
@@ -12277,7 +12277,7 @@
         <v>49</v>
       </c>
       <c r="AI54" s="1" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="55" spans="1:35" ht="68" customHeight="1">
@@ -12285,38 +12285,38 @@
         <v>113</v>
       </c>
       <c r="B55" s="72" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C55" s="72"/>
       <c r="D55" s="72">
         <v>2020</v>
       </c>
       <c r="E55" s="72" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="F55" s="74" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="G55" s="72">
         <v>2020</v>
       </c>
       <c r="H55" s="75" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="I55" s="72" t="s">
         <v>21</v>
       </c>
       <c r="J55" s="72" t="s">
+        <v>803</v>
+      </c>
+      <c r="K55" s="72" t="s">
+        <v>803</v>
+      </c>
+      <c r="L55" s="72" t="s">
         <v>804</v>
       </c>
-      <c r="K55" s="72" t="s">
-        <v>804</v>
-      </c>
-      <c r="L55" s="72" t="s">
+      <c r="M55" s="72" t="s">
         <v>805</v>
-      </c>
-      <c r="M55" s="72" t="s">
-        <v>806</v>
       </c>
       <c r="N55" s="72">
         <v>12</v>
@@ -12335,25 +12335,25 @@
         <v>26</v>
       </c>
       <c r="T55" s="72" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="U55" s="72" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="V55" s="72" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="W55" s="72" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="X55" s="72" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="Y55" s="72" t="s">
         <v>26</v>
       </c>
       <c r="Z55" s="72" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="AA55" s="72" t="s">
         <v>26</v>
@@ -12380,7 +12380,7 @@
         <v>49</v>
       </c>
       <c r="AI55" s="1" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="56" spans="1:35" ht="143" customHeight="1">
@@ -12388,23 +12388,23 @@
         <v>114</v>
       </c>
       <c r="B56" s="72" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C56" s="72"/>
       <c r="D56" s="72">
         <v>2020</v>
       </c>
       <c r="E56" s="72" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="F56" s="74" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="G56" s="72">
         <v>2020</v>
       </c>
       <c r="H56" s="75" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="I56" s="72" t="s">
         <v>34</v>
@@ -12419,7 +12419,7 @@
         <v>176</v>
       </c>
       <c r="M56" s="72" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="N56" s="72">
         <v>14</v>
@@ -12438,28 +12438,28 @@
         <v>26</v>
       </c>
       <c r="T56" s="72" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="U56" s="72" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="V56" s="72" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="W56" s="72" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="X56" s="72" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Y56" s="72" t="s">
         <v>26</v>
       </c>
       <c r="Z56" s="72" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="AA56" s="72" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="AB56" s="72" t="s">
         <v>26</v>
@@ -12483,7 +12483,7 @@
         <v>49</v>
       </c>
       <c r="AI56" s="1" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="57" spans="1:35" ht="113" customHeight="1">
@@ -12491,75 +12491,75 @@
         <v>115</v>
       </c>
       <c r="B57" s="72" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="C57" s="72"/>
       <c r="D57" s="72">
         <v>2020</v>
       </c>
       <c r="E57" s="73" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="F57" s="74" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="G57" s="72">
         <v>2020</v>
       </c>
       <c r="H57" s="75" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I57" s="72" t="s">
         <v>34</v>
       </c>
       <c r="J57" s="72" t="s">
+        <v>784</v>
+      </c>
+      <c r="K57" s="72" t="s">
+        <v>784</v>
+      </c>
+      <c r="L57" s="72" t="s">
         <v>785</v>
       </c>
-      <c r="K57" s="72" t="s">
-        <v>785</v>
-      </c>
-      <c r="L57" s="72" t="s">
+      <c r="M57" s="72" t="s">
         <v>786</v>
-      </c>
-      <c r="M57" s="72" t="s">
-        <v>787</v>
       </c>
       <c r="N57" s="72">
         <v>31</v>
       </c>
       <c r="O57" s="72"/>
       <c r="P57" s="72" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q57" s="72" t="s">
         <v>26</v>
       </c>
       <c r="R57" s="72" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="S57" s="72" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T57" s="72" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="U57" s="72" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="V57" s="72" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="W57" s="72" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="X57" s="72" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Y57" s="72" t="s">
         <v>26</v>
       </c>
       <c r="Z57" s="72" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="AA57" s="72" t="s">
         <v>26</v>
@@ -12586,7 +12586,7 @@
         <v>49</v>
       </c>
       <c r="AI57" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="58" spans="1:35" ht="124" customHeight="1">
@@ -12594,75 +12594,75 @@
         <v>116</v>
       </c>
       <c r="B58" s="72" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="C58" s="72"/>
       <c r="D58" s="72">
         <v>2020</v>
       </c>
       <c r="E58" s="73" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="F58" s="74" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="G58" s="72">
         <v>2020</v>
       </c>
       <c r="H58" s="75" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="I58" s="72" t="s">
         <v>34</v>
       </c>
       <c r="J58" s="77" t="s">
+        <v>777</v>
+      </c>
+      <c r="K58" s="72" t="s">
         <v>778</v>
-      </c>
-      <c r="K58" s="72" t="s">
-        <v>779</v>
       </c>
       <c r="L58" s="72" t="s">
         <v>176</v>
       </c>
       <c r="M58" s="72" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="N58" s="72">
         <v>49</v>
       </c>
       <c r="O58" s="72"/>
       <c r="P58" s="72" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Q58" s="72" t="s">
         <v>26</v>
       </c>
       <c r="R58" s="72" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="S58" s="72" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="T58" s="72" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="U58" s="72" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="V58" s="72" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="W58" s="72" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="X58" s="72" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Y58" s="72" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Z58" s="72" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="AA58" s="72" t="s">
         <v>26</v>
@@ -12689,7 +12689,7 @@
         <v>49</v>
       </c>
       <c r="AI58" s="1" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
   </sheetData>

</xml_diff>